<commit_message>
Completed Example3 of Flight Numbers
</commit_message>
<xml_diff>
--- a/ExcelEsport/FMWC_Examples/What Is My Flight Number - Patrick Chatain - My Work.xlsx
+++ b/ExcelEsport/FMWC_Examples/What Is My Flight Number - Patrick Chatain - My Work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\FMWC_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D256E729-0053-47BE-A8A6-A8DBB8AF0E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AAAF90-1A25-4879-B3C4-02E1312AB863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{114A3ACC-2F61-4F50-A5CF-63A86B2334B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{114A3ACC-2F61-4F50-A5CF-63A86B2334B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="29" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2045,57 +2045,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2165,7 +2115,57 @@
     <xf numFmtId="3" fontId="14" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="1" xr:uid="{C1B9BA85-4C62-429F-905A-EBA90D38020B}"/>
@@ -2723,8 +2723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCF8115-0CC8-46F8-8E7E-E74BDD47BD6B}">
   <dimension ref="A1:AZ216"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A90" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView showGridLines="0" topLeftCell="A114" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108:E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2777,34 +2777,34 @@
       <c r="AZ1" s="6"/>
     </row>
     <row r="2" spans="2:52" ht="60.6" customHeight="1">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="105" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="81"/>
-      <c r="AA2" s="81"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
       <c r="AO2" s="3"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6"/>
@@ -2820,32 +2820,32 @@
       <c r="AZ3" s="6"/>
     </row>
     <row r="4" spans="2:52" ht="33.6" customHeight="1">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="Y4" s="93" t="s">
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="106"/>
+      <c r="T4" s="106"/>
+      <c r="Y4" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="82"/>
+      <c r="Z4" s="117"/>
+      <c r="AA4" s="106"/>
       <c r="AO4" s="3"/>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -3045,11 +3045,11 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
       <c r="X11" s="31"/>
-      <c r="Y11" s="94" t="s">
+      <c r="Y11" s="118" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="95"/>
-      <c r="AA11" s="96"/>
+      <c r="Z11" s="119"/>
+      <c r="AA11" s="120"/>
       <c r="AO11" s="3"/>
       <c r="AY11" s="6"/>
       <c r="AZ11" s="6"/>
@@ -3084,33 +3084,33 @@
       <c r="AZ12" s="6"/>
     </row>
     <row r="13" spans="2:52" ht="24.95" customHeight="1" thickBot="1">
-      <c r="B13" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="82"/>
-      <c r="T13" s="82"/>
+      <c r="B13" s="107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
+      <c r="R13" s="106"/>
+      <c r="S13" s="106"/>
+      <c r="T13" s="106"/>
       <c r="U13" s="60"/>
-      <c r="Y13" s="83" t="s">
+      <c r="Y13" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="Z13" s="82"/>
-      <c r="AA13" s="82"/>
+      <c r="Z13" s="106"/>
+      <c r="AA13" s="106"/>
       <c r="AF13" s="60"/>
       <c r="AG13" s="60"/>
       <c r="AH13" s="60"/>
@@ -3118,27 +3118,27 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:52" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="108" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="86"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="109"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="109"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="109"/>
+      <c r="S14" s="109"/>
+      <c r="T14" s="110"/>
       <c r="U14" s="3"/>
       <c r="Y14" s="61" t="s">
         <v>31</v>
@@ -3158,25 +3158,25 @@
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:52" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="88"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="89"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="112"/>
+      <c r="P15" s="112"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="112"/>
+      <c r="S15" s="112"/>
+      <c r="T15" s="113"/>
       <c r="U15" s="3"/>
       <c r="Y15" s="62" t="s">
         <v>32</v>
@@ -3196,25 +3196,25 @@
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B16" s="87"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="89"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="112"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="112"/>
+      <c r="O16" s="112"/>
+      <c r="P16" s="112"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
+      <c r="T16" s="113"/>
       <c r="U16" s="3"/>
       <c r="Y16" s="62" t="s">
         <v>47</v>
@@ -3233,25 +3233,25 @@
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B17" s="87"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="88"/>
-      <c r="P17" s="88"/>
-      <c r="Q17" s="88"/>
-      <c r="R17" s="88"/>
-      <c r="S17" s="88"/>
-      <c r="T17" s="89"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="112"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="112"/>
+      <c r="N17" s="112"/>
+      <c r="O17" s="112"/>
+      <c r="P17" s="112"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112"/>
+      <c r="T17" s="113"/>
       <c r="U17" s="3"/>
       <c r="Y17" s="62" t="s">
         <v>39</v>
@@ -3270,25 +3270,25 @@
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B18" s="87"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="88"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="88"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-      <c r="T18" s="89"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="112"/>
+      <c r="T18" s="113"/>
       <c r="U18" s="3"/>
       <c r="Y18" s="62" t="s">
         <v>35</v>
@@ -3307,25 +3307,25 @@
       <c r="AO18" s="3"/>
     </row>
     <row r="19" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="88"/>
-      <c r="R19" s="88"/>
-      <c r="S19" s="88"/>
-      <c r="T19" s="89"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="112"/>
+      <c r="N19" s="112"/>
+      <c r="O19" s="112"/>
+      <c r="P19" s="112"/>
+      <c r="Q19" s="112"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="112"/>
+      <c r="T19" s="113"/>
       <c r="U19" s="3"/>
       <c r="Y19" s="62" t="s">
         <v>42</v>
@@ -3344,25 +3344,25 @@
       <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B20" s="87"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="88"/>
-      <c r="S20" s="88"/>
-      <c r="T20" s="89"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="112"/>
+      <c r="M20" s="112"/>
+      <c r="N20" s="112"/>
+      <c r="O20" s="112"/>
+      <c r="P20" s="112"/>
+      <c r="Q20" s="112"/>
+      <c r="R20" s="112"/>
+      <c r="S20" s="112"/>
+      <c r="T20" s="113"/>
       <c r="U20" s="3"/>
       <c r="Y20" s="62" t="s">
         <v>48</v>
@@ -3379,25 +3379,25 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B21" s="87"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="88"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
-      <c r="Q21" s="88"/>
-      <c r="R21" s="88"/>
-      <c r="S21" s="88"/>
-      <c r="T21" s="89"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
+      <c r="M21" s="112"/>
+      <c r="N21" s="112"/>
+      <c r="O21" s="112"/>
+      <c r="P21" s="112"/>
+      <c r="Q21" s="112"/>
+      <c r="R21" s="112"/>
+      <c r="S21" s="112"/>
+      <c r="T21" s="113"/>
       <c r="U21" s="3"/>
       <c r="Y21" s="62" t="s">
         <v>49</v>
@@ -3416,25 +3416,25 @@
       <c r="AO21" s="3"/>
     </row>
     <row r="22" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="88"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="88"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88"/>
-      <c r="Q22" s="88"/>
-      <c r="R22" s="88"/>
-      <c r="S22" s="88"/>
-      <c r="T22" s="89"/>
+      <c r="B22" s="111"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="112"/>
+      <c r="Q22" s="112"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="112"/>
+      <c r="T22" s="113"/>
       <c r="U22" s="3"/>
       <c r="Y22" s="62" t="s">
         <v>50</v>
@@ -3454,25 +3454,25 @@
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="89"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="112"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="112"/>
+      <c r="M23" s="112"/>
+      <c r="N23" s="112"/>
+      <c r="O23" s="112"/>
+      <c r="P23" s="112"/>
+      <c r="Q23" s="112"/>
+      <c r="R23" s="112"/>
+      <c r="S23" s="112"/>
+      <c r="T23" s="113"/>
       <c r="U23" s="3"/>
       <c r="Y23" s="62" t="s">
         <v>51</v>
@@ -3492,25 +3492,25 @@
       <c r="AP23" s="3"/>
     </row>
     <row r="24" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="88"/>
-      <c r="S24" s="88"/>
-      <c r="T24" s="89"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="112"/>
+      <c r="R24" s="112"/>
+      <c r="S24" s="112"/>
+      <c r="T24" s="113"/>
       <c r="U24" s="3"/>
       <c r="Y24" s="62" t="s">
         <v>52</v>
@@ -3530,25 +3530,25 @@
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B25" s="87"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="88"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="88"/>
-      <c r="Q25" s="88"/>
-      <c r="R25" s="88"/>
-      <c r="S25" s="88"/>
-      <c r="T25" s="89"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="112"/>
+      <c r="H25" s="112"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
+      <c r="K25" s="112"/>
+      <c r="L25" s="112"/>
+      <c r="M25" s="112"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="112"/>
+      <c r="Q25" s="112"/>
+      <c r="R25" s="112"/>
+      <c r="S25" s="112"/>
+      <c r="T25" s="113"/>
       <c r="U25" s="3"/>
       <c r="Y25" s="62" t="s">
         <v>53</v>
@@ -3566,25 +3566,25 @@
       <c r="AP25" s="3"/>
     </row>
     <row r="26" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="88"/>
-      <c r="T26" s="89"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="112"/>
+      <c r="M26" s="112"/>
+      <c r="N26" s="112"/>
+      <c r="O26" s="112"/>
+      <c r="P26" s="112"/>
+      <c r="Q26" s="112"/>
+      <c r="R26" s="112"/>
+      <c r="S26" s="112"/>
+      <c r="T26" s="113"/>
       <c r="U26" s="3"/>
       <c r="Y26" s="62" t="s">
         <v>105</v>
@@ -3607,25 +3607,25 @@
       <c r="AP26" s="3"/>
     </row>
     <row r="27" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="88"/>
-      <c r="R27" s="88"/>
-      <c r="S27" s="88"/>
-      <c r="T27" s="89"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="112"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
+      <c r="M27" s="112"/>
+      <c r="N27" s="112"/>
+      <c r="O27" s="112"/>
+      <c r="P27" s="112"/>
+      <c r="Q27" s="112"/>
+      <c r="R27" s="112"/>
+      <c r="S27" s="112"/>
+      <c r="T27" s="113"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -3644,25 +3644,25 @@
       <c r="AP27" s="3"/>
     </row>
     <row r="28" spans="2:52" ht="47.25" customHeight="1">
-      <c r="B28" s="90"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="91"/>
-      <c r="L28" s="91"/>
-      <c r="M28" s="91"/>
-      <c r="N28" s="91"/>
-      <c r="O28" s="91"/>
-      <c r="P28" s="91"/>
-      <c r="Q28" s="91"/>
-      <c r="R28" s="91"/>
-      <c r="S28" s="91"/>
-      <c r="T28" s="92"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="115"/>
+      <c r="M28" s="115"/>
+      <c r="N28" s="115"/>
+      <c r="O28" s="115"/>
+      <c r="P28" s="115"/>
+      <c r="Q28" s="115"/>
+      <c r="R28" s="115"/>
+      <c r="S28" s="115"/>
+      <c r="T28" s="116"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -3673,10 +3673,10 @@
       <c r="AC28" s="63"/>
       <c r="AD28" s="63"/>
       <c r="AE28" s="64"/>
-      <c r="AF28" s="80"/>
-      <c r="AG28" s="80"/>
-      <c r="AH28" s="80"/>
-      <c r="AI28" s="80"/>
+      <c r="AF28" s="104"/>
+      <c r="AG28" s="104"/>
+      <c r="AH28" s="104"/>
+      <c r="AI28" s="104"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
     </row>
@@ -3721,34 +3721,34 @@
       <c r="AZ29" s="6"/>
     </row>
     <row r="30" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-      <c r="I30" s="101"/>
-      <c r="J30" s="101"/>
-      <c r="K30" s="101"/>
-      <c r="L30" s="101"/>
-      <c r="M30" s="101"/>
-      <c r="N30" s="101"/>
-      <c r="O30" s="101"/>
-      <c r="P30" s="101"/>
-      <c r="Q30" s="101"/>
-      <c r="R30" s="101"/>
-      <c r="S30" s="101"/>
-      <c r="T30" s="101"/>
-      <c r="U30" s="101"/>
-      <c r="V30" s="101"/>
-      <c r="W30" s="101"/>
-      <c r="X30" s="101"/>
-      <c r="Y30" s="101"/>
-      <c r="Z30" s="101"/>
-      <c r="AA30" s="102"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="85"/>
+      <c r="O30" s="85"/>
+      <c r="P30" s="85"/>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="85"/>
+      <c r="V30" s="85"/>
+      <c r="W30" s="85"/>
+      <c r="X30" s="85"/>
+      <c r="Y30" s="85"/>
+      <c r="Z30" s="85"/>
+      <c r="AA30" s="86"/>
       <c r="AC30" s="63"/>
       <c r="AD30" s="63"/>
       <c r="AE30" s="64"/>
@@ -3799,29 +3799,29 @@
       <c r="E33" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="103" t="s">
+      <c r="G33" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="104"/>
-      <c r="I33" s="104"/>
-      <c r="J33" s="104"/>
-      <c r="K33" s="104"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
-      <c r="O33" s="104"/>
-      <c r="P33" s="104"/>
-      <c r="Q33" s="104"/>
-      <c r="R33" s="104"/>
-      <c r="S33" s="104"/>
-      <c r="T33" s="104"/>
-      <c r="U33" s="104"/>
-      <c r="V33" s="104"/>
-      <c r="W33" s="104"/>
-      <c r="X33" s="104"/>
-      <c r="Y33" s="104"/>
-      <c r="Z33" s="104"/>
-      <c r="AA33" s="105"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="88"/>
+      <c r="P33" s="88"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="88"/>
+      <c r="S33" s="88"/>
+      <c r="T33" s="88"/>
+      <c r="U33" s="88"/>
+      <c r="V33" s="88"/>
+      <c r="W33" s="88"/>
+      <c r="X33" s="88"/>
+      <c r="Y33" s="88"/>
+      <c r="Z33" s="88"/>
+      <c r="AA33" s="89"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="63"/>
       <c r="AE33" s="64"/>
@@ -3841,29 +3841,29 @@
         <f>IF(AND(E34&lt;&gt;"",E34=Answers!E34),1,IF(ISBLANK(E34),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G34" s="106" t="s">
+      <c r="G34" s="90" t="s">
         <v>308</v>
       </c>
-      <c r="H34" s="107"/>
-      <c r="I34" s="107"/>
-      <c r="J34" s="107"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="107"/>
-      <c r="O34" s="107"/>
-      <c r="P34" s="107"/>
-      <c r="Q34" s="107"/>
-      <c r="R34" s="107"/>
-      <c r="S34" s="107"/>
-      <c r="T34" s="107"/>
-      <c r="U34" s="107"/>
-      <c r="V34" s="107"/>
-      <c r="W34" s="107"/>
-      <c r="X34" s="107"/>
-      <c r="Y34" s="107"/>
-      <c r="Z34" s="107"/>
-      <c r="AA34" s="108"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="91"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="91"/>
+      <c r="P34" s="91"/>
+      <c r="Q34" s="91"/>
+      <c r="R34" s="91"/>
+      <c r="S34" s="91"/>
+      <c r="T34" s="91"/>
+      <c r="U34" s="91"/>
+      <c r="V34" s="91"/>
+      <c r="W34" s="91"/>
+      <c r="X34" s="91"/>
+      <c r="Y34" s="91"/>
+      <c r="Z34" s="91"/>
+      <c r="AA34" s="92"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="63"/>
       <c r="AE34" s="64"/>
@@ -3883,29 +3883,29 @@
         <f>IF(AND(E35&lt;&gt;"",E35=Answers!E35),1,IF(ISBLANK(E35),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G35" s="109" t="s">
+      <c r="G35" s="93" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="110"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="110"/>
-      <c r="L35" s="110"/>
-      <c r="M35" s="110"/>
-      <c r="N35" s="110"/>
-      <c r="O35" s="110"/>
-      <c r="P35" s="110"/>
-      <c r="Q35" s="110"/>
-      <c r="R35" s="110"/>
-      <c r="S35" s="110"/>
-      <c r="T35" s="110"/>
-      <c r="U35" s="110"/>
-      <c r="V35" s="110"/>
-      <c r="W35" s="110"/>
-      <c r="X35" s="110"/>
-      <c r="Y35" s="110"/>
-      <c r="Z35" s="110"/>
-      <c r="AA35" s="111"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="94"/>
+      <c r="R35" s="94"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="94"/>
+      <c r="X35" s="94"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="95"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="63"/>
       <c r="AE35" s="64"/>
@@ -3925,29 +3925,29 @@
         <f>IF(AND(E36&lt;&gt;"",E36=Answers!E36),1,IF(ISBLANK(E36),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G36" s="112" t="s">
+      <c r="G36" s="96" t="s">
         <v>309</v>
       </c>
-      <c r="H36" s="113"/>
-      <c r="I36" s="113"/>
-      <c r="J36" s="113"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="113"/>
-      <c r="M36" s="113"/>
-      <c r="N36" s="113"/>
-      <c r="O36" s="113"/>
-      <c r="P36" s="113"/>
-      <c r="Q36" s="113"/>
-      <c r="R36" s="113"/>
-      <c r="S36" s="113"/>
-      <c r="T36" s="113"/>
-      <c r="U36" s="113"/>
-      <c r="V36" s="113"/>
-      <c r="W36" s="113"/>
-      <c r="X36" s="113"/>
-      <c r="Y36" s="113"/>
-      <c r="Z36" s="113"/>
-      <c r="AA36" s="114"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="97"/>
+      <c r="O36" s="97"/>
+      <c r="P36" s="97"/>
+      <c r="Q36" s="97"/>
+      <c r="R36" s="97"/>
+      <c r="S36" s="97"/>
+      <c r="T36" s="97"/>
+      <c r="U36" s="97"/>
+      <c r="V36" s="97"/>
+      <c r="W36" s="97"/>
+      <c r="X36" s="97"/>
+      <c r="Y36" s="97"/>
+      <c r="Z36" s="97"/>
+      <c r="AA36" s="98"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="63"/>
       <c r="AE36" s="64"/>
@@ -4050,13 +4050,13 @@
       <c r="C41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="116" t="s">
+      <c r="J41" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="K41" s="116"/>
-      <c r="L41" s="116"/>
-      <c r="M41" s="116"/>
-      <c r="N41" s="116"/>
+      <c r="K41" s="100"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="100"/>
+      <c r="N41" s="100"/>
       <c r="AS41" s="6"/>
       <c r="AT41" s="6"/>
       <c r="AU41" s="6"/>
@@ -4067,14 +4067,14 @@
       <c r="AZ41" s="6"/>
     </row>
     <row r="42" spans="2:52" ht="15" customHeight="1" thickTop="1">
-      <c r="J42" s="115" cm="1">
+      <c r="J42" s="99" cm="1">
         <f t="array" ref="J42">SUMPRODUCT(--(F34:F216=1),F34:F216,D34:D216)</f>
-        <v>220</v>
-      </c>
-      <c r="K42" s="115"/>
-      <c r="L42" s="115"/>
-      <c r="M42" s="115"/>
-      <c r="N42" s="115"/>
+        <v>420</v>
+      </c>
+      <c r="K42" s="99"/>
+      <c r="L42" s="99"/>
+      <c r="M42" s="99"/>
+      <c r="N42" s="99"/>
       <c r="AS42" s="6"/>
       <c r="AT42" s="6"/>
       <c r="AU42" s="6"/>
@@ -4088,11 +4088,11 @@
       <c r="B43" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="J43" s="115"/>
-      <c r="K43" s="115"/>
-      <c r="L43" s="115"/>
-      <c r="M43" s="115"/>
-      <c r="N43" s="115"/>
+      <c r="J43" s="99"/>
+      <c r="K43" s="99"/>
+      <c r="L43" s="99"/>
+      <c r="M43" s="99"/>
+      <c r="N43" s="99"/>
       <c r="AS43" s="6"/>
       <c r="AT43" s="6"/>
       <c r="AU43" s="6"/>
@@ -4105,11 +4105,11 @@
     <row r="44" spans="2:52" ht="15" customHeight="1" thickBot="1">
       <c r="B44" s="20"/>
       <c r="G44" s="27"/>
-      <c r="J44" s="115"/>
-      <c r="K44" s="115"/>
-      <c r="L44" s="115"/>
-      <c r="M44" s="115"/>
-      <c r="N44" s="115"/>
+      <c r="J44" s="99"/>
+      <c r="K44" s="99"/>
+      <c r="L44" s="99"/>
+      <c r="M44" s="99"/>
+      <c r="N44" s="99"/>
       <c r="R44" s="6"/>
     </row>
     <row r="45" spans="2:52" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
@@ -4130,11 +4130,11 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="115"/>
-      <c r="K45" s="115"/>
-      <c r="L45" s="115"/>
-      <c r="M45" s="115"/>
-      <c r="N45" s="115"/>
+      <c r="J45" s="99"/>
+      <c r="K45" s="99"/>
+      <c r="L45" s="99"/>
+      <c r="M45" s="99"/>
+      <c r="N45" s="99"/>
       <c r="R45" s="6"/>
       <c r="AB45" s="6"/>
       <c r="AC45" s="6"/>
@@ -5326,20 +5326,20 @@
       <c r="E67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="103" t="s">
+      <c r="G67" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="H67" s="104"/>
-      <c r="I67" s="104"/>
-      <c r="J67" s="104"/>
-      <c r="K67" s="104"/>
-      <c r="L67" s="104"/>
-      <c r="M67" s="104"/>
-      <c r="N67" s="104"/>
-      <c r="O67" s="104"/>
-      <c r="P67" s="104"/>
-      <c r="Q67" s="104"/>
-      <c r="R67" s="105"/>
+      <c r="H67" s="88"/>
+      <c r="I67" s="88"/>
+      <c r="J67" s="88"/>
+      <c r="K67" s="88"/>
+      <c r="L67" s="88"/>
+      <c r="M67" s="88"/>
+      <c r="N67" s="88"/>
+      <c r="O67" s="88"/>
+      <c r="P67" s="88"/>
+      <c r="Q67" s="88"/>
+      <c r="R67" s="89"/>
       <c r="S67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -7382,35 +7382,35 @@
         <v>4</v>
       </c>
       <c r="E104" s="44"/>
-      <c r="G104" s="117" t="s">
+      <c r="G104" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="H104" s="118"/>
-      <c r="I104" s="118"/>
-      <c r="J104" s="118"/>
-      <c r="K104" s="118"/>
-      <c r="L104" s="118"/>
-      <c r="M104" s="118"/>
-      <c r="N104" s="118"/>
-      <c r="O104" s="118"/>
-      <c r="P104" s="118"/>
-      <c r="Q104" s="118"/>
-      <c r="R104" s="118"/>
-      <c r="S104" s="118"/>
-      <c r="T104" s="118"/>
-      <c r="U104" s="118"/>
-      <c r="V104" s="118"/>
-      <c r="W104" s="118"/>
-      <c r="X104" s="118"/>
-      <c r="Y104" s="118"/>
-      <c r="Z104" s="118"/>
-      <c r="AA104" s="118"/>
-      <c r="AB104" s="118"/>
-      <c r="AC104" s="118"/>
-      <c r="AD104" s="118"/>
-      <c r="AE104" s="118"/>
-      <c r="AF104" s="118"/>
-      <c r="AG104" s="119"/>
+      <c r="H104" s="102"/>
+      <c r="I104" s="102"/>
+      <c r="J104" s="102"/>
+      <c r="K104" s="102"/>
+      <c r="L104" s="102"/>
+      <c r="M104" s="102"/>
+      <c r="N104" s="102"/>
+      <c r="O104" s="102"/>
+      <c r="P104" s="102"/>
+      <c r="Q104" s="102"/>
+      <c r="R104" s="102"/>
+      <c r="S104" s="102"/>
+      <c r="T104" s="102"/>
+      <c r="U104" s="102"/>
+      <c r="V104" s="102"/>
+      <c r="W104" s="102"/>
+      <c r="X104" s="102"/>
+      <c r="Y104" s="102"/>
+      <c r="Z104" s="102"/>
+      <c r="AA104" s="102"/>
+      <c r="AB104" s="102"/>
+      <c r="AC104" s="102"/>
+      <c r="AD104" s="102"/>
+      <c r="AE104" s="102"/>
+      <c r="AF104" s="102"/>
+      <c r="AG104" s="103"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
       <c r="AJ104" s="6"/>
@@ -7551,10 +7551,12 @@
       <c r="D108" s="18">
         <v>10</v>
       </c>
-      <c r="E108" s="30"/>
+      <c r="E108" s="30">
+        <v>75</v>
+      </c>
       <c r="F108" s="36">
         <f>IF(AND(E108&lt;&gt;"",E108=Answers!E108),1,IF(ISBLANK(E108),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="32" t="s">
         <v>214</v>
@@ -7597,10 +7599,12 @@
       <c r="D109" s="18">
         <v>10</v>
       </c>
-      <c r="E109" s="30"/>
+      <c r="E109" s="30">
+        <v>107</v>
+      </c>
       <c r="F109" s="36">
         <f>IF(AND(E109&lt;&gt;"",E109=Answers!E109),1,IF(ISBLANK(E109),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="32" t="s">
         <v>196</v>
@@ -7643,10 +7647,12 @@
       <c r="D110" s="18">
         <v>10</v>
       </c>
-      <c r="E110" s="30"/>
+      <c r="E110" s="30">
+        <v>128</v>
+      </c>
       <c r="F110" s="36">
         <f>IF(AND(E110&lt;&gt;"",E110=Answers!E110),1,IF(ISBLANK(E110),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110" s="32" t="s">
         <v>197</v>
@@ -7689,10 +7695,12 @@
       <c r="D111" s="18">
         <v>10</v>
       </c>
-      <c r="E111" s="30"/>
+      <c r="E111" s="30">
+        <v>107</v>
+      </c>
       <c r="F111" s="36">
         <f>IF(AND(E111&lt;&gt;"",E111=Answers!E111),1,IF(ISBLANK(E111),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111" s="32" t="s">
         <v>198</v>
@@ -7735,10 +7743,12 @@
       <c r="D112" s="18">
         <v>10</v>
       </c>
-      <c r="E112" s="30"/>
+      <c r="E112" s="30">
+        <v>99</v>
+      </c>
       <c r="F112" s="36">
         <f>IF(AND(E112&lt;&gt;"",E112=Answers!E112),1,IF(ISBLANK(E112),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112" s="32" t="s">
         <v>199</v>
@@ -7781,10 +7791,12 @@
       <c r="D113" s="18">
         <v>10</v>
       </c>
-      <c r="E113" s="30"/>
+      <c r="E113" s="30">
+        <v>97</v>
+      </c>
       <c r="F113" s="36">
         <f>IF(AND(E113&lt;&gt;"",E113=Answers!E113),1,IF(ISBLANK(E113),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" s="32" t="s">
         <v>200</v>
@@ -7827,10 +7839,12 @@
       <c r="D114" s="18">
         <v>10</v>
       </c>
-      <c r="E114" s="30"/>
+      <c r="E114" s="30">
+        <v>69</v>
+      </c>
       <c r="F114" s="36">
         <f>IF(AND(E114&lt;&gt;"",E114=Answers!E114),1,IF(ISBLANK(E114),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G114" s="32" t="s">
         <v>215</v>
@@ -7873,10 +7887,12 @@
       <c r="D115" s="18">
         <v>10</v>
       </c>
-      <c r="E115" s="30"/>
+      <c r="E115" s="30">
+        <v>117</v>
+      </c>
       <c r="F115" s="36">
         <f>IF(AND(E115&lt;&gt;"",E115=Answers!E115),1,IF(ISBLANK(E115),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115" s="32" t="s">
         <v>201</v>
@@ -7919,10 +7935,12 @@
       <c r="D116" s="18">
         <v>10</v>
       </c>
-      <c r="E116" s="30"/>
+      <c r="E116" s="30">
+        <v>83</v>
+      </c>
       <c r="F116" s="36">
         <f>IF(AND(E116&lt;&gt;"",E116=Answers!E116),1,IF(ISBLANK(E116),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116" s="32" t="s">
         <v>202</v>
@@ -7965,10 +7983,12 @@
       <c r="D117" s="18">
         <v>10</v>
       </c>
-      <c r="E117" s="30"/>
+      <c r="E117" s="30">
+        <v>102</v>
+      </c>
       <c r="F117" s="36">
         <f>IF(AND(E117&lt;&gt;"",E117=Answers!E117),1,IF(ISBLANK(E117),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117" s="32" t="s">
         <v>203</v>
@@ -8011,10 +8031,12 @@
       <c r="D118" s="18">
         <v>10</v>
       </c>
-      <c r="E118" s="30"/>
+      <c r="E118" s="30">
+        <v>138</v>
+      </c>
       <c r="F118" s="36">
         <f>IF(AND(E118&lt;&gt;"",E118=Answers!E118),1,IF(ISBLANK(E118),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G118" s="32" t="s">
         <v>204</v>
@@ -8057,10 +8079,12 @@
       <c r="D119" s="18">
         <v>10</v>
       </c>
-      <c r="E119" s="30"/>
+      <c r="E119" s="30">
+        <v>113</v>
+      </c>
       <c r="F119" s="36">
         <f>IF(AND(E119&lt;&gt;"",E119=Answers!E119),1,IF(ISBLANK(E119),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119" s="32" t="s">
         <v>205</v>
@@ -8103,10 +8127,12 @@
       <c r="D120" s="18">
         <v>10</v>
       </c>
-      <c r="E120" s="30"/>
+      <c r="E120" s="30">
+        <v>89</v>
+      </c>
       <c r="F120" s="36">
         <f>IF(AND(E120&lt;&gt;"",E120=Answers!E120),1,IF(ISBLANK(E120),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120" s="32" t="s">
         <v>206</v>
@@ -8149,10 +8175,12 @@
       <c r="D121" s="18">
         <v>10</v>
       </c>
-      <c r="E121" s="30"/>
+      <c r="E121" s="30">
+        <v>97</v>
+      </c>
       <c r="F121" s="36">
         <f>IF(AND(E121&lt;&gt;"",E121=Answers!E121),1,IF(ISBLANK(E121),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121" s="32" t="s">
         <v>207</v>
@@ -8195,10 +8223,12 @@
       <c r="D122" s="18">
         <v>10</v>
       </c>
-      <c r="E122" s="30"/>
+      <c r="E122" s="30">
+        <v>107</v>
+      </c>
       <c r="F122" s="36">
         <f>IF(AND(E122&lt;&gt;"",E122=Answers!E122),1,IF(ISBLANK(E122),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122" s="32" t="s">
         <v>208</v>
@@ -8241,10 +8271,12 @@
       <c r="D123" s="18">
         <v>10</v>
       </c>
-      <c r="E123" s="30"/>
+      <c r="E123" s="30">
+        <v>89</v>
+      </c>
       <c r="F123" s="36">
         <f>IF(AND(E123&lt;&gt;"",E123=Answers!E123),1,IF(ISBLANK(E123),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G123" s="32" t="s">
         <v>209</v>
@@ -8287,10 +8319,12 @@
       <c r="D124" s="18">
         <v>10</v>
       </c>
-      <c r="E124" s="30"/>
+      <c r="E124" s="30">
+        <v>75</v>
+      </c>
       <c r="F124" s="36">
         <f>IF(AND(E124&lt;&gt;"",E124=Answers!E124),1,IF(ISBLANK(E124),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G124" s="32" t="s">
         <v>213</v>
@@ -8333,10 +8367,12 @@
       <c r="D125" s="18">
         <v>10</v>
       </c>
-      <c r="E125" s="30"/>
+      <c r="E125" s="30">
+        <v>90</v>
+      </c>
       <c r="F125" s="36">
         <f>IF(AND(E125&lt;&gt;"",E125=Answers!E125),1,IF(ISBLANK(E125),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" s="32" t="s">
         <v>210</v>
@@ -8379,10 +8415,12 @@
       <c r="D126" s="18">
         <v>10</v>
       </c>
-      <c r="E126" s="30"/>
+      <c r="E126" s="30">
+        <v>118</v>
+      </c>
       <c r="F126" s="36">
         <f>IF(AND(E126&lt;&gt;"",E126=Answers!E126),1,IF(ISBLANK(E126),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" s="32" t="s">
         <v>211</v>
@@ -8425,10 +8463,12 @@
       <c r="D127" s="18">
         <v>10</v>
       </c>
-      <c r="E127" s="30"/>
+      <c r="E127" s="30">
+        <v>112</v>
+      </c>
       <c r="F127" s="36">
         <f>IF(AND(E127&lt;&gt;"",E127=Answers!E127),1,IF(ISBLANK(E127),0,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G127" s="32" t="s">
         <v>212</v>
@@ -8485,11 +8525,11 @@
       </c>
       <c r="E129" s="30">
         <f>SUM(E108:E127)</f>
-        <v>0</v>
+        <v>2012</v>
       </c>
       <c r="F129" s="36">
         <f>IF(AND(E129&lt;&gt;"",E129=Answers!E129),1,IF(ISBLANK(E129),0,-1))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="S129" s="6"/>
       <c r="T129" s="6"/>
@@ -9046,48 +9086,48 @@
       <c r="G144" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I144" s="97" t="s">
+      <c r="I144" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="J144" s="98"/>
-      <c r="K144" s="98"/>
-      <c r="L144" s="98"/>
-      <c r="M144" s="98"/>
-      <c r="N144" s="98"/>
-      <c r="O144" s="98"/>
-      <c r="P144" s="98"/>
-      <c r="Q144" s="98"/>
-      <c r="R144" s="98"/>
-      <c r="S144" s="98"/>
-      <c r="T144" s="98"/>
-      <c r="U144" s="98"/>
-      <c r="V144" s="98"/>
-      <c r="W144" s="98"/>
-      <c r="X144" s="98"/>
-      <c r="Y144" s="98"/>
-      <c r="Z144" s="98"/>
-      <c r="AA144" s="98"/>
-      <c r="AB144" s="98"/>
-      <c r="AC144" s="98"/>
-      <c r="AD144" s="98"/>
-      <c r="AE144" s="98"/>
-      <c r="AF144" s="98"/>
-      <c r="AG144" s="98"/>
-      <c r="AH144" s="98"/>
-      <c r="AI144" s="98"/>
-      <c r="AJ144" s="98"/>
-      <c r="AK144" s="98"/>
-      <c r="AL144" s="98"/>
-      <c r="AM144" s="98"/>
-      <c r="AN144" s="98"/>
-      <c r="AO144" s="98"/>
-      <c r="AP144" s="98"/>
-      <c r="AQ144" s="98"/>
-      <c r="AR144" s="98"/>
-      <c r="AS144" s="98"/>
-      <c r="AT144" s="98"/>
-      <c r="AU144" s="98"/>
-      <c r="AV144" s="99"/>
+      <c r="J144" s="82"/>
+      <c r="K144" s="82"/>
+      <c r="L144" s="82"/>
+      <c r="M144" s="82"/>
+      <c r="N144" s="82"/>
+      <c r="O144" s="82"/>
+      <c r="P144" s="82"/>
+      <c r="Q144" s="82"/>
+      <c r="R144" s="82"/>
+      <c r="S144" s="82"/>
+      <c r="T144" s="82"/>
+      <c r="U144" s="82"/>
+      <c r="V144" s="82"/>
+      <c r="W144" s="82"/>
+      <c r="X144" s="82"/>
+      <c r="Y144" s="82"/>
+      <c r="Z144" s="82"/>
+      <c r="AA144" s="82"/>
+      <c r="AB144" s="82"/>
+      <c r="AC144" s="82"/>
+      <c r="AD144" s="82"/>
+      <c r="AE144" s="82"/>
+      <c r="AF144" s="82"/>
+      <c r="AG144" s="82"/>
+      <c r="AH144" s="82"/>
+      <c r="AI144" s="82"/>
+      <c r="AJ144" s="82"/>
+      <c r="AK144" s="82"/>
+      <c r="AL144" s="82"/>
+      <c r="AM144" s="82"/>
+      <c r="AN144" s="82"/>
+      <c r="AO144" s="82"/>
+      <c r="AP144" s="82"/>
+      <c r="AQ144" s="82"/>
+      <c r="AR144" s="82"/>
+      <c r="AS144" s="82"/>
+      <c r="AT144" s="82"/>
+      <c r="AU144" s="82"/>
+      <c r="AV144" s="83"/>
       <c r="AW144" s="6"/>
       <c r="AX144" s="6"/>
       <c r="AY144" s="6"/>
@@ -10678,52 +10718,52 @@
       <c r="G179" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I179" s="97" t="s">
+      <c r="I179" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="J179" s="98"/>
-      <c r="K179" s="98"/>
-      <c r="L179" s="98"/>
-      <c r="M179" s="98"/>
-      <c r="N179" s="98"/>
-      <c r="O179" s="98"/>
-      <c r="P179" s="98"/>
-      <c r="Q179" s="98"/>
-      <c r="R179" s="98"/>
-      <c r="S179" s="98"/>
-      <c r="T179" s="98"/>
-      <c r="U179" s="98"/>
-      <c r="V179" s="98"/>
-      <c r="W179" s="98"/>
-      <c r="X179" s="98"/>
-      <c r="Y179" s="98"/>
-      <c r="Z179" s="98"/>
-      <c r="AA179" s="98"/>
-      <c r="AB179" s="98"/>
-      <c r="AC179" s="98"/>
-      <c r="AD179" s="98"/>
-      <c r="AE179" s="98"/>
-      <c r="AF179" s="98"/>
-      <c r="AG179" s="98"/>
-      <c r="AH179" s="98"/>
-      <c r="AI179" s="98"/>
-      <c r="AJ179" s="98"/>
-      <c r="AK179" s="98"/>
-      <c r="AL179" s="98"/>
-      <c r="AM179" s="98"/>
-      <c r="AN179" s="98"/>
-      <c r="AO179" s="98"/>
-      <c r="AP179" s="98"/>
-      <c r="AQ179" s="98"/>
-      <c r="AR179" s="98"/>
-      <c r="AS179" s="98"/>
-      <c r="AT179" s="98"/>
-      <c r="AU179" s="98"/>
-      <c r="AV179" s="98"/>
-      <c r="AW179" s="98"/>
-      <c r="AX179" s="98"/>
-      <c r="AY179" s="98"/>
-      <c r="AZ179" s="99"/>
+      <c r="J179" s="82"/>
+      <c r="K179" s="82"/>
+      <c r="L179" s="82"/>
+      <c r="M179" s="82"/>
+      <c r="N179" s="82"/>
+      <c r="O179" s="82"/>
+      <c r="P179" s="82"/>
+      <c r="Q179" s="82"/>
+      <c r="R179" s="82"/>
+      <c r="S179" s="82"/>
+      <c r="T179" s="82"/>
+      <c r="U179" s="82"/>
+      <c r="V179" s="82"/>
+      <c r="W179" s="82"/>
+      <c r="X179" s="82"/>
+      <c r="Y179" s="82"/>
+      <c r="Z179" s="82"/>
+      <c r="AA179" s="82"/>
+      <c r="AB179" s="82"/>
+      <c r="AC179" s="82"/>
+      <c r="AD179" s="82"/>
+      <c r="AE179" s="82"/>
+      <c r="AF179" s="82"/>
+      <c r="AG179" s="82"/>
+      <c r="AH179" s="82"/>
+      <c r="AI179" s="82"/>
+      <c r="AJ179" s="82"/>
+      <c r="AK179" s="82"/>
+      <c r="AL179" s="82"/>
+      <c r="AM179" s="82"/>
+      <c r="AN179" s="82"/>
+      <c r="AO179" s="82"/>
+      <c r="AP179" s="82"/>
+      <c r="AQ179" s="82"/>
+      <c r="AR179" s="82"/>
+      <c r="AS179" s="82"/>
+      <c r="AT179" s="82"/>
+      <c r="AU179" s="82"/>
+      <c r="AV179" s="82"/>
+      <c r="AW179" s="82"/>
+      <c r="AX179" s="82"/>
+      <c r="AY179" s="82"/>
+      <c r="AZ179" s="83"/>
     </row>
     <row r="180" spans="2:52" ht="15.75" thickTop="1">
       <c r="B180" s="1"/>
@@ -12927,6 +12967,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AH28:AI28"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="B14:T28"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y11:AA11"/>
     <mergeCell ref="I179:AZ179"/>
     <mergeCell ref="B30:AA30"/>
     <mergeCell ref="G33:AA33"/>
@@ -12938,15 +12987,6 @@
     <mergeCell ref="J41:N41"/>
     <mergeCell ref="G104:AG104"/>
     <mergeCell ref="I144:AV144"/>
-    <mergeCell ref="AH28:AI28"/>
-    <mergeCell ref="AF28:AG28"/>
-    <mergeCell ref="B2:AA2"/>
-    <mergeCell ref="B4:T4"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="B14:T28"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y11:AA11"/>
   </mergeCells>
   <conditionalFormatting sqref="Y15:AA26 AE26 AC27:AE39">
     <cfRule type="expression" dxfId="3" priority="18">
@@ -13273,8 +13313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF1246F-240F-4F65-8DBE-618A3738E125}">
   <dimension ref="A1:U1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -13318,6 +13358,10 @@
       <c r="I3" s="79">
         <v>0</v>
       </c>
+      <c r="M3" s="79">
+        <f>I43</f>
+        <v>107</v>
+      </c>
       <c r="S3" s="79" t="s">
         <v>325</v>
       </c>
@@ -13344,13 +13388,20 @@
       <c r="G4" s="79">
         <v>1</v>
       </c>
-      <c r="H4" s="120">
+      <c r="H4" s="80">
         <f>--OR(F4:G4)</f>
         <v>1</v>
       </c>
       <c r="I4" s="79">
-        <f>IF(H4=1,_xlfn.XLOOKUP(I3+1,_nSevens,_nSevens,,1),I3+1)</f>
+        <f t="shared" ref="I4:I43" si="0">IF(H4=1,_xlfn.XLOOKUP(I3+1,_nSevens,_nSevens,,1),I3+1)</f>
         <v>7</v>
+      </c>
+      <c r="L4" s="79">
+        <v>31</v>
+      </c>
+      <c r="M4" s="79">
+        <f t="dataTable" ref="M4:M23" dt2D="0" dtr="0" r1="A1"/>
+        <v>75</v>
       </c>
       <c r="R4" s="79" cm="1">
         <f t="array" ref="R4:R1003">_xlfn.SEQUENCE(1000)</f>
@@ -13382,13 +13433,19 @@
       <c r="G5" s="79">
         <v>0</v>
       </c>
-      <c r="H5" s="120">
-        <f t="shared" ref="H5:H43" si="0">--OR(F5:G5)</f>
+      <c r="H5" s="80">
+        <f t="shared" ref="H5:H43" si="1">--OR(F5:G5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="79">
-        <f>IF(H5=1,_xlfn.XLOOKUP(I4+1,_nSevens,_nSevens,,1),I4+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
+      </c>
+      <c r="L5" s="79">
+        <v>32</v>
+      </c>
+      <c r="M5" s="79">
+        <v>107</v>
       </c>
       <c r="R5" s="79">
         <v>2</v>
@@ -13417,13 +13474,19 @@
       <c r="G6" s="79">
         <v>0</v>
       </c>
-      <c r="H6" s="120">
+      <c r="H6" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="79">
-        <f>IF(H6=1,_xlfn.XLOOKUP(I5+1,_nSevens,_nSevens,,1),I5+1)</f>
         <v>9</v>
+      </c>
+      <c r="L6" s="79">
+        <v>33</v>
+      </c>
+      <c r="M6" s="79">
+        <v>128</v>
       </c>
       <c r="R6" s="79">
         <v>3</v>
@@ -13452,13 +13515,19 @@
       <c r="G7" s="79">
         <v>0</v>
       </c>
-      <c r="H7" s="120">
+      <c r="H7" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I7" s="79">
-        <f>IF(H7=1,_xlfn.XLOOKUP(I6+1,_nSevens,_nSevens,,1),I6+1)</f>
         <v>17</v>
+      </c>
+      <c r="L7" s="79">
+        <v>34</v>
+      </c>
+      <c r="M7" s="79">
+        <v>107</v>
       </c>
       <c r="R7" s="79">
         <v>4</v>
@@ -13487,13 +13556,19 @@
       <c r="G8" s="79">
         <v>1</v>
       </c>
-      <c r="H8" s="120">
+      <c r="H8" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I8" s="79">
-        <f>IF(H8=1,_xlfn.XLOOKUP(I7+1,_nSevens,_nSevens,,1),I7+1)</f>
         <v>27</v>
+      </c>
+      <c r="L8" s="79">
+        <v>35</v>
+      </c>
+      <c r="M8" s="79">
+        <v>99</v>
       </c>
       <c r="R8" s="79">
         <v>5</v>
@@ -13522,13 +13597,19 @@
       <c r="G9" s="79">
         <v>0</v>
       </c>
-      <c r="H9" s="120">
+      <c r="H9" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="79">
-        <f>IF(H9=1,_xlfn.XLOOKUP(I8+1,_nSevens,_nSevens,,1),I8+1)</f>
         <v>28</v>
+      </c>
+      <c r="L9" s="79">
+        <v>36</v>
+      </c>
+      <c r="M9" s="79">
+        <v>97</v>
       </c>
       <c r="R9" s="79">
         <v>6</v>
@@ -13557,13 +13638,19 @@
       <c r="G10" s="79">
         <v>0</v>
       </c>
-      <c r="H10" s="120">
+      <c r="H10" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="79">
-        <f>IF(H10=1,_xlfn.XLOOKUP(I9+1,_nSevens,_nSevens,,1),I9+1)</f>
         <v>29</v>
+      </c>
+      <c r="L10" s="79">
+        <v>37</v>
+      </c>
+      <c r="M10" s="79">
+        <v>69</v>
       </c>
       <c r="R10" s="79">
         <v>7</v>
@@ -13592,13 +13679,19 @@
       <c r="G11" s="79">
         <v>0</v>
       </c>
-      <c r="H11" s="120">
+      <c r="H11" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="79">
-        <f>IF(H11=1,_xlfn.XLOOKUP(I10+1,_nSevens,_nSevens,,1),I10+1)</f>
         <v>30</v>
+      </c>
+      <c r="L11" s="79">
+        <v>38</v>
+      </c>
+      <c r="M11" s="79">
+        <v>117</v>
       </c>
       <c r="R11" s="79">
         <v>8</v>
@@ -13627,13 +13720,19 @@
       <c r="G12" s="79">
         <v>0</v>
       </c>
-      <c r="H12" s="120">
+      <c r="H12" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="79">
-        <f>IF(H12=1,_xlfn.XLOOKUP(I11+1,_nSevens,_nSevens,,1),I11+1)</f>
         <v>31</v>
+      </c>
+      <c r="L12" s="79">
+        <v>39</v>
+      </c>
+      <c r="M12" s="79">
+        <v>83</v>
       </c>
       <c r="R12" s="79">
         <v>9</v>
@@ -13662,13 +13761,19 @@
       <c r="G13" s="79">
         <v>0</v>
       </c>
-      <c r="H13" s="120">
+      <c r="H13" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="79">
-        <f>IF(H13=1,_xlfn.XLOOKUP(I12+1,_nSevens,_nSevens,,1),I12+1)</f>
         <v>32</v>
+      </c>
+      <c r="L13" s="79">
+        <v>40</v>
+      </c>
+      <c r="M13" s="79">
+        <v>102</v>
       </c>
       <c r="R13" s="79">
         <v>10</v>
@@ -13697,13 +13802,19 @@
       <c r="G14" s="79">
         <v>0</v>
       </c>
-      <c r="H14" s="120">
+      <c r="H14" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="79">
-        <f>IF(H14=1,_xlfn.XLOOKUP(I13+1,_nSevens,_nSevens,,1),I13+1)</f>
         <v>37</v>
+      </c>
+      <c r="L14" s="79">
+        <v>41</v>
+      </c>
+      <c r="M14" s="79">
+        <v>138</v>
       </c>
       <c r="R14" s="79">
         <v>11</v>
@@ -13732,13 +13843,19 @@
       <c r="G15" s="79">
         <v>0</v>
       </c>
-      <c r="H15" s="120">
+      <c r="H15" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="79">
-        <f>IF(H15=1,_xlfn.XLOOKUP(I14+1,_nSevens,_nSevens,,1),I14+1)</f>
         <v>38</v>
+      </c>
+      <c r="L15" s="79">
+        <v>42</v>
+      </c>
+      <c r="M15" s="79">
+        <v>113</v>
       </c>
       <c r="R15" s="79">
         <v>12</v>
@@ -13767,13 +13884,19 @@
       <c r="G16" s="79">
         <v>0</v>
       </c>
-      <c r="H16" s="120">
+      <c r="H16" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="79">
-        <f>IF(H16=1,_xlfn.XLOOKUP(I15+1,_nSevens,_nSevens,,1),I15+1)</f>
         <v>39</v>
+      </c>
+      <c r="L16" s="79">
+        <v>43</v>
+      </c>
+      <c r="M16" s="79">
+        <v>89</v>
       </c>
       <c r="R16" s="79">
         <v>13</v>
@@ -13802,13 +13925,19 @@
       <c r="G17" s="79">
         <v>0</v>
       </c>
-      <c r="H17" s="120">
+      <c r="H17" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="79">
-        <f>IF(H17=1,_xlfn.XLOOKUP(I16+1,_nSevens,_nSevens,,1),I16+1)</f>
         <v>40</v>
+      </c>
+      <c r="L17" s="79">
+        <v>44</v>
+      </c>
+      <c r="M17" s="79">
+        <v>97</v>
       </c>
       <c r="R17" s="79">
         <v>14</v>
@@ -13837,13 +13966,19 @@
       <c r="G18" s="79">
         <v>0</v>
       </c>
-      <c r="H18" s="120">
+      <c r="H18" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="79">
-        <f>IF(H18=1,_xlfn.XLOOKUP(I17+1,_nSevens,_nSevens,,1),I17+1)</f>
         <v>41</v>
+      </c>
+      <c r="L18" s="79">
+        <v>45</v>
+      </c>
+      <c r="M18" s="79">
+        <v>107</v>
       </c>
       <c r="R18" s="79">
         <v>15</v>
@@ -13872,13 +14007,19 @@
       <c r="G19" s="79">
         <v>0</v>
       </c>
-      <c r="H19" s="120">
+      <c r="H19" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I19" s="79">
-        <f>IF(H19=1,_xlfn.XLOOKUP(I18+1,_nSevens,_nSevens,,1),I18+1)</f>
         <v>47</v>
+      </c>
+      <c r="L19" s="79">
+        <v>46</v>
+      </c>
+      <c r="M19" s="79">
+        <v>89</v>
       </c>
       <c r="R19" s="79">
         <v>16</v>
@@ -13907,13 +14048,19 @@
       <c r="G20" s="79">
         <v>0</v>
       </c>
-      <c r="H20" s="120">
+      <c r="H20" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I20" s="79">
-        <f>IF(H20=1,_xlfn.XLOOKUP(I19+1,_nSevens,_nSevens,,1),I19+1)</f>
         <v>57</v>
+      </c>
+      <c r="L20" s="79">
+        <v>47</v>
+      </c>
+      <c r="M20" s="79">
+        <v>75</v>
       </c>
       <c r="R20" s="79">
         <v>17</v>
@@ -13942,13 +14089,19 @@
       <c r="G21" s="79">
         <v>0</v>
       </c>
-      <c r="H21" s="120">
+      <c r="H21" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="79">
-        <f>IF(H21=1,_xlfn.XLOOKUP(I20+1,_nSevens,_nSevens,,1),I20+1)</f>
         <v>58</v>
+      </c>
+      <c r="L21" s="79">
+        <v>48</v>
+      </c>
+      <c r="M21" s="79">
+        <v>90</v>
       </c>
       <c r="R21" s="79">
         <v>18</v>
@@ -13977,13 +14130,19 @@
       <c r="G22" s="79">
         <v>0</v>
       </c>
-      <c r="H22" s="120">
+      <c r="H22" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="79">
-        <f>IF(H22=1,_xlfn.XLOOKUP(I21+1,_nSevens,_nSevens,,1),I21+1)</f>
         <v>59</v>
+      </c>
+      <c r="L22" s="79">
+        <v>49</v>
+      </c>
+      <c r="M22" s="79">
+        <v>118</v>
       </c>
       <c r="R22" s="79">
         <v>19</v>
@@ -14012,13 +14171,19 @@
       <c r="G23" s="79">
         <v>0</v>
       </c>
-      <c r="H23" s="120">
+      <c r="H23" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="79">
-        <f>IF(H23=1,_xlfn.XLOOKUP(I22+1,_nSevens,_nSevens,,1),I22+1)</f>
         <v>60</v>
+      </c>
+      <c r="L23" s="79">
+        <v>50</v>
+      </c>
+      <c r="M23" s="79">
+        <v>112</v>
       </c>
       <c r="R23" s="79">
         <v>20</v>
@@ -14047,12 +14212,12 @@
       <c r="G24" s="79">
         <v>1</v>
       </c>
-      <c r="H24" s="120">
+      <c r="H24" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I24" s="79">
-        <f>IF(H24=1,_xlfn.XLOOKUP(I23+1,_nSevens,_nSevens,,1),I23+1)</f>
         <v>67</v>
       </c>
       <c r="R24" s="79">
@@ -14082,12 +14247,12 @@
       <c r="G25" s="79">
         <v>0</v>
       </c>
-      <c r="H25" s="120">
+      <c r="H25" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="79">
-        <f>IF(H25=1,_xlfn.XLOOKUP(I24+1,_nSevens,_nSevens,,1),I24+1)</f>
         <v>68</v>
       </c>
       <c r="R25" s="79">
@@ -14117,12 +14282,12 @@
       <c r="G26" s="79">
         <v>0</v>
       </c>
-      <c r="H26" s="120">
+      <c r="H26" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="79">
-        <f>IF(H26=1,_xlfn.XLOOKUP(I25+1,_nSevens,_nSevens,,1),I25+1)</f>
         <v>69</v>
       </c>
       <c r="R26" s="79">
@@ -14152,12 +14317,12 @@
       <c r="G27" s="79">
         <v>0</v>
       </c>
-      <c r="H27" s="120">
+      <c r="H27" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I27" s="79">
-        <f>IF(H27=1,_xlfn.XLOOKUP(I26+1,_nSevens,_nSevens,,1),I26+1)</f>
         <v>70</v>
       </c>
       <c r="R27" s="79">
@@ -14187,12 +14352,12 @@
       <c r="G28" s="79">
         <v>0</v>
       </c>
-      <c r="H28" s="120">
+      <c r="H28" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="79">
-        <f>IF(H28=1,_xlfn.XLOOKUP(I27+1,_nSevens,_nSevens,,1),I27+1)</f>
         <v>71</v>
       </c>
       <c r="R28" s="79">
@@ -14222,12 +14387,12 @@
       <c r="G29" s="79">
         <v>1</v>
       </c>
-      <c r="H29" s="120">
+      <c r="H29" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I29" s="79">
-        <f>IF(H29=1,_xlfn.XLOOKUP(I28+1,_nSevens,_nSevens,,1),I28+1)</f>
         <v>72</v>
       </c>
       <c r="R29" s="79">
@@ -14257,12 +14422,12 @@
       <c r="G30" s="79">
         <v>0</v>
       </c>
-      <c r="H30" s="120">
+      <c r="H30" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="79">
-        <f>IF(H30=1,_xlfn.XLOOKUP(I29+1,_nSevens,_nSevens,,1),I29+1)</f>
         <v>73</v>
       </c>
       <c r="R30" s="79">
@@ -14292,12 +14457,12 @@
       <c r="G31" s="79">
         <v>0</v>
       </c>
-      <c r="H31" s="120">
+      <c r="H31" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="79">
-        <f>IF(H31=1,_xlfn.XLOOKUP(I30+1,_nSevens,_nSevens,,1),I30+1)</f>
         <v>74</v>
       </c>
       <c r="R31" s="79">
@@ -14327,12 +14492,12 @@
       <c r="G32" s="79">
         <v>0</v>
       </c>
-      <c r="H32" s="120">
+      <c r="H32" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="79">
-        <f>IF(H32=1,_xlfn.XLOOKUP(I31+1,_nSevens,_nSevens,,1),I31+1)</f>
         <v>75</v>
       </c>
       <c r="R32" s="79">
@@ -14362,12 +14527,12 @@
       <c r="G33" s="79">
         <v>0</v>
       </c>
-      <c r="H33" s="120">
+      <c r="H33" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="79">
-        <f>IF(H33=1,_xlfn.XLOOKUP(I32+1,_nSevens,_nSevens,,1),I32+1)</f>
         <v>76</v>
       </c>
       <c r="R33" s="79">
@@ -14397,12 +14562,12 @@
       <c r="G34" s="79">
         <v>0</v>
       </c>
-      <c r="H34" s="120">
+      <c r="H34" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="79">
-        <f>IF(H34=1,_xlfn.XLOOKUP(I33+1,_nSevens,_nSevens,,1),I33+1)</f>
         <v>77</v>
       </c>
       <c r="R34" s="79">
@@ -14432,12 +14597,12 @@
       <c r="G35" s="79">
         <v>0</v>
       </c>
-      <c r="H35" s="120">
+      <c r="H35" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="79">
-        <f>IF(H35=1,_xlfn.XLOOKUP(I34+1,_nSevens,_nSevens,,1),I34+1)</f>
         <v>78</v>
       </c>
       <c r="R35" s="79">
@@ -14467,12 +14632,12 @@
       <c r="G36" s="79">
         <v>0</v>
       </c>
-      <c r="H36" s="120">
+      <c r="H36" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="79">
-        <f>IF(H36=1,_xlfn.XLOOKUP(I35+1,_nSevens,_nSevens,,1),I35+1)</f>
         <v>79</v>
       </c>
       <c r="R36" s="79">
@@ -14502,12 +14667,12 @@
       <c r="G37" s="79">
         <v>0</v>
       </c>
-      <c r="H37" s="120">
+      <c r="H37" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="79">
-        <f>IF(H37=1,_xlfn.XLOOKUP(I36+1,_nSevens,_nSevens,,1),I36+1)</f>
         <v>80</v>
       </c>
       <c r="R37" s="79">
@@ -14537,12 +14702,12 @@
       <c r="G38" s="79">
         <v>1</v>
       </c>
-      <c r="H38" s="120">
+      <c r="H38" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I38" s="79">
-        <f>IF(H38=1,_xlfn.XLOOKUP(I37+1,_nSevens,_nSevens,,1),I37+1)</f>
         <v>87</v>
       </c>
       <c r="R38" s="79">
@@ -14572,12 +14737,12 @@
       <c r="G39" s="79">
         <v>0</v>
       </c>
-      <c r="H39" s="120">
+      <c r="H39" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I39" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I39" s="79">
-        <f>IF(H39=1,_xlfn.XLOOKUP(I38+1,_nSevens,_nSevens,,1),I38+1)</f>
         <v>97</v>
       </c>
       <c r="R39" s="79">
@@ -14607,12 +14772,12 @@
       <c r="G40" s="79">
         <v>0</v>
       </c>
-      <c r="H40" s="120">
+      <c r="H40" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="79">
-        <f>IF(H40=1,_xlfn.XLOOKUP(I39+1,_nSevens,_nSevens,,1),I39+1)</f>
         <v>98</v>
       </c>
       <c r="R40" s="79">
@@ -14642,12 +14807,12 @@
       <c r="G41" s="79">
         <v>0</v>
       </c>
-      <c r="H41" s="120">
+      <c r="H41" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="79">
-        <f>IF(H41=1,_xlfn.XLOOKUP(I40+1,_nSevens,_nSevens,,1),I40+1)</f>
         <v>99</v>
       </c>
       <c r="R41" s="79">
@@ -14677,12 +14842,12 @@
       <c r="G42" s="79">
         <v>0</v>
       </c>
-      <c r="H42" s="120">
+      <c r="H42" s="80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="79">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="79">
-        <f>IF(H42=1,_xlfn.XLOOKUP(I41+1,_nSevens,_nSevens,,1),I41+1)</f>
         <v>100</v>
       </c>
       <c r="R42" s="79">
@@ -14712,12 +14877,12 @@
       <c r="G43" s="79">
         <v>0</v>
       </c>
-      <c r="H43" s="120">
+      <c r="H43" s="80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I43" s="79">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I43" s="79">
-        <f>IF(H43=1,_xlfn.XLOOKUP(I42+1,_nSevens,_nSevens,,1),I42+1)</f>
         <v>107</v>
       </c>
       <c r="R43" s="79">
@@ -23105,6 +23270,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -37012,34 +37178,34 @@
       <c r="BD1" s="6"/>
     </row>
     <row r="2" spans="2:56" ht="60.6" customHeight="1">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="105" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="81"/>
-      <c r="AA2" s="81"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
       <c r="AO2" s="3"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6"/>
@@ -37063,32 +37229,32 @@
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="2:56" ht="33.6" customHeight="1">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="Y4" s="93" t="s">
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="106"/>
+      <c r="T4" s="106"/>
+      <c r="Y4" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="82"/>
+      <c r="Z4" s="117"/>
+      <c r="AA4" s="106"/>
       <c r="AO4" s="3"/>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -37316,11 +37482,11 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
       <c r="X11" s="31"/>
-      <c r="Y11" s="94" t="s">
+      <c r="Y11" s="118" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="95"/>
-      <c r="AA11" s="96"/>
+      <c r="Z11" s="119"/>
+      <c r="AA11" s="120"/>
       <c r="AO11" s="3"/>
       <c r="AY11" s="6"/>
       <c r="AZ11" s="6"/>
@@ -37365,33 +37531,33 @@
       <c r="BD12" s="6"/>
     </row>
     <row r="13" spans="2:56" ht="24.95" customHeight="1" thickBot="1">
-      <c r="B13" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="82"/>
-      <c r="T13" s="82"/>
+      <c r="B13" s="107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
+      <c r="R13" s="106"/>
+      <c r="S13" s="106"/>
+      <c r="T13" s="106"/>
       <c r="U13" s="60"/>
-      <c r="Y13" s="83" t="s">
+      <c r="Y13" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="Z13" s="82"/>
-      <c r="AA13" s="82"/>
+      <c r="Z13" s="106"/>
+      <c r="AA13" s="106"/>
       <c r="AF13" s="60"/>
       <c r="AG13" s="60"/>
       <c r="AH13" s="60"/>
@@ -37399,27 +37565,27 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:56" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="108" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="86"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="109"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="109"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="109"/>
+      <c r="S14" s="109"/>
+      <c r="T14" s="110"/>
       <c r="U14" s="3"/>
       <c r="Y14" s="61" t="s">
         <v>31</v>
@@ -37436,25 +37602,25 @@
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:56" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="88"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="88"/>
-      <c r="T15" s="89"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="112"/>
+      <c r="P15" s="112"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="112"/>
+      <c r="S15" s="112"/>
+      <c r="T15" s="113"/>
       <c r="U15" s="3"/>
       <c r="Y15" s="62" t="s">
         <v>32</v>
@@ -37471,25 +37637,25 @@
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B16" s="87"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="89"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="112"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="112"/>
+      <c r="O16" s="112"/>
+      <c r="P16" s="112"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
+      <c r="T16" s="113"/>
       <c r="U16" s="3"/>
       <c r="Y16" s="62" t="s">
         <v>47</v>
@@ -37505,25 +37671,25 @@
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B17" s="87"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="88"/>
-      <c r="P17" s="88"/>
-      <c r="Q17" s="88"/>
-      <c r="R17" s="88"/>
-      <c r="S17" s="88"/>
-      <c r="T17" s="89"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="112"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="112"/>
+      <c r="N17" s="112"/>
+      <c r="O17" s="112"/>
+      <c r="P17" s="112"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112"/>
+      <c r="T17" s="113"/>
       <c r="U17" s="3"/>
       <c r="Y17" s="62" t="s">
         <v>39</v>
@@ -37539,25 +37705,25 @@
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B18" s="87"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="88"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="88"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-      <c r="T18" s="89"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
+      <c r="N18" s="112"/>
+      <c r="O18" s="112"/>
+      <c r="P18" s="112"/>
+      <c r="Q18" s="112"/>
+      <c r="R18" s="112"/>
+      <c r="S18" s="112"/>
+      <c r="T18" s="113"/>
       <c r="U18" s="3"/>
       <c r="Y18" s="62" t="s">
         <v>35</v>
@@ -37573,25 +37739,25 @@
       <c r="AO18" s="3"/>
     </row>
     <row r="19" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B19" s="87"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="88"/>
-      <c r="R19" s="88"/>
-      <c r="S19" s="88"/>
-      <c r="T19" s="89"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="112"/>
+      <c r="N19" s="112"/>
+      <c r="O19" s="112"/>
+      <c r="P19" s="112"/>
+      <c r="Q19" s="112"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="112"/>
+      <c r="T19" s="113"/>
       <c r="U19" s="3"/>
       <c r="Y19" s="62" t="s">
         <v>42</v>
@@ -37607,25 +37773,25 @@
       <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B20" s="87"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="88"/>
-      <c r="S20" s="88"/>
-      <c r="T20" s="89"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="112"/>
+      <c r="M20" s="112"/>
+      <c r="N20" s="112"/>
+      <c r="O20" s="112"/>
+      <c r="P20" s="112"/>
+      <c r="Q20" s="112"/>
+      <c r="R20" s="112"/>
+      <c r="S20" s="112"/>
+      <c r="T20" s="113"/>
       <c r="U20" s="3"/>
       <c r="Y20" s="62" t="s">
         <v>48</v>
@@ -37639,25 +37805,25 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B21" s="87"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="88"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
-      <c r="Q21" s="88"/>
-      <c r="R21" s="88"/>
-      <c r="S21" s="88"/>
-      <c r="T21" s="89"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
+      <c r="M21" s="112"/>
+      <c r="N21" s="112"/>
+      <c r="O21" s="112"/>
+      <c r="P21" s="112"/>
+      <c r="Q21" s="112"/>
+      <c r="R21" s="112"/>
+      <c r="S21" s="112"/>
+      <c r="T21" s="113"/>
       <c r="U21" s="3"/>
       <c r="Y21" s="62" t="s">
         <v>49</v>
@@ -37673,25 +37839,25 @@
       <c r="AO21" s="3"/>
     </row>
     <row r="22" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B22" s="87"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="88"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="88"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88"/>
-      <c r="Q22" s="88"/>
-      <c r="R22" s="88"/>
-      <c r="S22" s="88"/>
-      <c r="T22" s="89"/>
+      <c r="B22" s="111"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="112"/>
+      <c r="O22" s="112"/>
+      <c r="P22" s="112"/>
+      <c r="Q22" s="112"/>
+      <c r="R22" s="112"/>
+      <c r="S22" s="112"/>
+      <c r="T22" s="113"/>
       <c r="U22" s="3"/>
       <c r="Y22" s="62" t="s">
         <v>50</v>
@@ -37708,25 +37874,25 @@
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="89"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="112"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="112"/>
+      <c r="M23" s="112"/>
+      <c r="N23" s="112"/>
+      <c r="O23" s="112"/>
+      <c r="P23" s="112"/>
+      <c r="Q23" s="112"/>
+      <c r="R23" s="112"/>
+      <c r="S23" s="112"/>
+      <c r="T23" s="113"/>
       <c r="U23" s="3"/>
       <c r="Y23" s="62" t="s">
         <v>51</v>
@@ -37743,25 +37909,25 @@
       <c r="AP23" s="3"/>
     </row>
     <row r="24" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="88"/>
-      <c r="S24" s="88"/>
-      <c r="T24" s="89"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="112"/>
+      <c r="R24" s="112"/>
+      <c r="S24" s="112"/>
+      <c r="T24" s="113"/>
       <c r="U24" s="3"/>
       <c r="Y24" s="62" t="s">
         <v>52</v>
@@ -37778,25 +37944,25 @@
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B25" s="87"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="88"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="88"/>
-      <c r="Q25" s="88"/>
-      <c r="R25" s="88"/>
-      <c r="S25" s="88"/>
-      <c r="T25" s="89"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="112"/>
+      <c r="H25" s="112"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
+      <c r="K25" s="112"/>
+      <c r="L25" s="112"/>
+      <c r="M25" s="112"/>
+      <c r="N25" s="112"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="112"/>
+      <c r="Q25" s="112"/>
+      <c r="R25" s="112"/>
+      <c r="S25" s="112"/>
+      <c r="T25" s="113"/>
       <c r="U25" s="3"/>
       <c r="Y25" s="62" t="s">
         <v>53</v>
@@ -37811,25 +37977,25 @@
       <c r="AP25" s="3"/>
     </row>
     <row r="26" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="88"/>
-      <c r="T26" s="89"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="112"/>
+      <c r="M26" s="112"/>
+      <c r="N26" s="112"/>
+      <c r="O26" s="112"/>
+      <c r="P26" s="112"/>
+      <c r="Q26" s="112"/>
+      <c r="R26" s="112"/>
+      <c r="S26" s="112"/>
+      <c r="T26" s="113"/>
       <c r="U26" s="3"/>
       <c r="Y26" s="62" t="s">
         <v>105</v>
@@ -37849,25 +38015,25 @@
       <c r="AP26" s="3"/>
     </row>
     <row r="27" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="88"/>
-      <c r="R27" s="88"/>
-      <c r="S27" s="88"/>
-      <c r="T27" s="89"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="112"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
+      <c r="M27" s="112"/>
+      <c r="N27" s="112"/>
+      <c r="O27" s="112"/>
+      <c r="P27" s="112"/>
+      <c r="Q27" s="112"/>
+      <c r="R27" s="112"/>
+      <c r="S27" s="112"/>
+      <c r="T27" s="113"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -37886,25 +38052,25 @@
       <c r="AP27" s="3"/>
     </row>
     <row r="28" spans="2:56" ht="47.25" customHeight="1">
-      <c r="B28" s="90"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="91"/>
-      <c r="L28" s="91"/>
-      <c r="M28" s="91"/>
-      <c r="N28" s="91"/>
-      <c r="O28" s="91"/>
-      <c r="P28" s="91"/>
-      <c r="Q28" s="91"/>
-      <c r="R28" s="91"/>
-      <c r="S28" s="91"/>
-      <c r="T28" s="92"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="115"/>
+      <c r="M28" s="115"/>
+      <c r="N28" s="115"/>
+      <c r="O28" s="115"/>
+      <c r="P28" s="115"/>
+      <c r="Q28" s="115"/>
+      <c r="R28" s="115"/>
+      <c r="S28" s="115"/>
+      <c r="T28" s="116"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -37915,10 +38081,10 @@
       <c r="AC28" s="63"/>
       <c r="AD28" s="63"/>
       <c r="AE28" s="64"/>
-      <c r="AF28" s="80"/>
-      <c r="AG28" s="80"/>
-      <c r="AH28" s="80"/>
-      <c r="AI28" s="80"/>
+      <c r="AF28" s="104"/>
+      <c r="AG28" s="104"/>
+      <c r="AH28" s="104"/>
+      <c r="AI28" s="104"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
     </row>
@@ -37967,34 +38133,34 @@
       <c r="BD29" s="6"/>
     </row>
     <row r="30" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-      <c r="I30" s="101"/>
-      <c r="J30" s="101"/>
-      <c r="K30" s="101"/>
-      <c r="L30" s="101"/>
-      <c r="M30" s="101"/>
-      <c r="N30" s="101"/>
-      <c r="O30" s="101"/>
-      <c r="P30" s="101"/>
-      <c r="Q30" s="101"/>
-      <c r="R30" s="101"/>
-      <c r="S30" s="101"/>
-      <c r="T30" s="101"/>
-      <c r="U30" s="101"/>
-      <c r="V30" s="101"/>
-      <c r="W30" s="101"/>
-      <c r="X30" s="101"/>
-      <c r="Y30" s="101"/>
-      <c r="Z30" s="101"/>
-      <c r="AA30" s="102"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="85"/>
+      <c r="O30" s="85"/>
+      <c r="P30" s="85"/>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="85"/>
+      <c r="V30" s="85"/>
+      <c r="W30" s="85"/>
+      <c r="X30" s="85"/>
+      <c r="Y30" s="85"/>
+      <c r="Z30" s="85"/>
+      <c r="AA30" s="86"/>
       <c r="AC30" s="63"/>
       <c r="AD30" s="63"/>
       <c r="AE30" s="64"/>
@@ -38057,29 +38223,29 @@
       <c r="E33" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="103" t="s">
+      <c r="G33" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="104"/>
-      <c r="I33" s="104"/>
-      <c r="J33" s="104"/>
-      <c r="K33" s="104"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
-      <c r="O33" s="104"/>
-      <c r="P33" s="104"/>
-      <c r="Q33" s="104"/>
-      <c r="R33" s="104"/>
-      <c r="S33" s="104"/>
-      <c r="T33" s="104"/>
-      <c r="U33" s="104"/>
-      <c r="V33" s="104"/>
-      <c r="W33" s="104"/>
-      <c r="X33" s="104"/>
-      <c r="Y33" s="104"/>
-      <c r="Z33" s="104"/>
-      <c r="AA33" s="105"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="88"/>
+      <c r="P33" s="88"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="88"/>
+      <c r="S33" s="88"/>
+      <c r="T33" s="88"/>
+      <c r="U33" s="88"/>
+      <c r="V33" s="88"/>
+      <c r="W33" s="88"/>
+      <c r="X33" s="88"/>
+      <c r="Y33" s="88"/>
+      <c r="Z33" s="88"/>
+      <c r="AA33" s="89"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="63"/>
       <c r="AE33" s="64"/>
@@ -38102,29 +38268,29 @@
         <v>29</v>
       </c>
       <c r="F34" s="36"/>
-      <c r="G34" s="106" t="s">
+      <c r="G34" s="90" t="s">
         <v>302</v>
       </c>
-      <c r="H34" s="107"/>
-      <c r="I34" s="107"/>
-      <c r="J34" s="107"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="107"/>
-      <c r="O34" s="107"/>
-      <c r="P34" s="107"/>
-      <c r="Q34" s="107"/>
-      <c r="R34" s="107"/>
-      <c r="S34" s="107"/>
-      <c r="T34" s="107"/>
-      <c r="U34" s="107"/>
-      <c r="V34" s="107"/>
-      <c r="W34" s="107"/>
-      <c r="X34" s="107"/>
-      <c r="Y34" s="107"/>
-      <c r="Z34" s="107"/>
-      <c r="AA34" s="108"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="91"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="91"/>
+      <c r="P34" s="91"/>
+      <c r="Q34" s="91"/>
+      <c r="R34" s="91"/>
+      <c r="S34" s="91"/>
+      <c r="T34" s="91"/>
+      <c r="U34" s="91"/>
+      <c r="V34" s="91"/>
+      <c r="W34" s="91"/>
+      <c r="X34" s="91"/>
+      <c r="Y34" s="91"/>
+      <c r="Z34" s="91"/>
+      <c r="AA34" s="92"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="63"/>
       <c r="AE34" s="64"/>
@@ -38147,29 +38313,29 @@
         <v>51</v>
       </c>
       <c r="F35" s="36"/>
-      <c r="G35" s="109" t="s">
+      <c r="G35" s="93" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="110"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="110"/>
-      <c r="L35" s="110"/>
-      <c r="M35" s="110"/>
-      <c r="N35" s="110"/>
-      <c r="O35" s="110"/>
-      <c r="P35" s="110"/>
-      <c r="Q35" s="110"/>
-      <c r="R35" s="110"/>
-      <c r="S35" s="110"/>
-      <c r="T35" s="110"/>
-      <c r="U35" s="110"/>
-      <c r="V35" s="110"/>
-      <c r="W35" s="110"/>
-      <c r="X35" s="110"/>
-      <c r="Y35" s="110"/>
-      <c r="Z35" s="110"/>
-      <c r="AA35" s="111"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="94"/>
+      <c r="R35" s="94"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="94"/>
+      <c r="X35" s="94"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="95"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="63"/>
       <c r="AE35" s="64"/>
@@ -38192,29 +38358,29 @@
         <v>95</v>
       </c>
       <c r="F36" s="36"/>
-      <c r="G36" s="112" t="s">
+      <c r="G36" s="96" t="s">
         <v>301</v>
       </c>
-      <c r="H36" s="113"/>
-      <c r="I36" s="113"/>
-      <c r="J36" s="113"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="113"/>
-      <c r="M36" s="113"/>
-      <c r="N36" s="113"/>
-      <c r="O36" s="113"/>
-      <c r="P36" s="113"/>
-      <c r="Q36" s="113"/>
-      <c r="R36" s="113"/>
-      <c r="S36" s="113"/>
-      <c r="T36" s="113"/>
-      <c r="U36" s="113"/>
-      <c r="V36" s="113"/>
-      <c r="W36" s="113"/>
-      <c r="X36" s="113"/>
-      <c r="Y36" s="113"/>
-      <c r="Z36" s="113"/>
-      <c r="AA36" s="114"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="97"/>
+      <c r="O36" s="97"/>
+      <c r="P36" s="97"/>
+      <c r="Q36" s="97"/>
+      <c r="R36" s="97"/>
+      <c r="S36" s="97"/>
+      <c r="T36" s="97"/>
+      <c r="U36" s="97"/>
+      <c r="V36" s="97"/>
+      <c r="W36" s="97"/>
+      <c r="X36" s="97"/>
+      <c r="Y36" s="97"/>
+      <c r="Z36" s="97"/>
+      <c r="AA36" s="98"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="63"/>
       <c r="AE36" s="64"/>
@@ -39683,20 +39849,20 @@
       <c r="E67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="103" t="s">
+      <c r="G67" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="H67" s="104"/>
-      <c r="I67" s="104"/>
-      <c r="J67" s="104"/>
-      <c r="K67" s="104"/>
-      <c r="L67" s="104"/>
-      <c r="M67" s="104"/>
-      <c r="N67" s="104"/>
-      <c r="O67" s="104"/>
-      <c r="P67" s="104"/>
-      <c r="Q67" s="104"/>
-      <c r="R67" s="105"/>
+      <c r="H67" s="88"/>
+      <c r="I67" s="88"/>
+      <c r="J67" s="88"/>
+      <c r="K67" s="88"/>
+      <c r="L67" s="88"/>
+      <c r="M67" s="88"/>
+      <c r="N67" s="88"/>
+      <c r="O67" s="88"/>
+      <c r="P67" s="88"/>
+      <c r="Q67" s="88"/>
+      <c r="R67" s="89"/>
       <c r="S67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -41736,34 +41902,34 @@
       <c r="E104" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G104" s="117" t="s">
+      <c r="G104" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="H104" s="118"/>
-      <c r="I104" s="118"/>
-      <c r="J104" s="118"/>
-      <c r="K104" s="118"/>
-      <c r="L104" s="118"/>
-      <c r="M104" s="118"/>
-      <c r="N104" s="118"/>
-      <c r="O104" s="118"/>
-      <c r="P104" s="118"/>
-      <c r="Q104" s="118"/>
-      <c r="R104" s="118"/>
-      <c r="S104" s="118"/>
-      <c r="T104" s="118"/>
-      <c r="U104" s="118"/>
-      <c r="V104" s="118"/>
-      <c r="W104" s="118"/>
-      <c r="X104" s="118"/>
-      <c r="Y104" s="118"/>
-      <c r="Z104" s="118"/>
-      <c r="AA104" s="118"/>
-      <c r="AB104" s="118"/>
-      <c r="AC104" s="118"/>
-      <c r="AD104" s="118"/>
-      <c r="AE104" s="118"/>
-      <c r="AF104" s="119"/>
+      <c r="H104" s="102"/>
+      <c r="I104" s="102"/>
+      <c r="J104" s="102"/>
+      <c r="K104" s="102"/>
+      <c r="L104" s="102"/>
+      <c r="M104" s="102"/>
+      <c r="N104" s="102"/>
+      <c r="O104" s="102"/>
+      <c r="P104" s="102"/>
+      <c r="Q104" s="102"/>
+      <c r="R104" s="102"/>
+      <c r="S104" s="102"/>
+      <c r="T104" s="102"/>
+      <c r="U104" s="102"/>
+      <c r="V104" s="102"/>
+      <c r="W104" s="102"/>
+      <c r="X104" s="102"/>
+      <c r="Y104" s="102"/>
+      <c r="Z104" s="102"/>
+      <c r="AA104" s="102"/>
+      <c r="AB104" s="102"/>
+      <c r="AC104" s="102"/>
+      <c r="AD104" s="102"/>
+      <c r="AE104" s="102"/>
+      <c r="AF104" s="103"/>
       <c r="AG104" s="6"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
@@ -43479,47 +43645,47 @@
       <c r="G144" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I144" s="97" t="s">
+      <c r="I144" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="J144" s="98"/>
-      <c r="K144" s="98"/>
-      <c r="L144" s="98"/>
-      <c r="M144" s="98"/>
-      <c r="N144" s="98"/>
-      <c r="O144" s="98"/>
-      <c r="P144" s="98"/>
-      <c r="Q144" s="98"/>
-      <c r="R144" s="98"/>
-      <c r="S144" s="98"/>
-      <c r="T144" s="98"/>
-      <c r="U144" s="98"/>
-      <c r="V144" s="98"/>
-      <c r="W144" s="98"/>
-      <c r="X144" s="98"/>
-      <c r="Y144" s="98"/>
-      <c r="Z144" s="98"/>
-      <c r="AA144" s="98"/>
-      <c r="AB144" s="98"/>
-      <c r="AC144" s="98"/>
-      <c r="AD144" s="98"/>
-      <c r="AE144" s="98"/>
-      <c r="AF144" s="98"/>
-      <c r="AG144" s="98"/>
-      <c r="AH144" s="98"/>
-      <c r="AI144" s="98"/>
-      <c r="AJ144" s="98"/>
-      <c r="AK144" s="98"/>
-      <c r="AL144" s="98"/>
-      <c r="AM144" s="98"/>
-      <c r="AN144" s="98"/>
-      <c r="AO144" s="98"/>
-      <c r="AP144" s="98"/>
-      <c r="AQ144" s="98"/>
-      <c r="AR144" s="98"/>
-      <c r="AS144" s="98"/>
-      <c r="AT144" s="98"/>
-      <c r="AU144" s="99"/>
+      <c r="J144" s="82"/>
+      <c r="K144" s="82"/>
+      <c r="L144" s="82"/>
+      <c r="M144" s="82"/>
+      <c r="N144" s="82"/>
+      <c r="O144" s="82"/>
+      <c r="P144" s="82"/>
+      <c r="Q144" s="82"/>
+      <c r="R144" s="82"/>
+      <c r="S144" s="82"/>
+      <c r="T144" s="82"/>
+      <c r="U144" s="82"/>
+      <c r="V144" s="82"/>
+      <c r="W144" s="82"/>
+      <c r="X144" s="82"/>
+      <c r="Y144" s="82"/>
+      <c r="Z144" s="82"/>
+      <c r="AA144" s="82"/>
+      <c r="AB144" s="82"/>
+      <c r="AC144" s="82"/>
+      <c r="AD144" s="82"/>
+      <c r="AE144" s="82"/>
+      <c r="AF144" s="82"/>
+      <c r="AG144" s="82"/>
+      <c r="AH144" s="82"/>
+      <c r="AI144" s="82"/>
+      <c r="AJ144" s="82"/>
+      <c r="AK144" s="82"/>
+      <c r="AL144" s="82"/>
+      <c r="AM144" s="82"/>
+      <c r="AN144" s="82"/>
+      <c r="AO144" s="82"/>
+      <c r="AP144" s="82"/>
+      <c r="AQ144" s="82"/>
+      <c r="AR144" s="82"/>
+      <c r="AS144" s="82"/>
+      <c r="AT144" s="82"/>
+      <c r="AU144" s="83"/>
       <c r="AV144" s="6"/>
       <c r="AW144" s="6"/>
       <c r="AX144" s="6"/>
@@ -45171,55 +45337,55 @@
       <c r="G179" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I179" s="97" t="s">
+      <c r="I179" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="J179" s="98"/>
-      <c r="K179" s="98"/>
-      <c r="L179" s="98"/>
-      <c r="M179" s="98"/>
-      <c r="N179" s="98"/>
-      <c r="O179" s="98"/>
-      <c r="P179" s="98"/>
-      <c r="Q179" s="98"/>
-      <c r="R179" s="98"/>
-      <c r="S179" s="98"/>
-      <c r="T179" s="98"/>
-      <c r="U179" s="98"/>
-      <c r="V179" s="98"/>
-      <c r="W179" s="98"/>
-      <c r="X179" s="98"/>
-      <c r="Y179" s="98"/>
-      <c r="Z179" s="98"/>
-      <c r="AA179" s="98"/>
-      <c r="AB179" s="98"/>
-      <c r="AC179" s="98"/>
-      <c r="AD179" s="98"/>
-      <c r="AE179" s="98"/>
-      <c r="AF179" s="98"/>
-      <c r="AG179" s="98"/>
-      <c r="AH179" s="98"/>
-      <c r="AI179" s="98"/>
-      <c r="AJ179" s="98"/>
-      <c r="AK179" s="98"/>
-      <c r="AL179" s="98"/>
-      <c r="AM179" s="98"/>
-      <c r="AN179" s="98"/>
-      <c r="AO179" s="98"/>
-      <c r="AP179" s="98"/>
-      <c r="AQ179" s="98"/>
-      <c r="AR179" s="98"/>
-      <c r="AS179" s="98"/>
-      <c r="AT179" s="98"/>
-      <c r="AU179" s="98"/>
-      <c r="AV179" s="98"/>
-      <c r="AW179" s="98"/>
-      <c r="AX179" s="98"/>
-      <c r="AY179" s="98"/>
-      <c r="AZ179" s="98"/>
-      <c r="BA179" s="98"/>
-      <c r="BB179" s="98"/>
-      <c r="BC179" s="99"/>
+      <c r="J179" s="82"/>
+      <c r="K179" s="82"/>
+      <c r="L179" s="82"/>
+      <c r="M179" s="82"/>
+      <c r="N179" s="82"/>
+      <c r="O179" s="82"/>
+      <c r="P179" s="82"/>
+      <c r="Q179" s="82"/>
+      <c r="R179" s="82"/>
+      <c r="S179" s="82"/>
+      <c r="T179" s="82"/>
+      <c r="U179" s="82"/>
+      <c r="V179" s="82"/>
+      <c r="W179" s="82"/>
+      <c r="X179" s="82"/>
+      <c r="Y179" s="82"/>
+      <c r="Z179" s="82"/>
+      <c r="AA179" s="82"/>
+      <c r="AB179" s="82"/>
+      <c r="AC179" s="82"/>
+      <c r="AD179" s="82"/>
+      <c r="AE179" s="82"/>
+      <c r="AF179" s="82"/>
+      <c r="AG179" s="82"/>
+      <c r="AH179" s="82"/>
+      <c r="AI179" s="82"/>
+      <c r="AJ179" s="82"/>
+      <c r="AK179" s="82"/>
+      <c r="AL179" s="82"/>
+      <c r="AM179" s="82"/>
+      <c r="AN179" s="82"/>
+      <c r="AO179" s="82"/>
+      <c r="AP179" s="82"/>
+      <c r="AQ179" s="82"/>
+      <c r="AR179" s="82"/>
+      <c r="AS179" s="82"/>
+      <c r="AT179" s="82"/>
+      <c r="AU179" s="82"/>
+      <c r="AV179" s="82"/>
+      <c r="AW179" s="82"/>
+      <c r="AX179" s="82"/>
+      <c r="AY179" s="82"/>
+      <c r="AZ179" s="82"/>
+      <c r="BA179" s="82"/>
+      <c r="BB179" s="82"/>
+      <c r="BC179" s="83"/>
       <c r="BD179" s="6"/>
     </row>
     <row r="180" spans="2:56" ht="15.75" thickTop="1">
@@ -47535,12 +47701,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:AA2"/>
-    <mergeCell ref="B4:T4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="G36:AA36"/>
+    <mergeCell ref="G67:R67"/>
+    <mergeCell ref="I179:BC179"/>
+    <mergeCell ref="I144:AU144"/>
+    <mergeCell ref="G104:AF104"/>
     <mergeCell ref="AF28:AG28"/>
     <mergeCell ref="AH28:AI28"/>
     <mergeCell ref="B30:AA30"/>
@@ -47548,11 +47713,12 @@
     <mergeCell ref="G35:AA35"/>
     <mergeCell ref="G34:AA34"/>
     <mergeCell ref="B14:T28"/>
-    <mergeCell ref="G36:AA36"/>
-    <mergeCell ref="G67:R67"/>
-    <mergeCell ref="I179:BC179"/>
-    <mergeCell ref="I144:AU144"/>
-    <mergeCell ref="G104:AF104"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="Y13:AA13"/>
   </mergeCells>
   <conditionalFormatting sqref="Y15:AA26 AE26 AC27:AE39">
     <cfRule type="expression" dxfId="0" priority="16">

</xml_diff>

<commit_message>
My case page became corrupted. I moved the original in. This deleted my work, but that is okay. I learned a lot
</commit_message>
<xml_diff>
--- a/ExcelEsport/FMWC_Examples/What Is My Flight Number - Patrick Chatain - My Work.xlsx
+++ b/ExcelEsport/FMWC_Examples/What Is My Flight Number - Patrick Chatain - My Work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\FMWC_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E80DFA-8F73-4AD8-BD64-3F5C0657BA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D41DCE-8BD3-49C1-94F0-F309F2DF287C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{114A3ACC-2F61-4F50-A5CF-63A86B2334B2}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2086,6 +2086,57 @@
     <xf numFmtId="3" fontId="5" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2154,57 +2205,6 @@
     </xf>
     <xf numFmtId="3" fontId="14" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3345,7 +3345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B840F547-97A4-4023-9D52-57A423820E20}">
   <dimension ref="A1:AZ216"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A123" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -3397,34 +3397,34 @@
       <c r="AZ1" s="6"/>
     </row>
     <row r="2" spans="2:52" ht="60.6" customHeight="1">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="88" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
       <c r="AO2" s="3"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6"/>
@@ -3440,32 +3440,32 @@
       <c r="AZ3" s="6"/>
     </row>
     <row r="4" spans="2:52" ht="33.6" customHeight="1">
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="Y4" s="123" t="s">
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="Y4" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="123"/>
-      <c r="AA4" s="112"/>
+      <c r="Z4" s="100"/>
+      <c r="AA4" s="89"/>
       <c r="AO4" s="3"/>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -3665,11 +3665,11 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
       <c r="X11" s="31"/>
-      <c r="Y11" s="124" t="s">
+      <c r="Y11" s="101" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="125"/>
-      <c r="AA11" s="126"/>
+      <c r="Z11" s="102"/>
+      <c r="AA11" s="103"/>
       <c r="AO11" s="3"/>
       <c r="AY11" s="6"/>
       <c r="AZ11" s="6"/>
@@ -3704,33 +3704,33 @@
       <c r="AZ12" s="6"/>
     </row>
     <row r="13" spans="2:52" ht="24.9" customHeight="1" thickBot="1">
-      <c r="B13" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-      <c r="N13" s="112"/>
-      <c r="O13" s="112"/>
-      <c r="P13" s="112"/>
-      <c r="Q13" s="112"/>
-      <c r="R13" s="112"/>
-      <c r="S13" s="112"/>
-      <c r="T13" s="112"/>
+      <c r="B13" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
       <c r="U13" s="60"/>
-      <c r="Y13" s="113" t="s">
+      <c r="Y13" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="Z13" s="112"/>
-      <c r="AA13" s="112"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
       <c r="AF13" s="60"/>
       <c r="AG13" s="60"/>
       <c r="AH13" s="60"/>
@@ -3738,27 +3738,27 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:52" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="114" t="s">
+      <c r="B14" s="91" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="115"/>
-      <c r="D14" s="115"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="115"/>
-      <c r="H14" s="115"/>
-      <c r="I14" s="115"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="115"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
-      <c r="N14" s="115"/>
-      <c r="O14" s="115"/>
-      <c r="P14" s="115"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="115"/>
-      <c r="S14" s="115"/>
-      <c r="T14" s="116"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="92"/>
+      <c r="Q14" s="92"/>
+      <c r="R14" s="92"/>
+      <c r="S14" s="92"/>
+      <c r="T14" s="93"/>
       <c r="U14" s="3"/>
       <c r="Y14" s="61" t="s">
         <v>31</v>
@@ -3775,25 +3775,25 @@
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:52" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B15" s="117"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-      <c r="S15" s="118"/>
-      <c r="T15" s="119"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95"/>
+      <c r="Q15" s="95"/>
+      <c r="R15" s="95"/>
+      <c r="S15" s="95"/>
+      <c r="T15" s="96"/>
       <c r="U15" s="3"/>
       <c r="Y15" s="62" t="s">
         <v>32</v>
@@ -3813,25 +3813,25 @@
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B16" s="117"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-      <c r="S16" s="118"/>
-      <c r="T16" s="119"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="95"/>
+      <c r="L16" s="95"/>
+      <c r="M16" s="95"/>
+      <c r="N16" s="95"/>
+      <c r="O16" s="95"/>
+      <c r="P16" s="95"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="95"/>
+      <c r="T16" s="96"/>
       <c r="U16" s="3"/>
       <c r="Y16" s="62" t="s">
         <v>47</v>
@@ -3850,25 +3850,25 @@
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="119"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="95"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="95"/>
+      <c r="T17" s="96"/>
       <c r="U17" s="3"/>
       <c r="Y17" s="62" t="s">
         <v>39</v>
@@ -3887,25 +3887,25 @@
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B18" s="117"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="118"/>
-      <c r="K18" s="118"/>
-      <c r="L18" s="118"/>
-      <c r="M18" s="118"/>
-      <c r="N18" s="118"/>
-      <c r="O18" s="118"/>
-      <c r="P18" s="118"/>
-      <c r="Q18" s="118"/>
-      <c r="R18" s="118"/>
-      <c r="S18" s="118"/>
-      <c r="T18" s="119"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="95"/>
+      <c r="M18" s="95"/>
+      <c r="N18" s="95"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="95"/>
+      <c r="R18" s="95"/>
+      <c r="S18" s="95"/>
+      <c r="T18" s="96"/>
       <c r="U18" s="3"/>
       <c r="Y18" s="62" t="s">
         <v>35</v>
@@ -3924,25 +3924,25 @@
       <c r="AO18" s="3"/>
     </row>
     <row r="19" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B19" s="117"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="118"/>
-      <c r="K19" s="118"/>
-      <c r="L19" s="118"/>
-      <c r="M19" s="118"/>
-      <c r="N19" s="118"/>
-      <c r="O19" s="118"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="118"/>
-      <c r="R19" s="118"/>
-      <c r="S19" s="118"/>
-      <c r="T19" s="119"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="95"/>
+      <c r="T19" s="96"/>
       <c r="U19" s="3"/>
       <c r="Y19" s="62" t="s">
         <v>42</v>
@@ -3961,25 +3961,25 @@
       <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="118"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118"/>
-      <c r="O20" s="118"/>
-      <c r="P20" s="118"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="118"/>
-      <c r="S20" s="118"/>
-      <c r="T20" s="119"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
+      <c r="R20" s="95"/>
+      <c r="S20" s="95"/>
+      <c r="T20" s="96"/>
       <c r="U20" s="3"/>
       <c r="Y20" s="62" t="s">
         <v>48</v>
@@ -3996,25 +3996,25 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B21" s="117"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="118"/>
-      <c r="S21" s="118"/>
-      <c r="T21" s="119"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
+      <c r="S21" s="95"/>
+      <c r="T21" s="96"/>
       <c r="U21" s="3"/>
       <c r="Y21" s="62" t="s">
         <v>49</v>
@@ -4033,25 +4033,25 @@
       <c r="AO21" s="3"/>
     </row>
     <row r="22" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B22" s="117"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
-      <c r="P22" s="118"/>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="118"/>
-      <c r="S22" s="118"/>
-      <c r="T22" s="119"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="95"/>
+      <c r="L22" s="95"/>
+      <c r="M22" s="95"/>
+      <c r="N22" s="95"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="95"/>
+      <c r="Q22" s="95"/>
+      <c r="R22" s="95"/>
+      <c r="S22" s="95"/>
+      <c r="T22" s="96"/>
       <c r="U22" s="3"/>
       <c r="Y22" s="62" t="s">
         <v>50</v>
@@ -4071,25 +4071,25 @@
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="118"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="118"/>
-      <c r="S23" s="118"/>
-      <c r="T23" s="119"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="95"/>
+      <c r="K23" s="95"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="95"/>
+      <c r="Q23" s="95"/>
+      <c r="R23" s="95"/>
+      <c r="S23" s="95"/>
+      <c r="T23" s="96"/>
       <c r="U23" s="3"/>
       <c r="Y23" s="62" t="s">
         <v>51</v>
@@ -4109,25 +4109,25 @@
       <c r="AP23" s="3"/>
     </row>
     <row r="24" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B24" s="117"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="118"/>
-      <c r="P24" s="118"/>
-      <c r="Q24" s="118"/>
-      <c r="R24" s="118"/>
-      <c r="S24" s="118"/>
-      <c r="T24" s="119"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="95"/>
+      <c r="K24" s="95"/>
+      <c r="L24" s="95"/>
+      <c r="M24" s="95"/>
+      <c r="N24" s="95"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="95"/>
+      <c r="T24" s="96"/>
       <c r="U24" s="3"/>
       <c r="Y24" s="62" t="s">
         <v>52</v>
@@ -4147,25 +4147,25 @@
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="118"/>
-      <c r="S25" s="118"/>
-      <c r="T25" s="119"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="95"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="95"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="95"/>
+      <c r="S25" s="95"/>
+      <c r="T25" s="96"/>
       <c r="U25" s="3"/>
       <c r="Y25" s="62" t="s">
         <v>53</v>
@@ -4183,25 +4183,25 @@
       <c r="AP25" s="3"/>
     </row>
     <row r="26" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="118"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
-      <c r="O26" s="118"/>
-      <c r="P26" s="118"/>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="118"/>
-      <c r="S26" s="118"/>
-      <c r="T26" s="119"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="95"/>
+      <c r="M26" s="95"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="95"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="95"/>
+      <c r="S26" s="95"/>
+      <c r="T26" s="96"/>
       <c r="U26" s="3"/>
       <c r="Y26" s="62" t="s">
         <v>105</v>
@@ -4224,25 +4224,25 @@
       <c r="AP26" s="3"/>
     </row>
     <row r="27" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B27" s="117"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
-      <c r="O27" s="118"/>
-      <c r="P27" s="118"/>
-      <c r="Q27" s="118"/>
-      <c r="R27" s="118"/>
-      <c r="S27" s="118"/>
-      <c r="T27" s="119"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="95"/>
+      <c r="M27" s="95"/>
+      <c r="N27" s="95"/>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="95"/>
+      <c r="T27" s="96"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -4261,25 +4261,25 @@
       <c r="AP27" s="3"/>
     </row>
     <row r="28" spans="2:52" ht="47.25" customHeight="1">
-      <c r="B28" s="120"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="121"/>
-      <c r="J28" s="121"/>
-      <c r="K28" s="121"/>
-      <c r="L28" s="121"/>
-      <c r="M28" s="121"/>
-      <c r="N28" s="121"/>
-      <c r="O28" s="121"/>
-      <c r="P28" s="121"/>
-      <c r="Q28" s="121"/>
-      <c r="R28" s="121"/>
-      <c r="S28" s="121"/>
-      <c r="T28" s="122"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
+      <c r="O28" s="98"/>
+      <c r="P28" s="98"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="99"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -4290,10 +4290,10 @@
       <c r="AC28" s="63"/>
       <c r="AD28" s="63"/>
       <c r="AE28" s="64"/>
-      <c r="AF28" s="110"/>
-      <c r="AG28" s="110"/>
-      <c r="AH28" s="110"/>
-      <c r="AI28" s="110"/>
+      <c r="AF28" s="87"/>
+      <c r="AG28" s="87"/>
+      <c r="AH28" s="87"/>
+      <c r="AI28" s="87"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
     </row>
@@ -4338,34 +4338,34 @@
       <c r="AZ29" s="6"/>
     </row>
     <row r="30" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="91"/>
-      <c r="N30" s="91"/>
-      <c r="O30" s="91"/>
-      <c r="P30" s="91"/>
-      <c r="Q30" s="91"/>
-      <c r="R30" s="91"/>
-      <c r="S30" s="91"/>
-      <c r="T30" s="91"/>
-      <c r="U30" s="91"/>
-      <c r="V30" s="91"/>
-      <c r="W30" s="91"/>
-      <c r="X30" s="91"/>
-      <c r="Y30" s="91"/>
-      <c r="Z30" s="91"/>
-      <c r="AA30" s="92"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="108"/>
+      <c r="L30" s="108"/>
+      <c r="M30" s="108"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="108"/>
+      <c r="T30" s="108"/>
+      <c r="U30" s="108"/>
+      <c r="V30" s="108"/>
+      <c r="W30" s="108"/>
+      <c r="X30" s="108"/>
+      <c r="Y30" s="108"/>
+      <c r="Z30" s="108"/>
+      <c r="AA30" s="109"/>
       <c r="AC30" s="63"/>
       <c r="AD30" s="63"/>
       <c r="AE30" s="64"/>
@@ -4416,29 +4416,29 @@
       <c r="E33" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="93" t="s">
+      <c r="G33" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="94"/>
-      <c r="O33" s="94"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="94"/>
-      <c r="R33" s="94"/>
-      <c r="S33" s="94"/>
-      <c r="T33" s="94"/>
-      <c r="U33" s="94"/>
-      <c r="V33" s="94"/>
-      <c r="W33" s="94"/>
-      <c r="X33" s="94"/>
-      <c r="Y33" s="94"/>
-      <c r="Z33" s="94"/>
-      <c r="AA33" s="95"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="111"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="111"/>
+      <c r="O33" s="111"/>
+      <c r="P33" s="111"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="111"/>
+      <c r="S33" s="111"/>
+      <c r="T33" s="111"/>
+      <c r="U33" s="111"/>
+      <c r="V33" s="111"/>
+      <c r="W33" s="111"/>
+      <c r="X33" s="111"/>
+      <c r="Y33" s="111"/>
+      <c r="Z33" s="111"/>
+      <c r="AA33" s="112"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="63"/>
       <c r="AE33" s="64"/>
@@ -4458,29 +4458,29 @@
         <f>IF(AND(E34&lt;&gt;"",E34=[1]Answers!E34),1,IF(ISBLANK(E34),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G34" s="96" t="s">
+      <c r="G34" s="113" t="s">
         <v>308</v>
       </c>
-      <c r="H34" s="97"/>
-      <c r="I34" s="97"/>
-      <c r="J34" s="97"/>
-      <c r="K34" s="97"/>
-      <c r="L34" s="97"/>
-      <c r="M34" s="97"/>
-      <c r="N34" s="97"/>
-      <c r="O34" s="97"/>
-      <c r="P34" s="97"/>
-      <c r="Q34" s="97"/>
-      <c r="R34" s="97"/>
-      <c r="S34" s="97"/>
-      <c r="T34" s="97"/>
-      <c r="U34" s="97"/>
-      <c r="V34" s="97"/>
-      <c r="W34" s="97"/>
-      <c r="X34" s="97"/>
-      <c r="Y34" s="97"/>
-      <c r="Z34" s="97"/>
-      <c r="AA34" s="98"/>
+      <c r="H34" s="114"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="114"/>
+      <c r="K34" s="114"/>
+      <c r="L34" s="114"/>
+      <c r="M34" s="114"/>
+      <c r="N34" s="114"/>
+      <c r="O34" s="114"/>
+      <c r="P34" s="114"/>
+      <c r="Q34" s="114"/>
+      <c r="R34" s="114"/>
+      <c r="S34" s="114"/>
+      <c r="T34" s="114"/>
+      <c r="U34" s="114"/>
+      <c r="V34" s="114"/>
+      <c r="W34" s="114"/>
+      <c r="X34" s="114"/>
+      <c r="Y34" s="114"/>
+      <c r="Z34" s="114"/>
+      <c r="AA34" s="115"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="63"/>
       <c r="AE34" s="64"/>
@@ -4500,29 +4500,29 @@
         <f>IF(AND(E35&lt;&gt;"",E35=[1]Answers!E35),1,IF(ISBLANK(E35),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G35" s="99" t="s">
+      <c r="G35" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="100"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="100"/>
-      <c r="N35" s="100"/>
-      <c r="O35" s="100"/>
-      <c r="P35" s="100"/>
-      <c r="Q35" s="100"/>
-      <c r="R35" s="100"/>
-      <c r="S35" s="100"/>
-      <c r="T35" s="100"/>
-      <c r="U35" s="100"/>
-      <c r="V35" s="100"/>
-      <c r="W35" s="100"/>
-      <c r="X35" s="100"/>
-      <c r="Y35" s="100"/>
-      <c r="Z35" s="100"/>
-      <c r="AA35" s="101"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="117"/>
+      <c r="N35" s="117"/>
+      <c r="O35" s="117"/>
+      <c r="P35" s="117"/>
+      <c r="Q35" s="117"/>
+      <c r="R35" s="117"/>
+      <c r="S35" s="117"/>
+      <c r="T35" s="117"/>
+      <c r="U35" s="117"/>
+      <c r="V35" s="117"/>
+      <c r="W35" s="117"/>
+      <c r="X35" s="117"/>
+      <c r="Y35" s="117"/>
+      <c r="Z35" s="117"/>
+      <c r="AA35" s="118"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="63"/>
       <c r="AE35" s="64"/>
@@ -4542,29 +4542,29 @@
         <f>IF(AND(E36&lt;&gt;"",E36=[1]Answers!E36),1,IF(ISBLANK(E36),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G36" s="102" t="s">
+      <c r="G36" s="119" t="s">
         <v>309</v>
       </c>
-      <c r="H36" s="103"/>
-      <c r="I36" s="103"/>
-      <c r="J36" s="103"/>
-      <c r="K36" s="103"/>
-      <c r="L36" s="103"/>
-      <c r="M36" s="103"/>
-      <c r="N36" s="103"/>
-      <c r="O36" s="103"/>
-      <c r="P36" s="103"/>
-      <c r="Q36" s="103"/>
-      <c r="R36" s="103"/>
-      <c r="S36" s="103"/>
-      <c r="T36" s="103"/>
-      <c r="U36" s="103"/>
-      <c r="V36" s="103"/>
-      <c r="W36" s="103"/>
-      <c r="X36" s="103"/>
-      <c r="Y36" s="103"/>
-      <c r="Z36" s="103"/>
-      <c r="AA36" s="104"/>
+      <c r="H36" s="120"/>
+      <c r="I36" s="120"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="120"/>
+      <c r="N36" s="120"/>
+      <c r="O36" s="120"/>
+      <c r="P36" s="120"/>
+      <c r="Q36" s="120"/>
+      <c r="R36" s="120"/>
+      <c r="S36" s="120"/>
+      <c r="T36" s="120"/>
+      <c r="U36" s="120"/>
+      <c r="V36" s="120"/>
+      <c r="W36" s="120"/>
+      <c r="X36" s="120"/>
+      <c r="Y36" s="120"/>
+      <c r="Z36" s="120"/>
+      <c r="AA36" s="121"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="63"/>
       <c r="AE36" s="64"/>
@@ -4667,13 +4667,13 @@
       <c r="C41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="106" t="s">
+      <c r="J41" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="K41" s="106"/>
-      <c r="L41" s="106"/>
-      <c r="M41" s="106"/>
-      <c r="N41" s="106"/>
+      <c r="K41" s="123"/>
+      <c r="L41" s="123"/>
+      <c r="M41" s="123"/>
+      <c r="N41" s="123"/>
       <c r="AS41" s="6"/>
       <c r="AT41" s="6"/>
       <c r="AU41" s="6"/>
@@ -4684,14 +4684,14 @@
       <c r="AZ41" s="6"/>
     </row>
     <row r="42" spans="2:52" ht="15" customHeight="1" thickTop="1">
-      <c r="J42" s="105" cm="1">
+      <c r="J42" s="122" cm="1">
         <f t="array" ref="J42">SUMPRODUCT(--(F34:F216=1),F34:F216,D34:D216)</f>
         <v>420</v>
       </c>
-      <c r="K42" s="105"/>
-      <c r="L42" s="105"/>
-      <c r="M42" s="105"/>
-      <c r="N42" s="105"/>
+      <c r="K42" s="122"/>
+      <c r="L42" s="122"/>
+      <c r="M42" s="122"/>
+      <c r="N42" s="122"/>
       <c r="AS42" s="6"/>
       <c r="AT42" s="6"/>
       <c r="AU42" s="6"/>
@@ -4705,11 +4705,11 @@
       <c r="B43" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="J43" s="105"/>
-      <c r="K43" s="105"/>
-      <c r="L43" s="105"/>
-      <c r="M43" s="105"/>
-      <c r="N43" s="105"/>
+      <c r="J43" s="122"/>
+      <c r="K43" s="122"/>
+      <c r="L43" s="122"/>
+      <c r="M43" s="122"/>
+      <c r="N43" s="122"/>
       <c r="AS43" s="6"/>
       <c r="AT43" s="6"/>
       <c r="AU43" s="6"/>
@@ -4722,11 +4722,11 @@
     <row r="44" spans="2:52" ht="15" customHeight="1" thickBot="1">
       <c r="B44" s="20"/>
       <c r="G44" s="27"/>
-      <c r="J44" s="105"/>
-      <c r="K44" s="105"/>
-      <c r="L44" s="105"/>
-      <c r="M44" s="105"/>
-      <c r="N44" s="105"/>
+      <c r="J44" s="122"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="122"/>
+      <c r="M44" s="122"/>
+      <c r="N44" s="122"/>
       <c r="R44" s="6"/>
     </row>
     <row r="45" spans="2:52" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
@@ -4747,11 +4747,11 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="105"/>
-      <c r="L45" s="105"/>
-      <c r="M45" s="105"/>
-      <c r="N45" s="105"/>
+      <c r="J45" s="122"/>
+      <c r="K45" s="122"/>
+      <c r="L45" s="122"/>
+      <c r="M45" s="122"/>
+      <c r="N45" s="122"/>
       <c r="R45" s="6"/>
       <c r="AB45" s="6"/>
       <c r="AC45" s="6"/>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G47,"-"),_nCode,_nCity)</f>
+        <f t="shared" ref="I47:I58" si="0">_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G47,"-"),_nCode,_nCity)</f>
         <v>Toronto</v>
       </c>
       <c r="R47" s="6"/>
@@ -4890,7 +4890,7 @@
       <c r="E48" s="39"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6" t="e">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G48,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="R48" s="6"/>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G49,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Lisbon</v>
       </c>
       <c r="R49" s="6"/>
@@ -4992,7 +4992,7 @@
     </row>
     <row r="50" spans="2:52" ht="23.4">
       <c r="B50" s="17">
-        <f t="shared" ref="B50:B58" si="0">B49+1</f>
+        <f t="shared" ref="B50:B58" si="1">B49+1</f>
         <v>2</v>
       </c>
       <c r="C50" s="17">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G50,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Los Angeles</v>
       </c>
       <c r="J50" s="6"/>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="51" spans="2:52" ht="23.4">
       <c r="B51" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C51" s="17">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G51,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Madrid</v>
       </c>
       <c r="J51" s="6"/>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="52" spans="2:52" ht="23.4">
       <c r="B52" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C52" s="17">
@@ -5151,7 +5151,7 @@
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G52,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>London</v>
       </c>
       <c r="J52" s="6"/>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="53" spans="2:52" ht="23.4">
       <c r="B53" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C53" s="17">
@@ -5220,7 +5220,7 @@
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G53,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Montreal</v>
       </c>
       <c r="J53" s="6"/>
@@ -5268,7 +5268,7 @@
     </row>
     <row r="54" spans="2:52" ht="23.4">
       <c r="B54" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C54" s="17">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G54,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Bogota</v>
       </c>
       <c r="J54" s="6"/>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="55" spans="2:52" ht="23.4">
       <c r="B55" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C55" s="17">
@@ -5358,7 +5358,7 @@
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G55,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Buenos Aires</v>
       </c>
       <c r="J55" s="6"/>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="56" spans="2:52" ht="23.4">
       <c r="B56" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C56" s="17">
@@ -5427,7 +5427,7 @@
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G56,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Cape Town</v>
       </c>
       <c r="J56" s="6"/>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="57" spans="2:52" ht="23.4">
       <c r="B57" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C57" s="17">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G57,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Lisbon</v>
       </c>
       <c r="J57" s="6"/>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="58" spans="2:52" ht="23.4">
       <c r="B58" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C58" s="17">
@@ -5565,7 +5565,7 @@
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6" t="str">
-        <f>_xlfn.XLOOKUP(_xlfn.TEXTBEFORE(G58,"-"),_nCode,_nCity)</f>
+        <f t="shared" si="0"/>
         <v>Buenos Aires</v>
       </c>
       <c r="J58" s="6"/>
@@ -5904,20 +5904,20 @@
       <c r="E67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="93" t="s">
+      <c r="G67" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="H67" s="94"/>
-      <c r="I67" s="94"/>
-      <c r="J67" s="94"/>
-      <c r="K67" s="94"/>
-      <c r="L67" s="94"/>
-      <c r="M67" s="94"/>
-      <c r="N67" s="94"/>
-      <c r="O67" s="94"/>
-      <c r="P67" s="94"/>
-      <c r="Q67" s="94"/>
-      <c r="R67" s="95"/>
+      <c r="H67" s="111"/>
+      <c r="I67" s="111"/>
+      <c r="J67" s="111"/>
+      <c r="K67" s="111"/>
+      <c r="L67" s="111"/>
+      <c r="M67" s="111"/>
+      <c r="N67" s="111"/>
+      <c r="O67" s="111"/>
+      <c r="P67" s="111"/>
+      <c r="Q67" s="111"/>
+      <c r="R67" s="112"/>
       <c r="S67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -6125,7 +6125,7 @@
     </row>
     <row r="72" spans="2:52" ht="25.5" customHeight="1">
       <c r="B72" s="17">
-        <f t="shared" ref="B72:B90" si="1">B71+1</f>
+        <f t="shared" ref="B72:B90" si="2">B71+1</f>
         <v>12</v>
       </c>
       <c r="C72" s="17">
@@ -6178,7 +6178,7 @@
     </row>
     <row r="73" spans="2:52" ht="25.5" customHeight="1">
       <c r="B73" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C73" s="17">
@@ -6230,7 +6230,7 @@
     </row>
     <row r="74" spans="2:52" ht="25.5" customHeight="1">
       <c r="B74" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C74" s="17">
@@ -6282,7 +6282,7 @@
     </row>
     <row r="75" spans="2:52" ht="25.5" customHeight="1">
       <c r="B75" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C75" s="17">
@@ -6352,7 +6352,7 @@
     </row>
     <row r="76" spans="2:52" ht="25.5" customHeight="1">
       <c r="B76" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C76" s="17">
@@ -6421,7 +6421,7 @@
     </row>
     <row r="77" spans="2:52" ht="25.5" customHeight="1">
       <c r="B77" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C77" s="17">
@@ -6491,7 +6491,7 @@
     </row>
     <row r="78" spans="2:52" ht="25.5" customHeight="1">
       <c r="B78" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C78" s="17">
@@ -6561,7 +6561,7 @@
     </row>
     <row r="79" spans="2:52" ht="25.5" customHeight="1">
       <c r="B79" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C79" s="17">
@@ -6631,7 +6631,7 @@
     </row>
     <row r="80" spans="2:52" ht="25.5" customHeight="1">
       <c r="B80" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C80" s="17">
@@ -6701,7 +6701,7 @@
     </row>
     <row r="81" spans="2:52" ht="25.5" customHeight="1">
       <c r="B81" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C81" s="17">
@@ -6771,7 +6771,7 @@
     </row>
     <row r="82" spans="2:52" ht="25.5" customHeight="1">
       <c r="B82" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C82" s="17">
@@ -6841,7 +6841,7 @@
     </row>
     <row r="83" spans="2:52" ht="25.5" customHeight="1">
       <c r="B83" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C83" s="17">
@@ -6911,7 +6911,7 @@
     </row>
     <row r="84" spans="2:52" ht="25.5" customHeight="1">
       <c r="B84" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C84" s="17">
@@ -6981,7 +6981,7 @@
     </row>
     <row r="85" spans="2:52" ht="25.5" customHeight="1">
       <c r="B85" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C85" s="17">
@@ -7051,7 +7051,7 @@
     </row>
     <row r="86" spans="2:52" ht="25.5" customHeight="1">
       <c r="B86" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C86" s="17">
@@ -7121,7 +7121,7 @@
     </row>
     <row r="87" spans="2:52" ht="25.5" customHeight="1">
       <c r="B87" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C87" s="17">
@@ -7191,7 +7191,7 @@
     </row>
     <row r="88" spans="2:52" ht="25.5" customHeight="1">
       <c r="B88" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C88" s="17">
@@ -7261,7 +7261,7 @@
     </row>
     <row r="89" spans="2:52" ht="25.5" customHeight="1">
       <c r="B89" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C89" s="17">
@@ -7331,7 +7331,7 @@
     </row>
     <row r="90" spans="2:52" ht="25.5" customHeight="1">
       <c r="B90" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C90" s="17">
@@ -7964,35 +7964,35 @@
         <v>4</v>
       </c>
       <c r="E104" s="44"/>
-      <c r="G104" s="107" t="s">
+      <c r="G104" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="H104" s="108"/>
-      <c r="I104" s="108"/>
-      <c r="J104" s="108"/>
-      <c r="K104" s="108"/>
-      <c r="L104" s="108"/>
-      <c r="M104" s="108"/>
-      <c r="N104" s="108"/>
-      <c r="O104" s="108"/>
-      <c r="P104" s="108"/>
-      <c r="Q104" s="108"/>
-      <c r="R104" s="108"/>
-      <c r="S104" s="108"/>
-      <c r="T104" s="108"/>
-      <c r="U104" s="108"/>
-      <c r="V104" s="108"/>
-      <c r="W104" s="108"/>
-      <c r="X104" s="108"/>
-      <c r="Y104" s="108"/>
-      <c r="Z104" s="108"/>
-      <c r="AA104" s="108"/>
-      <c r="AB104" s="108"/>
-      <c r="AC104" s="108"/>
-      <c r="AD104" s="108"/>
-      <c r="AE104" s="108"/>
-      <c r="AF104" s="108"/>
-      <c r="AG104" s="109"/>
+      <c r="H104" s="125"/>
+      <c r="I104" s="125"/>
+      <c r="J104" s="125"/>
+      <c r="K104" s="125"/>
+      <c r="L104" s="125"/>
+      <c r="M104" s="125"/>
+      <c r="N104" s="125"/>
+      <c r="O104" s="125"/>
+      <c r="P104" s="125"/>
+      <c r="Q104" s="125"/>
+      <c r="R104" s="125"/>
+      <c r="S104" s="125"/>
+      <c r="T104" s="125"/>
+      <c r="U104" s="125"/>
+      <c r="V104" s="125"/>
+      <c r="W104" s="125"/>
+      <c r="X104" s="125"/>
+      <c r="Y104" s="125"/>
+      <c r="Z104" s="125"/>
+      <c r="AA104" s="125"/>
+      <c r="AB104" s="125"/>
+      <c r="AC104" s="125"/>
+      <c r="AD104" s="125"/>
+      <c r="AE104" s="125"/>
+      <c r="AF104" s="125"/>
+      <c r="AG104" s="126"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
       <c r="AJ104" s="6"/>
@@ -8172,7 +8172,7 @@
     </row>
     <row r="109" spans="2:52" ht="23.4">
       <c r="B109" s="17">
-        <f t="shared" ref="B109:B127" si="2">B108+1</f>
+        <f t="shared" ref="B109:B127" si="3">B108+1</f>
         <v>32</v>
       </c>
       <c r="C109" s="17">
@@ -8220,7 +8220,7 @@
     </row>
     <row r="110" spans="2:52" ht="23.4">
       <c r="B110" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="C110" s="17">
@@ -8268,7 +8268,7 @@
     </row>
     <row r="111" spans="2:52" ht="23.4">
       <c r="B111" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="C111" s="17">
@@ -8316,7 +8316,7 @@
     </row>
     <row r="112" spans="2:52" ht="23.4">
       <c r="B112" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="C112" s="17">
@@ -8364,7 +8364,7 @@
     </row>
     <row r="113" spans="2:33" ht="23.4">
       <c r="B113" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="C113" s="17">
@@ -8412,7 +8412,7 @@
     </row>
     <row r="114" spans="2:33" ht="23.4">
       <c r="B114" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="C114" s="17">
@@ -8460,7 +8460,7 @@
     </row>
     <row r="115" spans="2:33" ht="23.4">
       <c r="B115" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="C115" s="17">
@@ -8508,7 +8508,7 @@
     </row>
     <row r="116" spans="2:33" ht="23.4">
       <c r="B116" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="C116" s="17">
@@ -8556,7 +8556,7 @@
     </row>
     <row r="117" spans="2:33" ht="23.4">
       <c r="B117" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="C117" s="17">
@@ -8604,7 +8604,7 @@
     </row>
     <row r="118" spans="2:33" ht="23.4">
       <c r="B118" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="C118" s="17">
@@ -8652,7 +8652,7 @@
     </row>
     <row r="119" spans="2:33" ht="23.4">
       <c r="B119" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="C119" s="17">
@@ -8700,7 +8700,7 @@
     </row>
     <row r="120" spans="2:33" ht="23.4">
       <c r="B120" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="C120" s="17">
@@ -8748,7 +8748,7 @@
     </row>
     <row r="121" spans="2:33" ht="23.4">
       <c r="B121" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="C121" s="17">
@@ -8796,7 +8796,7 @@
     </row>
     <row r="122" spans="2:33" ht="23.4">
       <c r="B122" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="C122" s="17">
@@ -8844,7 +8844,7 @@
     </row>
     <row r="123" spans="2:33" ht="23.4">
       <c r="B123" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="C123" s="17">
@@ -8892,7 +8892,7 @@
     </row>
     <row r="124" spans="2:33" ht="23.4">
       <c r="B124" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="C124" s="17">
@@ -8940,7 +8940,7 @@
     </row>
     <row r="125" spans="2:33" ht="23.4">
       <c r="B125" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="C125" s="17">
@@ -8988,7 +8988,7 @@
     </row>
     <row r="126" spans="2:33" ht="23.4">
       <c r="B126" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="C126" s="17">
@@ -9036,7 +9036,7 @@
     </row>
     <row r="127" spans="2:33" ht="23.4">
       <c r="B127" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="C127" s="17">
@@ -9668,48 +9668,48 @@
       <c r="G144" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I144" s="87" t="s">
+      <c r="I144" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="J144" s="88"/>
-      <c r="K144" s="88"/>
-      <c r="L144" s="88"/>
-      <c r="M144" s="88"/>
-      <c r="N144" s="88"/>
-      <c r="O144" s="88"/>
-      <c r="P144" s="88"/>
-      <c r="Q144" s="88"/>
-      <c r="R144" s="88"/>
-      <c r="S144" s="88"/>
-      <c r="T144" s="88"/>
-      <c r="U144" s="88"/>
-      <c r="V144" s="88"/>
-      <c r="W144" s="88"/>
-      <c r="X144" s="88"/>
-      <c r="Y144" s="88"/>
-      <c r="Z144" s="88"/>
-      <c r="AA144" s="88"/>
-      <c r="AB144" s="88"/>
-      <c r="AC144" s="88"/>
-      <c r="AD144" s="88"/>
-      <c r="AE144" s="88"/>
-      <c r="AF144" s="88"/>
-      <c r="AG144" s="88"/>
-      <c r="AH144" s="88"/>
-      <c r="AI144" s="88"/>
-      <c r="AJ144" s="88"/>
-      <c r="AK144" s="88"/>
-      <c r="AL144" s="88"/>
-      <c r="AM144" s="88"/>
-      <c r="AN144" s="88"/>
-      <c r="AO144" s="88"/>
-      <c r="AP144" s="88"/>
-      <c r="AQ144" s="88"/>
-      <c r="AR144" s="88"/>
-      <c r="AS144" s="88"/>
-      <c r="AT144" s="88"/>
-      <c r="AU144" s="88"/>
-      <c r="AV144" s="89"/>
+      <c r="J144" s="105"/>
+      <c r="K144" s="105"/>
+      <c r="L144" s="105"/>
+      <c r="M144" s="105"/>
+      <c r="N144" s="105"/>
+      <c r="O144" s="105"/>
+      <c r="P144" s="105"/>
+      <c r="Q144" s="105"/>
+      <c r="R144" s="105"/>
+      <c r="S144" s="105"/>
+      <c r="T144" s="105"/>
+      <c r="U144" s="105"/>
+      <c r="V144" s="105"/>
+      <c r="W144" s="105"/>
+      <c r="X144" s="105"/>
+      <c r="Y144" s="105"/>
+      <c r="Z144" s="105"/>
+      <c r="AA144" s="105"/>
+      <c r="AB144" s="105"/>
+      <c r="AC144" s="105"/>
+      <c r="AD144" s="105"/>
+      <c r="AE144" s="105"/>
+      <c r="AF144" s="105"/>
+      <c r="AG144" s="105"/>
+      <c r="AH144" s="105"/>
+      <c r="AI144" s="105"/>
+      <c r="AJ144" s="105"/>
+      <c r="AK144" s="105"/>
+      <c r="AL144" s="105"/>
+      <c r="AM144" s="105"/>
+      <c r="AN144" s="105"/>
+      <c r="AO144" s="105"/>
+      <c r="AP144" s="105"/>
+      <c r="AQ144" s="105"/>
+      <c r="AR144" s="105"/>
+      <c r="AS144" s="105"/>
+      <c r="AT144" s="105"/>
+      <c r="AU144" s="105"/>
+      <c r="AV144" s="106"/>
       <c r="AW144" s="6"/>
       <c r="AX144" s="6"/>
       <c r="AY144" s="6"/>
@@ -9921,7 +9921,7 @@
     </row>
     <row r="149" spans="2:52" ht="23.4">
       <c r="B149" s="17">
-        <f t="shared" ref="B149:B167" si="3">B148+1</f>
+        <f t="shared" ref="B149:B167" si="4">B148+1</f>
         <v>52</v>
       </c>
       <c r="C149" s="17">
@@ -9984,7 +9984,7 @@
     </row>
     <row r="150" spans="2:52" ht="23.4">
       <c r="B150" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="C150" s="17">
@@ -10047,7 +10047,7 @@
     </row>
     <row r="151" spans="2:52" ht="23.4">
       <c r="B151" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="C151" s="17">
@@ -10110,7 +10110,7 @@
     </row>
     <row r="152" spans="2:52" ht="23.4">
       <c r="B152" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="C152" s="17">
@@ -10173,7 +10173,7 @@
     </row>
     <row r="153" spans="2:52" ht="23.4">
       <c r="B153" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="C153" s="17">
@@ -10236,7 +10236,7 @@
     </row>
     <row r="154" spans="2:52" ht="23.4">
       <c r="B154" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="C154" s="17">
@@ -10299,7 +10299,7 @@
     </row>
     <row r="155" spans="2:52" ht="23.4">
       <c r="B155" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="C155" s="17">
@@ -10362,7 +10362,7 @@
     </row>
     <row r="156" spans="2:52" ht="23.4">
       <c r="B156" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
       <c r="C156" s="17">
@@ -10425,7 +10425,7 @@
     </row>
     <row r="157" spans="2:52" ht="23.4">
       <c r="B157" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="C157" s="17">
@@ -10488,7 +10488,7 @@
     </row>
     <row r="158" spans="2:52" ht="23.4">
       <c r="B158" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="C158" s="17">
@@ -10551,7 +10551,7 @@
     </row>
     <row r="159" spans="2:52" ht="23.4">
       <c r="B159" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="C159" s="17">
@@ -10614,7 +10614,7 @@
     </row>
     <row r="160" spans="2:52" ht="23.4">
       <c r="B160" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="C160" s="17">
@@ -10677,7 +10677,7 @@
     </row>
     <row r="161" spans="2:48" ht="23.4">
       <c r="B161" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="C161" s="17">
@@ -10740,7 +10740,7 @@
     </row>
     <row r="162" spans="2:48" ht="23.4">
       <c r="B162" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="C162" s="17">
@@ -10803,7 +10803,7 @@
     </row>
     <row r="163" spans="2:48" ht="23.4">
       <c r="B163" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="C163" s="17">
@@ -10866,7 +10866,7 @@
     </row>
     <row r="164" spans="2:48" ht="23.4">
       <c r="B164" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="C164" s="17">
@@ -10929,7 +10929,7 @@
     </row>
     <row r="165" spans="2:48" ht="23.4">
       <c r="B165" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68</v>
       </c>
       <c r="C165" s="17">
@@ -10992,7 +10992,7 @@
     </row>
     <row r="166" spans="2:48" ht="23.4">
       <c r="B166" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="C166" s="17">
@@ -11055,7 +11055,7 @@
     </row>
     <row r="167" spans="2:48" ht="23.4">
       <c r="B167" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C167" s="17">
@@ -11300,52 +11300,52 @@
       <c r="G179" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I179" s="87" t="s">
+      <c r="I179" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="J179" s="88"/>
-      <c r="K179" s="88"/>
-      <c r="L179" s="88"/>
-      <c r="M179" s="88"/>
-      <c r="N179" s="88"/>
-      <c r="O179" s="88"/>
-      <c r="P179" s="88"/>
-      <c r="Q179" s="88"/>
-      <c r="R179" s="88"/>
-      <c r="S179" s="88"/>
-      <c r="T179" s="88"/>
-      <c r="U179" s="88"/>
-      <c r="V179" s="88"/>
-      <c r="W179" s="88"/>
-      <c r="X179" s="88"/>
-      <c r="Y179" s="88"/>
-      <c r="Z179" s="88"/>
-      <c r="AA179" s="88"/>
-      <c r="AB179" s="88"/>
-      <c r="AC179" s="88"/>
-      <c r="AD179" s="88"/>
-      <c r="AE179" s="88"/>
-      <c r="AF179" s="88"/>
-      <c r="AG179" s="88"/>
-      <c r="AH179" s="88"/>
-      <c r="AI179" s="88"/>
-      <c r="AJ179" s="88"/>
-      <c r="AK179" s="88"/>
-      <c r="AL179" s="88"/>
-      <c r="AM179" s="88"/>
-      <c r="AN179" s="88"/>
-      <c r="AO179" s="88"/>
-      <c r="AP179" s="88"/>
-      <c r="AQ179" s="88"/>
-      <c r="AR179" s="88"/>
-      <c r="AS179" s="88"/>
-      <c r="AT179" s="88"/>
-      <c r="AU179" s="88"/>
-      <c r="AV179" s="88"/>
-      <c r="AW179" s="88"/>
-      <c r="AX179" s="88"/>
-      <c r="AY179" s="88"/>
-      <c r="AZ179" s="89"/>
+      <c r="J179" s="105"/>
+      <c r="K179" s="105"/>
+      <c r="L179" s="105"/>
+      <c r="M179" s="105"/>
+      <c r="N179" s="105"/>
+      <c r="O179" s="105"/>
+      <c r="P179" s="105"/>
+      <c r="Q179" s="105"/>
+      <c r="R179" s="105"/>
+      <c r="S179" s="105"/>
+      <c r="T179" s="105"/>
+      <c r="U179" s="105"/>
+      <c r="V179" s="105"/>
+      <c r="W179" s="105"/>
+      <c r="X179" s="105"/>
+      <c r="Y179" s="105"/>
+      <c r="Z179" s="105"/>
+      <c r="AA179" s="105"/>
+      <c r="AB179" s="105"/>
+      <c r="AC179" s="105"/>
+      <c r="AD179" s="105"/>
+      <c r="AE179" s="105"/>
+      <c r="AF179" s="105"/>
+      <c r="AG179" s="105"/>
+      <c r="AH179" s="105"/>
+      <c r="AI179" s="105"/>
+      <c r="AJ179" s="105"/>
+      <c r="AK179" s="105"/>
+      <c r="AL179" s="105"/>
+      <c r="AM179" s="105"/>
+      <c r="AN179" s="105"/>
+      <c r="AO179" s="105"/>
+      <c r="AP179" s="105"/>
+      <c r="AQ179" s="105"/>
+      <c r="AR179" s="105"/>
+      <c r="AS179" s="105"/>
+      <c r="AT179" s="105"/>
+      <c r="AU179" s="105"/>
+      <c r="AV179" s="105"/>
+      <c r="AW179" s="105"/>
+      <c r="AX179" s="105"/>
+      <c r="AY179" s="105"/>
+      <c r="AZ179" s="106"/>
     </row>
     <row r="180" spans="2:52" ht="15" thickTop="1">
       <c r="B180" s="1"/>
@@ -11565,7 +11565,7 @@
     </row>
     <row r="184" spans="2:52" ht="23.4">
       <c r="B184" s="17">
-        <f t="shared" ref="B184:B212" si="4">B183+1</f>
+        <f t="shared" ref="B184:B212" si="5">B183+1</f>
         <v>72</v>
       </c>
       <c r="C184" s="17">
@@ -11632,7 +11632,7 @@
     </row>
     <row r="185" spans="2:52" ht="23.4">
       <c r="B185" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73</v>
       </c>
       <c r="C185" s="17">
@@ -11699,7 +11699,7 @@
     </row>
     <row r="186" spans="2:52" ht="23.4">
       <c r="B186" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74</v>
       </c>
       <c r="C186" s="17">
@@ -11766,7 +11766,7 @@
     </row>
     <row r="187" spans="2:52" ht="23.4">
       <c r="B187" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="C187" s="17">
@@ -11833,7 +11833,7 @@
     </row>
     <row r="188" spans="2:52" ht="23.4">
       <c r="B188" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
       <c r="C188" s="17">
@@ -11900,7 +11900,7 @@
     </row>
     <row r="189" spans="2:52" ht="23.4">
       <c r="B189" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
       <c r="C189" s="17">
@@ -11967,7 +11967,7 @@
     </row>
     <row r="190" spans="2:52" ht="23.4">
       <c r="B190" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="C190" s="17">
@@ -12034,7 +12034,7 @@
     </row>
     <row r="191" spans="2:52" ht="23.4">
       <c r="B191" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
       <c r="C191" s="17">
@@ -12101,7 +12101,7 @@
     </row>
     <row r="192" spans="2:52" ht="23.4">
       <c r="B192" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
       <c r="C192" s="17">
@@ -12168,7 +12168,7 @@
     </row>
     <row r="193" spans="2:52" ht="23.4">
       <c r="B193" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
       <c r="C193" s="17">
@@ -12235,7 +12235,7 @@
     </row>
     <row r="194" spans="2:52" ht="23.4">
       <c r="B194" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82</v>
       </c>
       <c r="C194" s="17">
@@ -12302,7 +12302,7 @@
     </row>
     <row r="195" spans="2:52" ht="23.4">
       <c r="B195" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83</v>
       </c>
       <c r="C195" s="17">
@@ -12369,7 +12369,7 @@
     </row>
     <row r="196" spans="2:52" ht="23.4">
       <c r="B196" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
       <c r="C196" s="17">
@@ -12436,7 +12436,7 @@
     </row>
     <row r="197" spans="2:52" ht="23.4">
       <c r="B197" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
       <c r="C197" s="17">
@@ -12503,7 +12503,7 @@
     </row>
     <row r="198" spans="2:52" ht="23.4">
       <c r="B198" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86</v>
       </c>
       <c r="C198" s="17">
@@ -12570,7 +12570,7 @@
     </row>
     <row r="199" spans="2:52" ht="23.4">
       <c r="B199" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
       <c r="C199" s="17">
@@ -12637,7 +12637,7 @@
     </row>
     <row r="200" spans="2:52" ht="23.4">
       <c r="B200" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88</v>
       </c>
       <c r="C200" s="17">
@@ -12704,7 +12704,7 @@
     </row>
     <row r="201" spans="2:52" ht="23.4">
       <c r="B201" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89</v>
       </c>
       <c r="C201" s="17">
@@ -12771,7 +12771,7 @@
     </row>
     <row r="202" spans="2:52" ht="23.4">
       <c r="B202" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="C202" s="17">
@@ -12838,7 +12838,7 @@
     </row>
     <row r="203" spans="2:52" ht="23.4">
       <c r="B203" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
       <c r="C203" s="17">
@@ -12905,7 +12905,7 @@
     </row>
     <row r="204" spans="2:52" ht="23.4">
       <c r="B204" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="C204" s="17">
@@ -12972,7 +12972,7 @@
     </row>
     <row r="205" spans="2:52" ht="23.4">
       <c r="B205" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>93</v>
       </c>
       <c r="C205" s="17">
@@ -13039,7 +13039,7 @@
     </row>
     <row r="206" spans="2:52" ht="23.4">
       <c r="B206" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>94</v>
       </c>
       <c r="C206" s="17">
@@ -13106,7 +13106,7 @@
     </row>
     <row r="207" spans="2:52" ht="23.4">
       <c r="B207" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="C207" s="17">
@@ -13173,7 +13173,7 @@
     </row>
     <row r="208" spans="2:52" ht="23.4">
       <c r="B208" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>96</v>
       </c>
       <c r="C208" s="17">
@@ -13240,7 +13240,7 @@
     </row>
     <row r="209" spans="2:52" ht="23.4">
       <c r="B209" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97</v>
       </c>
       <c r="C209" s="17">
@@ -13307,7 +13307,7 @@
     </row>
     <row r="210" spans="2:52" ht="23.4">
       <c r="B210" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="C210" s="17">
@@ -13374,7 +13374,7 @@
     </row>
     <row r="211" spans="2:52" ht="23.4">
       <c r="B211" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99</v>
       </c>
       <c r="C211" s="17">
@@ -13441,7 +13441,7 @@
     </row>
     <row r="212" spans="2:52" ht="23.4">
       <c r="B212" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="C212" s="17">
@@ -13549,15 +13549,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AH28:AI28"/>
-    <mergeCell ref="AF28:AG28"/>
-    <mergeCell ref="B2:AA2"/>
-    <mergeCell ref="B4:T4"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="B14:T28"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y11:AA11"/>
     <mergeCell ref="I144:AV144"/>
     <mergeCell ref="I179:AZ179"/>
     <mergeCell ref="B30:AA30"/>
@@ -13569,6 +13560,15 @@
     <mergeCell ref="J42:N45"/>
     <mergeCell ref="J41:N41"/>
     <mergeCell ref="G104:AG104"/>
+    <mergeCell ref="AH28:AI28"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="B14:T28"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y11:AA11"/>
   </mergeCells>
   <conditionalFormatting sqref="Y15:AA26 AE26 AC27:AE39">
     <cfRule type="expression" dxfId="4" priority="16">
@@ -52167,34 +52167,34 @@
       <c r="BD1" s="6"/>
     </row>
     <row r="2" spans="2:56" ht="60.6" customHeight="1">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="88" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="111"/>
-      <c r="AA2" s="111"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
       <c r="AO2" s="3"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6"/>
@@ -52218,32 +52218,32 @@
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="2:56" ht="33.6" customHeight="1">
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="112"/>
-      <c r="R4" s="112"/>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="Y4" s="123" t="s">
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="Y4" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="123"/>
-      <c r="AA4" s="112"/>
+      <c r="Z4" s="100"/>
+      <c r="AA4" s="89"/>
       <c r="AO4" s="3"/>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -52471,11 +52471,11 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
       <c r="X11" s="31"/>
-      <c r="Y11" s="124" t="s">
+      <c r="Y11" s="101" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="125"/>
-      <c r="AA11" s="126"/>
+      <c r="Z11" s="102"/>
+      <c r="AA11" s="103"/>
       <c r="AO11" s="3"/>
       <c r="AY11" s="6"/>
       <c r="AZ11" s="6"/>
@@ -52520,33 +52520,33 @@
       <c r="BD12" s="6"/>
     </row>
     <row r="13" spans="2:56" ht="24.9" customHeight="1" thickBot="1">
-      <c r="B13" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="112"/>
-      <c r="N13" s="112"/>
-      <c r="O13" s="112"/>
-      <c r="P13" s="112"/>
-      <c r="Q13" s="112"/>
-      <c r="R13" s="112"/>
-      <c r="S13" s="112"/>
-      <c r="T13" s="112"/>
+      <c r="B13" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
       <c r="U13" s="60"/>
-      <c r="Y13" s="113" t="s">
+      <c r="Y13" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="Z13" s="112"/>
-      <c r="AA13" s="112"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
       <c r="AF13" s="60"/>
       <c r="AG13" s="60"/>
       <c r="AH13" s="60"/>
@@ -52554,27 +52554,27 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:56" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="114" t="s">
+      <c r="B14" s="91" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="115"/>
-      <c r="D14" s="115"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="115"/>
-      <c r="H14" s="115"/>
-      <c r="I14" s="115"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="115"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
-      <c r="N14" s="115"/>
-      <c r="O14" s="115"/>
-      <c r="P14" s="115"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="115"/>
-      <c r="S14" s="115"/>
-      <c r="T14" s="116"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="92"/>
+      <c r="Q14" s="92"/>
+      <c r="R14" s="92"/>
+      <c r="S14" s="92"/>
+      <c r="T14" s="93"/>
       <c r="U14" s="3"/>
       <c r="Y14" s="61" t="s">
         <v>31</v>
@@ -52591,25 +52591,25 @@
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:56" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B15" s="117"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-      <c r="S15" s="118"/>
-      <c r="T15" s="119"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95"/>
+      <c r="Q15" s="95"/>
+      <c r="R15" s="95"/>
+      <c r="S15" s="95"/>
+      <c r="T15" s="96"/>
       <c r="U15" s="3"/>
       <c r="Y15" s="62" t="s">
         <v>32</v>
@@ -52626,25 +52626,25 @@
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B16" s="117"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-      <c r="S16" s="118"/>
-      <c r="T16" s="119"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="95"/>
+      <c r="L16" s="95"/>
+      <c r="M16" s="95"/>
+      <c r="N16" s="95"/>
+      <c r="O16" s="95"/>
+      <c r="P16" s="95"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="95"/>
+      <c r="T16" s="96"/>
       <c r="U16" s="3"/>
       <c r="Y16" s="62" t="s">
         <v>47</v>
@@ -52660,25 +52660,25 @@
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B17" s="117"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-      <c r="S17" s="118"/>
-      <c r="T17" s="119"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="95"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="95"/>
+      <c r="T17" s="96"/>
       <c r="U17" s="3"/>
       <c r="Y17" s="62" t="s">
         <v>39</v>
@@ -52694,25 +52694,25 @@
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B18" s="117"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="118"/>
-      <c r="K18" s="118"/>
-      <c r="L18" s="118"/>
-      <c r="M18" s="118"/>
-      <c r="N18" s="118"/>
-      <c r="O18" s="118"/>
-      <c r="P18" s="118"/>
-      <c r="Q18" s="118"/>
-      <c r="R18" s="118"/>
-      <c r="S18" s="118"/>
-      <c r="T18" s="119"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="95"/>
+      <c r="M18" s="95"/>
+      <c r="N18" s="95"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="95"/>
+      <c r="R18" s="95"/>
+      <c r="S18" s="95"/>
+      <c r="T18" s="96"/>
       <c r="U18" s="3"/>
       <c r="Y18" s="62" t="s">
         <v>35</v>
@@ -52728,25 +52728,25 @@
       <c r="AO18" s="3"/>
     </row>
     <row r="19" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B19" s="117"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="118"/>
-      <c r="J19" s="118"/>
-      <c r="K19" s="118"/>
-      <c r="L19" s="118"/>
-      <c r="M19" s="118"/>
-      <c r="N19" s="118"/>
-      <c r="O19" s="118"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="118"/>
-      <c r="R19" s="118"/>
-      <c r="S19" s="118"/>
-      <c r="T19" s="119"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="95"/>
+      <c r="T19" s="96"/>
       <c r="U19" s="3"/>
       <c r="Y19" s="62" t="s">
         <v>42</v>
@@ -52762,25 +52762,25 @@
       <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="118"/>
-      <c r="K20" s="118"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118"/>
-      <c r="O20" s="118"/>
-      <c r="P20" s="118"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="118"/>
-      <c r="S20" s="118"/>
-      <c r="T20" s="119"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
+      <c r="R20" s="95"/>
+      <c r="S20" s="95"/>
+      <c r="T20" s="96"/>
       <c r="U20" s="3"/>
       <c r="Y20" s="62" t="s">
         <v>48</v>
@@ -52794,25 +52794,25 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B21" s="117"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="118"/>
-      <c r="S21" s="118"/>
-      <c r="T21" s="119"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="95"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
+      <c r="S21" s="95"/>
+      <c r="T21" s="96"/>
       <c r="U21" s="3"/>
       <c r="Y21" s="62" t="s">
         <v>49</v>
@@ -52828,25 +52828,25 @@
       <c r="AO21" s="3"/>
     </row>
     <row r="22" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B22" s="117"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
-      <c r="P22" s="118"/>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="118"/>
-      <c r="S22" s="118"/>
-      <c r="T22" s="119"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="95"/>
+      <c r="L22" s="95"/>
+      <c r="M22" s="95"/>
+      <c r="N22" s="95"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="95"/>
+      <c r="Q22" s="95"/>
+      <c r="R22" s="95"/>
+      <c r="S22" s="95"/>
+      <c r="T22" s="96"/>
       <c r="U22" s="3"/>
       <c r="Y22" s="62" t="s">
         <v>50</v>
@@ -52863,25 +52863,25 @@
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B23" s="117"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="118"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="118"/>
-      <c r="S23" s="118"/>
-      <c r="T23" s="119"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="95"/>
+      <c r="K23" s="95"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="95"/>
+      <c r="N23" s="95"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="95"/>
+      <c r="Q23" s="95"/>
+      <c r="R23" s="95"/>
+      <c r="S23" s="95"/>
+      <c r="T23" s="96"/>
       <c r="U23" s="3"/>
       <c r="Y23" s="62" t="s">
         <v>51</v>
@@ -52898,25 +52898,25 @@
       <c r="AP23" s="3"/>
     </row>
     <row r="24" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B24" s="117"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="118"/>
-      <c r="P24" s="118"/>
-      <c r="Q24" s="118"/>
-      <c r="R24" s="118"/>
-      <c r="S24" s="118"/>
-      <c r="T24" s="119"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="95"/>
+      <c r="K24" s="95"/>
+      <c r="L24" s="95"/>
+      <c r="M24" s="95"/>
+      <c r="N24" s="95"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="95"/>
+      <c r="T24" s="96"/>
       <c r="U24" s="3"/>
       <c r="Y24" s="62" t="s">
         <v>52</v>
@@ -52933,25 +52933,25 @@
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="118"/>
-      <c r="S25" s="118"/>
-      <c r="T25" s="119"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="95"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="95"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="95"/>
+      <c r="S25" s="95"/>
+      <c r="T25" s="96"/>
       <c r="U25" s="3"/>
       <c r="Y25" s="62" t="s">
         <v>53</v>
@@ -52966,25 +52966,25 @@
       <c r="AP25" s="3"/>
     </row>
     <row r="26" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B26" s="117"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="118"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
-      <c r="O26" s="118"/>
-      <c r="P26" s="118"/>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="118"/>
-      <c r="S26" s="118"/>
-      <c r="T26" s="119"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="95"/>
+      <c r="M26" s="95"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="95"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="95"/>
+      <c r="S26" s="95"/>
+      <c r="T26" s="96"/>
       <c r="U26" s="3"/>
       <c r="Y26" s="62" t="s">
         <v>105</v>
@@ -53004,25 +53004,25 @@
       <c r="AP26" s="3"/>
     </row>
     <row r="27" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B27" s="117"/>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
-      <c r="O27" s="118"/>
-      <c r="P27" s="118"/>
-      <c r="Q27" s="118"/>
-      <c r="R27" s="118"/>
-      <c r="S27" s="118"/>
-      <c r="T27" s="119"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="95"/>
+      <c r="M27" s="95"/>
+      <c r="N27" s="95"/>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="95"/>
+      <c r="T27" s="96"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -53041,25 +53041,25 @@
       <c r="AP27" s="3"/>
     </row>
     <row r="28" spans="2:56" ht="47.25" customHeight="1">
-      <c r="B28" s="120"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="121"/>
-      <c r="J28" s="121"/>
-      <c r="K28" s="121"/>
-      <c r="L28" s="121"/>
-      <c r="M28" s="121"/>
-      <c r="N28" s="121"/>
-      <c r="O28" s="121"/>
-      <c r="P28" s="121"/>
-      <c r="Q28" s="121"/>
-      <c r="R28" s="121"/>
-      <c r="S28" s="121"/>
-      <c r="T28" s="122"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="98"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="98"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
+      <c r="O28" s="98"/>
+      <c r="P28" s="98"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="99"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -53070,10 +53070,10 @@
       <c r="AC28" s="63"/>
       <c r="AD28" s="63"/>
       <c r="AE28" s="64"/>
-      <c r="AF28" s="110"/>
-      <c r="AG28" s="110"/>
-      <c r="AH28" s="110"/>
-      <c r="AI28" s="110"/>
+      <c r="AF28" s="87"/>
+      <c r="AG28" s="87"/>
+      <c r="AH28" s="87"/>
+      <c r="AI28" s="87"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
     </row>
@@ -53122,34 +53122,34 @@
       <c r="BD29" s="6"/>
     </row>
     <row r="30" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="91"/>
-      <c r="N30" s="91"/>
-      <c r="O30" s="91"/>
-      <c r="P30" s="91"/>
-      <c r="Q30" s="91"/>
-      <c r="R30" s="91"/>
-      <c r="S30" s="91"/>
-      <c r="T30" s="91"/>
-      <c r="U30" s="91"/>
-      <c r="V30" s="91"/>
-      <c r="W30" s="91"/>
-      <c r="X30" s="91"/>
-      <c r="Y30" s="91"/>
-      <c r="Z30" s="91"/>
-      <c r="AA30" s="92"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="108"/>
+      <c r="F30" s="108"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="108"/>
+      <c r="L30" s="108"/>
+      <c r="M30" s="108"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="108"/>
+      <c r="T30" s="108"/>
+      <c r="U30" s="108"/>
+      <c r="V30" s="108"/>
+      <c r="W30" s="108"/>
+      <c r="X30" s="108"/>
+      <c r="Y30" s="108"/>
+      <c r="Z30" s="108"/>
+      <c r="AA30" s="109"/>
       <c r="AC30" s="63"/>
       <c r="AD30" s="63"/>
       <c r="AE30" s="64"/>
@@ -53212,29 +53212,29 @@
       <c r="E33" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="93" t="s">
+      <c r="G33" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="94"/>
-      <c r="O33" s="94"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="94"/>
-      <c r="R33" s="94"/>
-      <c r="S33" s="94"/>
-      <c r="T33" s="94"/>
-      <c r="U33" s="94"/>
-      <c r="V33" s="94"/>
-      <c r="W33" s="94"/>
-      <c r="X33" s="94"/>
-      <c r="Y33" s="94"/>
-      <c r="Z33" s="94"/>
-      <c r="AA33" s="95"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="111"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="111"/>
+      <c r="O33" s="111"/>
+      <c r="P33" s="111"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="111"/>
+      <c r="S33" s="111"/>
+      <c r="T33" s="111"/>
+      <c r="U33" s="111"/>
+      <c r="V33" s="111"/>
+      <c r="W33" s="111"/>
+      <c r="X33" s="111"/>
+      <c r="Y33" s="111"/>
+      <c r="Z33" s="111"/>
+      <c r="AA33" s="112"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="63"/>
       <c r="AE33" s="64"/>
@@ -53257,29 +53257,29 @@
         <v>29</v>
       </c>
       <c r="F34" s="36"/>
-      <c r="G34" s="96" t="s">
+      <c r="G34" s="113" t="s">
         <v>302</v>
       </c>
-      <c r="H34" s="97"/>
-      <c r="I34" s="97"/>
-      <c r="J34" s="97"/>
-      <c r="K34" s="97"/>
-      <c r="L34" s="97"/>
-      <c r="M34" s="97"/>
-      <c r="N34" s="97"/>
-      <c r="O34" s="97"/>
-      <c r="P34" s="97"/>
-      <c r="Q34" s="97"/>
-      <c r="R34" s="97"/>
-      <c r="S34" s="97"/>
-      <c r="T34" s="97"/>
-      <c r="U34" s="97"/>
-      <c r="V34" s="97"/>
-      <c r="W34" s="97"/>
-      <c r="X34" s="97"/>
-      <c r="Y34" s="97"/>
-      <c r="Z34" s="97"/>
-      <c r="AA34" s="98"/>
+      <c r="H34" s="114"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="114"/>
+      <c r="K34" s="114"/>
+      <c r="L34" s="114"/>
+      <c r="M34" s="114"/>
+      <c r="N34" s="114"/>
+      <c r="O34" s="114"/>
+      <c r="P34" s="114"/>
+      <c r="Q34" s="114"/>
+      <c r="R34" s="114"/>
+      <c r="S34" s="114"/>
+      <c r="T34" s="114"/>
+      <c r="U34" s="114"/>
+      <c r="V34" s="114"/>
+      <c r="W34" s="114"/>
+      <c r="X34" s="114"/>
+      <c r="Y34" s="114"/>
+      <c r="Z34" s="114"/>
+      <c r="AA34" s="115"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="63"/>
       <c r="AE34" s="64"/>
@@ -53302,29 +53302,29 @@
         <v>51</v>
       </c>
       <c r="F35" s="36"/>
-      <c r="G35" s="99" t="s">
+      <c r="G35" s="116" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="100"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="100"/>
-      <c r="N35" s="100"/>
-      <c r="O35" s="100"/>
-      <c r="P35" s="100"/>
-      <c r="Q35" s="100"/>
-      <c r="R35" s="100"/>
-      <c r="S35" s="100"/>
-      <c r="T35" s="100"/>
-      <c r="U35" s="100"/>
-      <c r="V35" s="100"/>
-      <c r="W35" s="100"/>
-      <c r="X35" s="100"/>
-      <c r="Y35" s="100"/>
-      <c r="Z35" s="100"/>
-      <c r="AA35" s="101"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="117"/>
+      <c r="N35" s="117"/>
+      <c r="O35" s="117"/>
+      <c r="P35" s="117"/>
+      <c r="Q35" s="117"/>
+      <c r="R35" s="117"/>
+      <c r="S35" s="117"/>
+      <c r="T35" s="117"/>
+      <c r="U35" s="117"/>
+      <c r="V35" s="117"/>
+      <c r="W35" s="117"/>
+      <c r="X35" s="117"/>
+      <c r="Y35" s="117"/>
+      <c r="Z35" s="117"/>
+      <c r="AA35" s="118"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="63"/>
       <c r="AE35" s="64"/>
@@ -53347,29 +53347,29 @@
         <v>95</v>
       </c>
       <c r="F36" s="36"/>
-      <c r="G36" s="102" t="s">
+      <c r="G36" s="119" t="s">
         <v>301</v>
       </c>
-      <c r="H36" s="103"/>
-      <c r="I36" s="103"/>
-      <c r="J36" s="103"/>
-      <c r="K36" s="103"/>
-      <c r="L36" s="103"/>
-      <c r="M36" s="103"/>
-      <c r="N36" s="103"/>
-      <c r="O36" s="103"/>
-      <c r="P36" s="103"/>
-      <c r="Q36" s="103"/>
-      <c r="R36" s="103"/>
-      <c r="S36" s="103"/>
-      <c r="T36" s="103"/>
-      <c r="U36" s="103"/>
-      <c r="V36" s="103"/>
-      <c r="W36" s="103"/>
-      <c r="X36" s="103"/>
-      <c r="Y36" s="103"/>
-      <c r="Z36" s="103"/>
-      <c r="AA36" s="104"/>
+      <c r="H36" s="120"/>
+      <c r="I36" s="120"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="120"/>
+      <c r="N36" s="120"/>
+      <c r="O36" s="120"/>
+      <c r="P36" s="120"/>
+      <c r="Q36" s="120"/>
+      <c r="R36" s="120"/>
+      <c r="S36" s="120"/>
+      <c r="T36" s="120"/>
+      <c r="U36" s="120"/>
+      <c r="V36" s="120"/>
+      <c r="W36" s="120"/>
+      <c r="X36" s="120"/>
+      <c r="Y36" s="120"/>
+      <c r="Z36" s="120"/>
+      <c r="AA36" s="121"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="63"/>
       <c r="AE36" s="64"/>
@@ -54838,20 +54838,20 @@
       <c r="E67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="93" t="s">
+      <c r="G67" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="H67" s="94"/>
-      <c r="I67" s="94"/>
-      <c r="J67" s="94"/>
-      <c r="K67" s="94"/>
-      <c r="L67" s="94"/>
-      <c r="M67" s="94"/>
-      <c r="N67" s="94"/>
-      <c r="O67" s="94"/>
-      <c r="P67" s="94"/>
-      <c r="Q67" s="94"/>
-      <c r="R67" s="95"/>
+      <c r="H67" s="111"/>
+      <c r="I67" s="111"/>
+      <c r="J67" s="111"/>
+      <c r="K67" s="111"/>
+      <c r="L67" s="111"/>
+      <c r="M67" s="111"/>
+      <c r="N67" s="111"/>
+      <c r="O67" s="111"/>
+      <c r="P67" s="111"/>
+      <c r="Q67" s="111"/>
+      <c r="R67" s="112"/>
       <c r="S67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -56891,34 +56891,34 @@
       <c r="E104" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G104" s="107" t="s">
+      <c r="G104" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="H104" s="108"/>
-      <c r="I104" s="108"/>
-      <c r="J104" s="108"/>
-      <c r="K104" s="108"/>
-      <c r="L104" s="108"/>
-      <c r="M104" s="108"/>
-      <c r="N104" s="108"/>
-      <c r="O104" s="108"/>
-      <c r="P104" s="108"/>
-      <c r="Q104" s="108"/>
-      <c r="R104" s="108"/>
-      <c r="S104" s="108"/>
-      <c r="T104" s="108"/>
-      <c r="U104" s="108"/>
-      <c r="V104" s="108"/>
-      <c r="W104" s="108"/>
-      <c r="X104" s="108"/>
-      <c r="Y104" s="108"/>
-      <c r="Z104" s="108"/>
-      <c r="AA104" s="108"/>
-      <c r="AB104" s="108"/>
-      <c r="AC104" s="108"/>
-      <c r="AD104" s="108"/>
-      <c r="AE104" s="108"/>
-      <c r="AF104" s="109"/>
+      <c r="H104" s="125"/>
+      <c r="I104" s="125"/>
+      <c r="J104" s="125"/>
+      <c r="K104" s="125"/>
+      <c r="L104" s="125"/>
+      <c r="M104" s="125"/>
+      <c r="N104" s="125"/>
+      <c r="O104" s="125"/>
+      <c r="P104" s="125"/>
+      <c r="Q104" s="125"/>
+      <c r="R104" s="125"/>
+      <c r="S104" s="125"/>
+      <c r="T104" s="125"/>
+      <c r="U104" s="125"/>
+      <c r="V104" s="125"/>
+      <c r="W104" s="125"/>
+      <c r="X104" s="125"/>
+      <c r="Y104" s="125"/>
+      <c r="Z104" s="125"/>
+      <c r="AA104" s="125"/>
+      <c r="AB104" s="125"/>
+      <c r="AC104" s="125"/>
+      <c r="AD104" s="125"/>
+      <c r="AE104" s="125"/>
+      <c r="AF104" s="126"/>
       <c r="AG104" s="6"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
@@ -58634,47 +58634,47 @@
       <c r="G144" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I144" s="87" t="s">
+      <c r="I144" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="J144" s="88"/>
-      <c r="K144" s="88"/>
-      <c r="L144" s="88"/>
-      <c r="M144" s="88"/>
-      <c r="N144" s="88"/>
-      <c r="O144" s="88"/>
-      <c r="P144" s="88"/>
-      <c r="Q144" s="88"/>
-      <c r="R144" s="88"/>
-      <c r="S144" s="88"/>
-      <c r="T144" s="88"/>
-      <c r="U144" s="88"/>
-      <c r="V144" s="88"/>
-      <c r="W144" s="88"/>
-      <c r="X144" s="88"/>
-      <c r="Y144" s="88"/>
-      <c r="Z144" s="88"/>
-      <c r="AA144" s="88"/>
-      <c r="AB144" s="88"/>
-      <c r="AC144" s="88"/>
-      <c r="AD144" s="88"/>
-      <c r="AE144" s="88"/>
-      <c r="AF144" s="88"/>
-      <c r="AG144" s="88"/>
-      <c r="AH144" s="88"/>
-      <c r="AI144" s="88"/>
-      <c r="AJ144" s="88"/>
-      <c r="AK144" s="88"/>
-      <c r="AL144" s="88"/>
-      <c r="AM144" s="88"/>
-      <c r="AN144" s="88"/>
-      <c r="AO144" s="88"/>
-      <c r="AP144" s="88"/>
-      <c r="AQ144" s="88"/>
-      <c r="AR144" s="88"/>
-      <c r="AS144" s="88"/>
-      <c r="AT144" s="88"/>
-      <c r="AU144" s="89"/>
+      <c r="J144" s="105"/>
+      <c r="K144" s="105"/>
+      <c r="L144" s="105"/>
+      <c r="M144" s="105"/>
+      <c r="N144" s="105"/>
+      <c r="O144" s="105"/>
+      <c r="P144" s="105"/>
+      <c r="Q144" s="105"/>
+      <c r="R144" s="105"/>
+      <c r="S144" s="105"/>
+      <c r="T144" s="105"/>
+      <c r="U144" s="105"/>
+      <c r="V144" s="105"/>
+      <c r="W144" s="105"/>
+      <c r="X144" s="105"/>
+      <c r="Y144" s="105"/>
+      <c r="Z144" s="105"/>
+      <c r="AA144" s="105"/>
+      <c r="AB144" s="105"/>
+      <c r="AC144" s="105"/>
+      <c r="AD144" s="105"/>
+      <c r="AE144" s="105"/>
+      <c r="AF144" s="105"/>
+      <c r="AG144" s="105"/>
+      <c r="AH144" s="105"/>
+      <c r="AI144" s="105"/>
+      <c r="AJ144" s="105"/>
+      <c r="AK144" s="105"/>
+      <c r="AL144" s="105"/>
+      <c r="AM144" s="105"/>
+      <c r="AN144" s="105"/>
+      <c r="AO144" s="105"/>
+      <c r="AP144" s="105"/>
+      <c r="AQ144" s="105"/>
+      <c r="AR144" s="105"/>
+      <c r="AS144" s="105"/>
+      <c r="AT144" s="105"/>
+      <c r="AU144" s="106"/>
       <c r="AV144" s="6"/>
       <c r="AW144" s="6"/>
       <c r="AX144" s="6"/>
@@ -60326,55 +60326,55 @@
       <c r="G179" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I179" s="87" t="s">
+      <c r="I179" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="J179" s="88"/>
-      <c r="K179" s="88"/>
-      <c r="L179" s="88"/>
-      <c r="M179" s="88"/>
-      <c r="N179" s="88"/>
-      <c r="O179" s="88"/>
-      <c r="P179" s="88"/>
-      <c r="Q179" s="88"/>
-      <c r="R179" s="88"/>
-      <c r="S179" s="88"/>
-      <c r="T179" s="88"/>
-      <c r="U179" s="88"/>
-      <c r="V179" s="88"/>
-      <c r="W179" s="88"/>
-      <c r="X179" s="88"/>
-      <c r="Y179" s="88"/>
-      <c r="Z179" s="88"/>
-      <c r="AA179" s="88"/>
-      <c r="AB179" s="88"/>
-      <c r="AC179" s="88"/>
-      <c r="AD179" s="88"/>
-      <c r="AE179" s="88"/>
-      <c r="AF179" s="88"/>
-      <c r="AG179" s="88"/>
-      <c r="AH179" s="88"/>
-      <c r="AI179" s="88"/>
-      <c r="AJ179" s="88"/>
-      <c r="AK179" s="88"/>
-      <c r="AL179" s="88"/>
-      <c r="AM179" s="88"/>
-      <c r="AN179" s="88"/>
-      <c r="AO179" s="88"/>
-      <c r="AP179" s="88"/>
-      <c r="AQ179" s="88"/>
-      <c r="AR179" s="88"/>
-      <c r="AS179" s="88"/>
-      <c r="AT179" s="88"/>
-      <c r="AU179" s="88"/>
-      <c r="AV179" s="88"/>
-      <c r="AW179" s="88"/>
-      <c r="AX179" s="88"/>
-      <c r="AY179" s="88"/>
-      <c r="AZ179" s="88"/>
-      <c r="BA179" s="88"/>
-      <c r="BB179" s="88"/>
-      <c r="BC179" s="89"/>
+      <c r="J179" s="105"/>
+      <c r="K179" s="105"/>
+      <c r="L179" s="105"/>
+      <c r="M179" s="105"/>
+      <c r="N179" s="105"/>
+      <c r="O179" s="105"/>
+      <c r="P179" s="105"/>
+      <c r="Q179" s="105"/>
+      <c r="R179" s="105"/>
+      <c r="S179" s="105"/>
+      <c r="T179" s="105"/>
+      <c r="U179" s="105"/>
+      <c r="V179" s="105"/>
+      <c r="W179" s="105"/>
+      <c r="X179" s="105"/>
+      <c r="Y179" s="105"/>
+      <c r="Z179" s="105"/>
+      <c r="AA179" s="105"/>
+      <c r="AB179" s="105"/>
+      <c r="AC179" s="105"/>
+      <c r="AD179" s="105"/>
+      <c r="AE179" s="105"/>
+      <c r="AF179" s="105"/>
+      <c r="AG179" s="105"/>
+      <c r="AH179" s="105"/>
+      <c r="AI179" s="105"/>
+      <c r="AJ179" s="105"/>
+      <c r="AK179" s="105"/>
+      <c r="AL179" s="105"/>
+      <c r="AM179" s="105"/>
+      <c r="AN179" s="105"/>
+      <c r="AO179" s="105"/>
+      <c r="AP179" s="105"/>
+      <c r="AQ179" s="105"/>
+      <c r="AR179" s="105"/>
+      <c r="AS179" s="105"/>
+      <c r="AT179" s="105"/>
+      <c r="AU179" s="105"/>
+      <c r="AV179" s="105"/>
+      <c r="AW179" s="105"/>
+      <c r="AX179" s="105"/>
+      <c r="AY179" s="105"/>
+      <c r="AZ179" s="105"/>
+      <c r="BA179" s="105"/>
+      <c r="BB179" s="105"/>
+      <c r="BC179" s="106"/>
       <c r="BD179" s="6"/>
     </row>
     <row r="180" spans="2:56" ht="15" thickTop="1">
@@ -62690,11 +62690,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G36:AA36"/>
-    <mergeCell ref="G67:R67"/>
-    <mergeCell ref="I179:BC179"/>
-    <mergeCell ref="I144:AU144"/>
-    <mergeCell ref="G104:AF104"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="Y13:AA13"/>
     <mergeCell ref="AF28:AG28"/>
     <mergeCell ref="AH28:AI28"/>
     <mergeCell ref="B30:AA30"/>
@@ -62702,12 +62703,11 @@
     <mergeCell ref="G35:AA35"/>
     <mergeCell ref="G34:AA34"/>
     <mergeCell ref="B14:T28"/>
-    <mergeCell ref="B2:AA2"/>
-    <mergeCell ref="B4:T4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="G36:AA36"/>
+    <mergeCell ref="G67:R67"/>
+    <mergeCell ref="I179:BC179"/>
+    <mergeCell ref="I144:AU144"/>
+    <mergeCell ref="G104:AF104"/>
   </mergeCells>
   <conditionalFormatting sqref="Y15:AA26 AE26 AC27:AE39">
     <cfRule type="expression" dxfId="0" priority="16">

</xml_diff>

<commit_message>
Rebuilding my lost work
</commit_message>
<xml_diff>
--- a/ExcelEsport/FMWC_Examples/What Is My Flight Number - Patrick Chatain - My Work.xlsx
+++ b/ExcelEsport/FMWC_Examples/What Is My Flight Number - Patrick Chatain - My Work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\FMWC_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D41DCE-8BD3-49C1-94F0-F309F2DF287C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC27B03-FD3B-4695-8410-59B8ED23DC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{114A3ACC-2F61-4F50-A5CF-63A86B2334B2}"/>
   </bookViews>
@@ -2086,57 +2086,6 @@
     <xf numFmtId="3" fontId="5" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2205,6 +2154,57 @@
     </xf>
     <xf numFmtId="3" fontId="14" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3345,7 +3345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B840F547-97A4-4023-9D52-57A423820E20}">
   <dimension ref="A1:AZ216"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A123" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A131" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -3397,34 +3397,34 @@
       <c r="AZ1" s="6"/>
     </row>
     <row r="2" spans="2:52" ht="60.6" customHeight="1">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="111" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="88"/>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
       <c r="AO2" s="3"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6"/>
@@ -3440,32 +3440,32 @@
       <c r="AZ3" s="6"/>
     </row>
     <row r="4" spans="2:52" ht="33.6" customHeight="1">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="Y4" s="100" t="s">
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="Y4" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="100"/>
-      <c r="AA4" s="89"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="112"/>
       <c r="AO4" s="3"/>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -3665,11 +3665,11 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
       <c r="X11" s="31"/>
-      <c r="Y11" s="101" t="s">
+      <c r="Y11" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="102"/>
-      <c r="AA11" s="103"/>
+      <c r="Z11" s="125"/>
+      <c r="AA11" s="126"/>
       <c r="AO11" s="3"/>
       <c r="AY11" s="6"/>
       <c r="AZ11" s="6"/>
@@ -3704,33 +3704,33 @@
       <c r="AZ12" s="6"/>
     </row>
     <row r="13" spans="2:52" ht="24.9" customHeight="1" thickBot="1">
-      <c r="B13" s="90" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="89"/>
-      <c r="T13" s="89"/>
+      <c r="B13" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="112"/>
+      <c r="T13" s="112"/>
       <c r="U13" s="60"/>
-      <c r="Y13" s="90" t="s">
+      <c r="Y13" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="Z13" s="89"/>
-      <c r="AA13" s="89"/>
+      <c r="Z13" s="112"/>
+      <c r="AA13" s="112"/>
       <c r="AF13" s="60"/>
       <c r="AG13" s="60"/>
       <c r="AH13" s="60"/>
@@ -3738,27 +3738,27 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:52" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="114" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="92"/>
-      <c r="O14" s="92"/>
-      <c r="P14" s="92"/>
-      <c r="Q14" s="92"/>
-      <c r="R14" s="92"/>
-      <c r="S14" s="92"/>
-      <c r="T14" s="93"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="115"/>
+      <c r="L14" s="115"/>
+      <c r="M14" s="115"/>
+      <c r="N14" s="115"/>
+      <c r="O14" s="115"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="115"/>
+      <c r="R14" s="115"/>
+      <c r="S14" s="115"/>
+      <c r="T14" s="116"/>
       <c r="U14" s="3"/>
       <c r="Y14" s="61" t="s">
         <v>31</v>
@@ -3775,25 +3775,25 @@
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:52" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B15" s="94"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="95"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="95"/>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="95"/>
-      <c r="R15" s="95"/>
-      <c r="S15" s="95"/>
-      <c r="T15" s="96"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="118"/>
+      <c r="Q15" s="118"/>
+      <c r="R15" s="118"/>
+      <c r="S15" s="118"/>
+      <c r="T15" s="119"/>
       <c r="U15" s="3"/>
       <c r="Y15" s="62" t="s">
         <v>32</v>
@@ -3813,25 +3813,25 @@
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B16" s="94"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="95"/>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="95"/>
-      <c r="S16" s="95"/>
-      <c r="T16" s="96"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="118"/>
+      <c r="S16" s="118"/>
+      <c r="T16" s="119"/>
       <c r="U16" s="3"/>
       <c r="Y16" s="62" t="s">
         <v>47</v>
@@ -3850,25 +3850,25 @@
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="95"/>
-      <c r="N17" s="95"/>
-      <c r="O17" s="95"/>
-      <c r="P17" s="95"/>
-      <c r="Q17" s="95"/>
-      <c r="R17" s="95"/>
-      <c r="S17" s="95"/>
-      <c r="T17" s="96"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="118"/>
+      <c r="P17" s="118"/>
+      <c r="Q17" s="118"/>
+      <c r="R17" s="118"/>
+      <c r="S17" s="118"/>
+      <c r="T17" s="119"/>
       <c r="U17" s="3"/>
       <c r="Y17" s="62" t="s">
         <v>39</v>
@@ -3887,25 +3887,25 @@
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B18" s="94"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="95"/>
-      <c r="O18" s="95"/>
-      <c r="P18" s="95"/>
-      <c r="Q18" s="95"/>
-      <c r="R18" s="95"/>
-      <c r="S18" s="95"/>
-      <c r="T18" s="96"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
+      <c r="N18" s="118"/>
+      <c r="O18" s="118"/>
+      <c r="P18" s="118"/>
+      <c r="Q18" s="118"/>
+      <c r="R18" s="118"/>
+      <c r="S18" s="118"/>
+      <c r="T18" s="119"/>
       <c r="U18" s="3"/>
       <c r="Y18" s="62" t="s">
         <v>35</v>
@@ -3924,25 +3924,25 @@
       <c r="AO18" s="3"/>
     </row>
     <row r="19" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B19" s="94"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="95"/>
-      <c r="P19" s="95"/>
-      <c r="Q19" s="95"/>
-      <c r="R19" s="95"/>
-      <c r="S19" s="95"/>
-      <c r="T19" s="96"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="118"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="118"/>
+      <c r="N19" s="118"/>
+      <c r="O19" s="118"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="118"/>
+      <c r="R19" s="118"/>
+      <c r="S19" s="118"/>
+      <c r="T19" s="119"/>
       <c r="U19" s="3"/>
       <c r="Y19" s="62" t="s">
         <v>42</v>
@@ -3961,25 +3961,25 @@
       <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B20" s="94"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="95"/>
-      <c r="K20" s="95"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="95"/>
-      <c r="Q20" s="95"/>
-      <c r="R20" s="95"/>
-      <c r="S20" s="95"/>
-      <c r="T20" s="96"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="118"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="118"/>
+      <c r="K20" s="118"/>
+      <c r="L20" s="118"/>
+      <c r="M20" s="118"/>
+      <c r="N20" s="118"/>
+      <c r="O20" s="118"/>
+      <c r="P20" s="118"/>
+      <c r="Q20" s="118"/>
+      <c r="R20" s="118"/>
+      <c r="S20" s="118"/>
+      <c r="T20" s="119"/>
       <c r="U20" s="3"/>
       <c r="Y20" s="62" t="s">
         <v>48</v>
@@ -3996,25 +3996,25 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B21" s="94"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="95"/>
-      <c r="S21" s="95"/>
-      <c r="T21" s="96"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="118"/>
+      <c r="O21" s="118"/>
+      <c r="P21" s="118"/>
+      <c r="Q21" s="118"/>
+      <c r="R21" s="118"/>
+      <c r="S21" s="118"/>
+      <c r="T21" s="119"/>
       <c r="U21" s="3"/>
       <c r="Y21" s="62" t="s">
         <v>49</v>
@@ -4033,25 +4033,25 @@
       <c r="AO21" s="3"/>
     </row>
     <row r="22" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="95"/>
-      <c r="J22" s="95"/>
-      <c r="K22" s="95"/>
-      <c r="L22" s="95"/>
-      <c r="M22" s="95"/>
-      <c r="N22" s="95"/>
-      <c r="O22" s="95"/>
-      <c r="P22" s="95"/>
-      <c r="Q22" s="95"/>
-      <c r="R22" s="95"/>
-      <c r="S22" s="95"/>
-      <c r="T22" s="96"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="118"/>
+      <c r="P22" s="118"/>
+      <c r="Q22" s="118"/>
+      <c r="R22" s="118"/>
+      <c r="S22" s="118"/>
+      <c r="T22" s="119"/>
       <c r="U22" s="3"/>
       <c r="Y22" s="62" t="s">
         <v>50</v>
@@ -4071,25 +4071,25 @@
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B23" s="94"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="95"/>
-      <c r="K23" s="95"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
-      <c r="P23" s="95"/>
-      <c r="Q23" s="95"/>
-      <c r="R23" s="95"/>
-      <c r="S23" s="95"/>
-      <c r="T23" s="96"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="118"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="118"/>
+      <c r="M23" s="118"/>
+      <c r="N23" s="118"/>
+      <c r="O23" s="118"/>
+      <c r="P23" s="118"/>
+      <c r="Q23" s="118"/>
+      <c r="R23" s="118"/>
+      <c r="S23" s="118"/>
+      <c r="T23" s="119"/>
       <c r="U23" s="3"/>
       <c r="Y23" s="62" t="s">
         <v>51</v>
@@ -4109,25 +4109,25 @@
       <c r="AP23" s="3"/>
     </row>
     <row r="24" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B24" s="94"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="95"/>
-      <c r="N24" s="95"/>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="95"/>
-      <c r="S24" s="95"/>
-      <c r="T24" s="96"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="118"/>
+      <c r="M24" s="118"/>
+      <c r="N24" s="118"/>
+      <c r="O24" s="118"/>
+      <c r="P24" s="118"/>
+      <c r="Q24" s="118"/>
+      <c r="R24" s="118"/>
+      <c r="S24" s="118"/>
+      <c r="T24" s="119"/>
       <c r="U24" s="3"/>
       <c r="Y24" s="62" t="s">
         <v>52</v>
@@ -4147,25 +4147,25 @@
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B25" s="94"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="95"/>
-      <c r="Q25" s="95"/>
-      <c r="R25" s="95"/>
-      <c r="S25" s="95"/>
-      <c r="T25" s="96"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="118"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="118"/>
+      <c r="K25" s="118"/>
+      <c r="L25" s="118"/>
+      <c r="M25" s="118"/>
+      <c r="N25" s="118"/>
+      <c r="O25" s="118"/>
+      <c r="P25" s="118"/>
+      <c r="Q25" s="118"/>
+      <c r="R25" s="118"/>
+      <c r="S25" s="118"/>
+      <c r="T25" s="119"/>
       <c r="U25" s="3"/>
       <c r="Y25" s="62" t="s">
         <v>53</v>
@@ -4183,25 +4183,25 @@
       <c r="AP25" s="3"/>
     </row>
     <row r="26" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B26" s="94"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="95"/>
-      <c r="I26" s="95"/>
-      <c r="J26" s="95"/>
-      <c r="K26" s="95"/>
-      <c r="L26" s="95"/>
-      <c r="M26" s="95"/>
-      <c r="N26" s="95"/>
-      <c r="O26" s="95"/>
-      <c r="P26" s="95"/>
-      <c r="Q26" s="95"/>
-      <c r="R26" s="95"/>
-      <c r="S26" s="95"/>
-      <c r="T26" s="96"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="118"/>
+      <c r="M26" s="118"/>
+      <c r="N26" s="118"/>
+      <c r="O26" s="118"/>
+      <c r="P26" s="118"/>
+      <c r="Q26" s="118"/>
+      <c r="R26" s="118"/>
+      <c r="S26" s="118"/>
+      <c r="T26" s="119"/>
       <c r="U26" s="3"/>
       <c r="Y26" s="62" t="s">
         <v>105</v>
@@ -4224,25 +4224,25 @@
       <c r="AP26" s="3"/>
     </row>
     <row r="27" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B27" s="94"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="95"/>
-      <c r="N27" s="95"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="95"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="96"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="118"/>
+      <c r="O27" s="118"/>
+      <c r="P27" s="118"/>
+      <c r="Q27" s="118"/>
+      <c r="R27" s="118"/>
+      <c r="S27" s="118"/>
+      <c r="T27" s="119"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -4261,25 +4261,25 @@
       <c r="AP27" s="3"/>
     </row>
     <row r="28" spans="2:52" ht="47.25" customHeight="1">
-      <c r="B28" s="97"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
-      <c r="J28" s="98"/>
-      <c r="K28" s="98"/>
-      <c r="L28" s="98"/>
-      <c r="M28" s="98"/>
-      <c r="N28" s="98"/>
-      <c r="O28" s="98"/>
-      <c r="P28" s="98"/>
-      <c r="Q28" s="98"/>
-      <c r="R28" s="98"/>
-      <c r="S28" s="98"/>
-      <c r="T28" s="99"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="121"/>
+      <c r="K28" s="121"/>
+      <c r="L28" s="121"/>
+      <c r="M28" s="121"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="121"/>
+      <c r="P28" s="121"/>
+      <c r="Q28" s="121"/>
+      <c r="R28" s="121"/>
+      <c r="S28" s="121"/>
+      <c r="T28" s="122"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -4290,10 +4290,10 @@
       <c r="AC28" s="63"/>
       <c r="AD28" s="63"/>
       <c r="AE28" s="64"/>
-      <c r="AF28" s="87"/>
-      <c r="AG28" s="87"/>
-      <c r="AH28" s="87"/>
-      <c r="AI28" s="87"/>
+      <c r="AF28" s="110"/>
+      <c r="AG28" s="110"/>
+      <c r="AH28" s="110"/>
+      <c r="AI28" s="110"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
     </row>
@@ -4338,34 +4338,34 @@
       <c r="AZ29" s="6"/>
     </row>
     <row r="30" spans="2:52" ht="25.5" customHeight="1">
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="108"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="108"/>
-      <c r="F30" s="108"/>
-      <c r="G30" s="108"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="108"/>
-      <c r="J30" s="108"/>
-      <c r="K30" s="108"/>
-      <c r="L30" s="108"/>
-      <c r="M30" s="108"/>
-      <c r="N30" s="108"/>
-      <c r="O30" s="108"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="108"/>
-      <c r="T30" s="108"/>
-      <c r="U30" s="108"/>
-      <c r="V30" s="108"/>
-      <c r="W30" s="108"/>
-      <c r="X30" s="108"/>
-      <c r="Y30" s="108"/>
-      <c r="Z30" s="108"/>
-      <c r="AA30" s="109"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="91"/>
+      <c r="R30" s="91"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="91"/>
+      <c r="X30" s="91"/>
+      <c r="Y30" s="91"/>
+      <c r="Z30" s="91"/>
+      <c r="AA30" s="92"/>
       <c r="AC30" s="63"/>
       <c r="AD30" s="63"/>
       <c r="AE30" s="64"/>
@@ -4416,29 +4416,29 @@
       <c r="E33" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="110" t="s">
+      <c r="G33" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="111"/>
-      <c r="I33" s="111"/>
-      <c r="J33" s="111"/>
-      <c r="K33" s="111"/>
-      <c r="L33" s="111"/>
-      <c r="M33" s="111"/>
-      <c r="N33" s="111"/>
-      <c r="O33" s="111"/>
-      <c r="P33" s="111"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="111"/>
-      <c r="W33" s="111"/>
-      <c r="X33" s="111"/>
-      <c r="Y33" s="111"/>
-      <c r="Z33" s="111"/>
-      <c r="AA33" s="112"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="95"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="63"/>
       <c r="AE33" s="64"/>
@@ -4458,29 +4458,29 @@
         <f>IF(AND(E34&lt;&gt;"",E34=[1]Answers!E34),1,IF(ISBLANK(E34),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G34" s="113" t="s">
+      <c r="G34" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="H34" s="114"/>
-      <c r="I34" s="114"/>
-      <c r="J34" s="114"/>
-      <c r="K34" s="114"/>
-      <c r="L34" s="114"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="114"/>
-      <c r="O34" s="114"/>
-      <c r="P34" s="114"/>
-      <c r="Q34" s="114"/>
-      <c r="R34" s="114"/>
-      <c r="S34" s="114"/>
-      <c r="T34" s="114"/>
-      <c r="U34" s="114"/>
-      <c r="V34" s="114"/>
-      <c r="W34" s="114"/>
-      <c r="X34" s="114"/>
-      <c r="Y34" s="114"/>
-      <c r="Z34" s="114"/>
-      <c r="AA34" s="115"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="97"/>
+      <c r="N34" s="97"/>
+      <c r="O34" s="97"/>
+      <c r="P34" s="97"/>
+      <c r="Q34" s="97"/>
+      <c r="R34" s="97"/>
+      <c r="S34" s="97"/>
+      <c r="T34" s="97"/>
+      <c r="U34" s="97"/>
+      <c r="V34" s="97"/>
+      <c r="W34" s="97"/>
+      <c r="X34" s="97"/>
+      <c r="Y34" s="97"/>
+      <c r="Z34" s="97"/>
+      <c r="AA34" s="98"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="63"/>
       <c r="AE34" s="64"/>
@@ -4500,29 +4500,29 @@
         <f>IF(AND(E35&lt;&gt;"",E35=[1]Answers!E35),1,IF(ISBLANK(E35),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G35" s="116" t="s">
+      <c r="G35" s="99" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="117"/>
-      <c r="I35" s="117"/>
-      <c r="J35" s="117"/>
-      <c r="K35" s="117"/>
-      <c r="L35" s="117"/>
-      <c r="M35" s="117"/>
-      <c r="N35" s="117"/>
-      <c r="O35" s="117"/>
-      <c r="P35" s="117"/>
-      <c r="Q35" s="117"/>
-      <c r="R35" s="117"/>
-      <c r="S35" s="117"/>
-      <c r="T35" s="117"/>
-      <c r="U35" s="117"/>
-      <c r="V35" s="117"/>
-      <c r="W35" s="117"/>
-      <c r="X35" s="117"/>
-      <c r="Y35" s="117"/>
-      <c r="Z35" s="117"/>
-      <c r="AA35" s="118"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="100"/>
+      <c r="R35" s="100"/>
+      <c r="S35" s="100"/>
+      <c r="T35" s="100"/>
+      <c r="U35" s="100"/>
+      <c r="V35" s="100"/>
+      <c r="W35" s="100"/>
+      <c r="X35" s="100"/>
+      <c r="Y35" s="100"/>
+      <c r="Z35" s="100"/>
+      <c r="AA35" s="101"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="63"/>
       <c r="AE35" s="64"/>
@@ -4542,29 +4542,29 @@
         <f>IF(AND(E36&lt;&gt;"",E36=[1]Answers!E36),1,IF(ISBLANK(E36),0,-1))</f>
         <v>0</v>
       </c>
-      <c r="G36" s="119" t="s">
+      <c r="G36" s="102" t="s">
         <v>309</v>
       </c>
-      <c r="H36" s="120"/>
-      <c r="I36" s="120"/>
-      <c r="J36" s="120"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="120"/>
-      <c r="M36" s="120"/>
-      <c r="N36" s="120"/>
-      <c r="O36" s="120"/>
-      <c r="P36" s="120"/>
-      <c r="Q36" s="120"/>
-      <c r="R36" s="120"/>
-      <c r="S36" s="120"/>
-      <c r="T36" s="120"/>
-      <c r="U36" s="120"/>
-      <c r="V36" s="120"/>
-      <c r="W36" s="120"/>
-      <c r="X36" s="120"/>
-      <c r="Y36" s="120"/>
-      <c r="Z36" s="120"/>
-      <c r="AA36" s="121"/>
+      <c r="H36" s="103"/>
+      <c r="I36" s="103"/>
+      <c r="J36" s="103"/>
+      <c r="K36" s="103"/>
+      <c r="L36" s="103"/>
+      <c r="M36" s="103"/>
+      <c r="N36" s="103"/>
+      <c r="O36" s="103"/>
+      <c r="P36" s="103"/>
+      <c r="Q36" s="103"/>
+      <c r="R36" s="103"/>
+      <c r="S36" s="103"/>
+      <c r="T36" s="103"/>
+      <c r="U36" s="103"/>
+      <c r="V36" s="103"/>
+      <c r="W36" s="103"/>
+      <c r="X36" s="103"/>
+      <c r="Y36" s="103"/>
+      <c r="Z36" s="103"/>
+      <c r="AA36" s="104"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="63"/>
       <c r="AE36" s="64"/>
@@ -4667,13 +4667,13 @@
       <c r="C41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="123" t="s">
+      <c r="J41" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="K41" s="123"/>
-      <c r="L41" s="123"/>
-      <c r="M41" s="123"/>
-      <c r="N41" s="123"/>
+      <c r="K41" s="106"/>
+      <c r="L41" s="106"/>
+      <c r="M41" s="106"/>
+      <c r="N41" s="106"/>
       <c r="AS41" s="6"/>
       <c r="AT41" s="6"/>
       <c r="AU41" s="6"/>
@@ -4684,14 +4684,14 @@
       <c r="AZ41" s="6"/>
     </row>
     <row r="42" spans="2:52" ht="15" customHeight="1" thickTop="1">
-      <c r="J42" s="122" cm="1">
+      <c r="J42" s="105" cm="1">
         <f t="array" ref="J42">SUMPRODUCT(--(F34:F216=1),F34:F216,D34:D216)</f>
         <v>420</v>
       </c>
-      <c r="K42" s="122"/>
-      <c r="L42" s="122"/>
-      <c r="M42" s="122"/>
-      <c r="N42" s="122"/>
+      <c r="K42" s="105"/>
+      <c r="L42" s="105"/>
+      <c r="M42" s="105"/>
+      <c r="N42" s="105"/>
       <c r="AS42" s="6"/>
       <c r="AT42" s="6"/>
       <c r="AU42" s="6"/>
@@ -4705,11 +4705,11 @@
       <c r="B43" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="J43" s="122"/>
-      <c r="K43" s="122"/>
-      <c r="L43" s="122"/>
-      <c r="M43" s="122"/>
-      <c r="N43" s="122"/>
+      <c r="J43" s="105"/>
+      <c r="K43" s="105"/>
+      <c r="L43" s="105"/>
+      <c r="M43" s="105"/>
+      <c r="N43" s="105"/>
       <c r="AS43" s="6"/>
       <c r="AT43" s="6"/>
       <c r="AU43" s="6"/>
@@ -4722,11 +4722,11 @@
     <row r="44" spans="2:52" ht="15" customHeight="1" thickBot="1">
       <c r="B44" s="20"/>
       <c r="G44" s="27"/>
-      <c r="J44" s="122"/>
-      <c r="K44" s="122"/>
-      <c r="L44" s="122"/>
-      <c r="M44" s="122"/>
-      <c r="N44" s="122"/>
+      <c r="J44" s="105"/>
+      <c r="K44" s="105"/>
+      <c r="L44" s="105"/>
+      <c r="M44" s="105"/>
+      <c r="N44" s="105"/>
       <c r="R44" s="6"/>
     </row>
     <row r="45" spans="2:52" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
@@ -4747,11 +4747,11 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="122"/>
-      <c r="K45" s="122"/>
-      <c r="L45" s="122"/>
-      <c r="M45" s="122"/>
-      <c r="N45" s="122"/>
+      <c r="J45" s="105"/>
+      <c r="K45" s="105"/>
+      <c r="L45" s="105"/>
+      <c r="M45" s="105"/>
+      <c r="N45" s="105"/>
       <c r="R45" s="6"/>
       <c r="AB45" s="6"/>
       <c r="AC45" s="6"/>
@@ -5904,20 +5904,20 @@
       <c r="E67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="110" t="s">
+      <c r="G67" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="H67" s="111"/>
-      <c r="I67" s="111"/>
-      <c r="J67" s="111"/>
-      <c r="K67" s="111"/>
-      <c r="L67" s="111"/>
-      <c r="M67" s="111"/>
-      <c r="N67" s="111"/>
-      <c r="O67" s="111"/>
-      <c r="P67" s="111"/>
-      <c r="Q67" s="111"/>
-      <c r="R67" s="112"/>
+      <c r="H67" s="94"/>
+      <c r="I67" s="94"/>
+      <c r="J67" s="94"/>
+      <c r="K67" s="94"/>
+      <c r="L67" s="94"/>
+      <c r="M67" s="94"/>
+      <c r="N67" s="94"/>
+      <c r="O67" s="94"/>
+      <c r="P67" s="94"/>
+      <c r="Q67" s="94"/>
+      <c r="R67" s="95"/>
       <c r="S67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -7964,35 +7964,35 @@
         <v>4</v>
       </c>
       <c r="E104" s="44"/>
-      <c r="G104" s="124" t="s">
+      <c r="G104" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="H104" s="125"/>
-      <c r="I104" s="125"/>
-      <c r="J104" s="125"/>
-      <c r="K104" s="125"/>
-      <c r="L104" s="125"/>
-      <c r="M104" s="125"/>
-      <c r="N104" s="125"/>
-      <c r="O104" s="125"/>
-      <c r="P104" s="125"/>
-      <c r="Q104" s="125"/>
-      <c r="R104" s="125"/>
-      <c r="S104" s="125"/>
-      <c r="T104" s="125"/>
-      <c r="U104" s="125"/>
-      <c r="V104" s="125"/>
-      <c r="W104" s="125"/>
-      <c r="X104" s="125"/>
-      <c r="Y104" s="125"/>
-      <c r="Z104" s="125"/>
-      <c r="AA104" s="125"/>
-      <c r="AB104" s="125"/>
-      <c r="AC104" s="125"/>
-      <c r="AD104" s="125"/>
-      <c r="AE104" s="125"/>
-      <c r="AF104" s="125"/>
-      <c r="AG104" s="126"/>
+      <c r="H104" s="108"/>
+      <c r="I104" s="108"/>
+      <c r="J104" s="108"/>
+      <c r="K104" s="108"/>
+      <c r="L104" s="108"/>
+      <c r="M104" s="108"/>
+      <c r="N104" s="108"/>
+      <c r="O104" s="108"/>
+      <c r="P104" s="108"/>
+      <c r="Q104" s="108"/>
+      <c r="R104" s="108"/>
+      <c r="S104" s="108"/>
+      <c r="T104" s="108"/>
+      <c r="U104" s="108"/>
+      <c r="V104" s="108"/>
+      <c r="W104" s="108"/>
+      <c r="X104" s="108"/>
+      <c r="Y104" s="108"/>
+      <c r="Z104" s="108"/>
+      <c r="AA104" s="108"/>
+      <c r="AB104" s="108"/>
+      <c r="AC104" s="108"/>
+      <c r="AD104" s="108"/>
+      <c r="AE104" s="108"/>
+      <c r="AF104" s="108"/>
+      <c r="AG104" s="109"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
       <c r="AJ104" s="6"/>
@@ -9668,48 +9668,48 @@
       <c r="G144" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I144" s="104" t="s">
+      <c r="I144" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J144" s="105"/>
-      <c r="K144" s="105"/>
-      <c r="L144" s="105"/>
-      <c r="M144" s="105"/>
-      <c r="N144" s="105"/>
-      <c r="O144" s="105"/>
-      <c r="P144" s="105"/>
-      <c r="Q144" s="105"/>
-      <c r="R144" s="105"/>
-      <c r="S144" s="105"/>
-      <c r="T144" s="105"/>
-      <c r="U144" s="105"/>
-      <c r="V144" s="105"/>
-      <c r="W144" s="105"/>
-      <c r="X144" s="105"/>
-      <c r="Y144" s="105"/>
-      <c r="Z144" s="105"/>
-      <c r="AA144" s="105"/>
-      <c r="AB144" s="105"/>
-      <c r="AC144" s="105"/>
-      <c r="AD144" s="105"/>
-      <c r="AE144" s="105"/>
-      <c r="AF144" s="105"/>
-      <c r="AG144" s="105"/>
-      <c r="AH144" s="105"/>
-      <c r="AI144" s="105"/>
-      <c r="AJ144" s="105"/>
-      <c r="AK144" s="105"/>
-      <c r="AL144" s="105"/>
-      <c r="AM144" s="105"/>
-      <c r="AN144" s="105"/>
-      <c r="AO144" s="105"/>
-      <c r="AP144" s="105"/>
-      <c r="AQ144" s="105"/>
-      <c r="AR144" s="105"/>
-      <c r="AS144" s="105"/>
-      <c r="AT144" s="105"/>
-      <c r="AU144" s="105"/>
-      <c r="AV144" s="106"/>
+      <c r="J144" s="88"/>
+      <c r="K144" s="88"/>
+      <c r="L144" s="88"/>
+      <c r="M144" s="88"/>
+      <c r="N144" s="88"/>
+      <c r="O144" s="88"/>
+      <c r="P144" s="88"/>
+      <c r="Q144" s="88"/>
+      <c r="R144" s="88"/>
+      <c r="S144" s="88"/>
+      <c r="T144" s="88"/>
+      <c r="U144" s="88"/>
+      <c r="V144" s="88"/>
+      <c r="W144" s="88"/>
+      <c r="X144" s="88"/>
+      <c r="Y144" s="88"/>
+      <c r="Z144" s="88"/>
+      <c r="AA144" s="88"/>
+      <c r="AB144" s="88"/>
+      <c r="AC144" s="88"/>
+      <c r="AD144" s="88"/>
+      <c r="AE144" s="88"/>
+      <c r="AF144" s="88"/>
+      <c r="AG144" s="88"/>
+      <c r="AH144" s="88"/>
+      <c r="AI144" s="88"/>
+      <c r="AJ144" s="88"/>
+      <c r="AK144" s="88"/>
+      <c r="AL144" s="88"/>
+      <c r="AM144" s="88"/>
+      <c r="AN144" s="88"/>
+      <c r="AO144" s="88"/>
+      <c r="AP144" s="88"/>
+      <c r="AQ144" s="88"/>
+      <c r="AR144" s="88"/>
+      <c r="AS144" s="88"/>
+      <c r="AT144" s="88"/>
+      <c r="AU144" s="88"/>
+      <c r="AV144" s="89"/>
       <c r="AW144" s="6"/>
       <c r="AX144" s="6"/>
       <c r="AY144" s="6"/>
@@ -11300,52 +11300,52 @@
       <c r="G179" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I179" s="104" t="s">
+      <c r="I179" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J179" s="105"/>
-      <c r="K179" s="105"/>
-      <c r="L179" s="105"/>
-      <c r="M179" s="105"/>
-      <c r="N179" s="105"/>
-      <c r="O179" s="105"/>
-      <c r="P179" s="105"/>
-      <c r="Q179" s="105"/>
-      <c r="R179" s="105"/>
-      <c r="S179" s="105"/>
-      <c r="T179" s="105"/>
-      <c r="U179" s="105"/>
-      <c r="V179" s="105"/>
-      <c r="W179" s="105"/>
-      <c r="X179" s="105"/>
-      <c r="Y179" s="105"/>
-      <c r="Z179" s="105"/>
-      <c r="AA179" s="105"/>
-      <c r="AB179" s="105"/>
-      <c r="AC179" s="105"/>
-      <c r="AD179" s="105"/>
-      <c r="AE179" s="105"/>
-      <c r="AF179" s="105"/>
-      <c r="AG179" s="105"/>
-      <c r="AH179" s="105"/>
-      <c r="AI179" s="105"/>
-      <c r="AJ179" s="105"/>
-      <c r="AK179" s="105"/>
-      <c r="AL179" s="105"/>
-      <c r="AM179" s="105"/>
-      <c r="AN179" s="105"/>
-      <c r="AO179" s="105"/>
-      <c r="AP179" s="105"/>
-      <c r="AQ179" s="105"/>
-      <c r="AR179" s="105"/>
-      <c r="AS179" s="105"/>
-      <c r="AT179" s="105"/>
-      <c r="AU179" s="105"/>
-      <c r="AV179" s="105"/>
-      <c r="AW179" s="105"/>
-      <c r="AX179" s="105"/>
-      <c r="AY179" s="105"/>
-      <c r="AZ179" s="106"/>
+      <c r="J179" s="88"/>
+      <c r="K179" s="88"/>
+      <c r="L179" s="88"/>
+      <c r="M179" s="88"/>
+      <c r="N179" s="88"/>
+      <c r="O179" s="88"/>
+      <c r="P179" s="88"/>
+      <c r="Q179" s="88"/>
+      <c r="R179" s="88"/>
+      <c r="S179" s="88"/>
+      <c r="T179" s="88"/>
+      <c r="U179" s="88"/>
+      <c r="V179" s="88"/>
+      <c r="W179" s="88"/>
+      <c r="X179" s="88"/>
+      <c r="Y179" s="88"/>
+      <c r="Z179" s="88"/>
+      <c r="AA179" s="88"/>
+      <c r="AB179" s="88"/>
+      <c r="AC179" s="88"/>
+      <c r="AD179" s="88"/>
+      <c r="AE179" s="88"/>
+      <c r="AF179" s="88"/>
+      <c r="AG179" s="88"/>
+      <c r="AH179" s="88"/>
+      <c r="AI179" s="88"/>
+      <c r="AJ179" s="88"/>
+      <c r="AK179" s="88"/>
+      <c r="AL179" s="88"/>
+      <c r="AM179" s="88"/>
+      <c r="AN179" s="88"/>
+      <c r="AO179" s="88"/>
+      <c r="AP179" s="88"/>
+      <c r="AQ179" s="88"/>
+      <c r="AR179" s="88"/>
+      <c r="AS179" s="88"/>
+      <c r="AT179" s="88"/>
+      <c r="AU179" s="88"/>
+      <c r="AV179" s="88"/>
+      <c r="AW179" s="88"/>
+      <c r="AX179" s="88"/>
+      <c r="AY179" s="88"/>
+      <c r="AZ179" s="89"/>
     </row>
     <row r="180" spans="2:52" ht="15" thickTop="1">
       <c r="B180" s="1"/>
@@ -13549,6 +13549,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AH28:AI28"/>
+    <mergeCell ref="AF28:AG28"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="B14:T28"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y11:AA11"/>
     <mergeCell ref="I144:AV144"/>
     <mergeCell ref="I179:AZ179"/>
     <mergeCell ref="B30:AA30"/>
@@ -13560,15 +13569,6 @@
     <mergeCell ref="J42:N45"/>
     <mergeCell ref="J41:N41"/>
     <mergeCell ref="G104:AG104"/>
-    <mergeCell ref="AH28:AI28"/>
-    <mergeCell ref="AF28:AG28"/>
-    <mergeCell ref="B2:AA2"/>
-    <mergeCell ref="B4:T4"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="B14:T28"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y11:AA11"/>
   </mergeCells>
   <conditionalFormatting sqref="Y15:AA26 AE26 AC27:AE39">
     <cfRule type="expression" dxfId="4" priority="16">
@@ -52167,34 +52167,34 @@
       <c r="BD1" s="6"/>
     </row>
     <row r="2" spans="2:56" ht="60.6" customHeight="1">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="111" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="88"/>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
       <c r="AO2" s="3"/>
       <c r="AY2" s="6"/>
       <c r="AZ2" s="6"/>
@@ -52218,32 +52218,32 @@
       <c r="BD3" s="6"/>
     </row>
     <row r="4" spans="2:56" ht="33.6" customHeight="1">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="Y4" s="100" t="s">
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="Y4" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="Z4" s="100"/>
-      <c r="AA4" s="89"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="112"/>
       <c r="AO4" s="3"/>
       <c r="AY4" s="6"/>
       <c r="AZ4" s="6"/>
@@ -52471,11 +52471,11 @@
       <c r="T11" s="31"/>
       <c r="U11" s="31"/>
       <c r="X11" s="31"/>
-      <c r="Y11" s="101" t="s">
+      <c r="Y11" s="124" t="s">
         <v>164</v>
       </c>
-      <c r="Z11" s="102"/>
-      <c r="AA11" s="103"/>
+      <c r="Z11" s="125"/>
+      <c r="AA11" s="126"/>
       <c r="AO11" s="3"/>
       <c r="AY11" s="6"/>
       <c r="AZ11" s="6"/>
@@ -52520,33 +52520,33 @@
       <c r="BD12" s="6"/>
     </row>
     <row r="13" spans="2:56" ht="24.9" customHeight="1" thickBot="1">
-      <c r="B13" s="90" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="89"/>
-      <c r="T13" s="89"/>
+      <c r="B13" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+      <c r="Q13" s="112"/>
+      <c r="R13" s="112"/>
+      <c r="S13" s="112"/>
+      <c r="T13" s="112"/>
       <c r="U13" s="60"/>
-      <c r="Y13" s="90" t="s">
+      <c r="Y13" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="Z13" s="89"/>
-      <c r="AA13" s="89"/>
+      <c r="Z13" s="112"/>
+      <c r="AA13" s="112"/>
       <c r="AF13" s="60"/>
       <c r="AG13" s="60"/>
       <c r="AH13" s="60"/>
@@ -52554,27 +52554,27 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="2:56" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="114" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="92"/>
-      <c r="O14" s="92"/>
-      <c r="P14" s="92"/>
-      <c r="Q14" s="92"/>
-      <c r="R14" s="92"/>
-      <c r="S14" s="92"/>
-      <c r="T14" s="93"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="115"/>
+      <c r="L14" s="115"/>
+      <c r="M14" s="115"/>
+      <c r="N14" s="115"/>
+      <c r="O14" s="115"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="115"/>
+      <c r="R14" s="115"/>
+      <c r="S14" s="115"/>
+      <c r="T14" s="116"/>
       <c r="U14" s="3"/>
       <c r="Y14" s="61" t="s">
         <v>31</v>
@@ -52591,25 +52591,25 @@
       <c r="AP14" s="3"/>
     </row>
     <row r="15" spans="2:56" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B15" s="94"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="95"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="95"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="95"/>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="95"/>
-      <c r="R15" s="95"/>
-      <c r="S15" s="95"/>
-      <c r="T15" s="96"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="118"/>
+      <c r="Q15" s="118"/>
+      <c r="R15" s="118"/>
+      <c r="S15" s="118"/>
+      <c r="T15" s="119"/>
       <c r="U15" s="3"/>
       <c r="Y15" s="62" t="s">
         <v>32</v>
@@ -52626,25 +52626,25 @@
       <c r="AP15" s="3"/>
     </row>
     <row r="16" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B16" s="94"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="95"/>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="95"/>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="95"/>
-      <c r="S16" s="95"/>
-      <c r="T16" s="96"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="118"/>
+      <c r="S16" s="118"/>
+      <c r="T16" s="119"/>
       <c r="U16" s="3"/>
       <c r="Y16" s="62" t="s">
         <v>47</v>
@@ -52660,25 +52660,25 @@
       <c r="AP16" s="3"/>
     </row>
     <row r="17" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="95"/>
-      <c r="N17" s="95"/>
-      <c r="O17" s="95"/>
-      <c r="P17" s="95"/>
-      <c r="Q17" s="95"/>
-      <c r="R17" s="95"/>
-      <c r="S17" s="95"/>
-      <c r="T17" s="96"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="118"/>
+      <c r="P17" s="118"/>
+      <c r="Q17" s="118"/>
+      <c r="R17" s="118"/>
+      <c r="S17" s="118"/>
+      <c r="T17" s="119"/>
       <c r="U17" s="3"/>
       <c r="Y17" s="62" t="s">
         <v>39</v>
@@ -52694,25 +52694,25 @@
       <c r="AP17" s="3"/>
     </row>
     <row r="18" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B18" s="94"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="95"/>
-      <c r="O18" s="95"/>
-      <c r="P18" s="95"/>
-      <c r="Q18" s="95"/>
-      <c r="R18" s="95"/>
-      <c r="S18" s="95"/>
-      <c r="T18" s="96"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
+      <c r="N18" s="118"/>
+      <c r="O18" s="118"/>
+      <c r="P18" s="118"/>
+      <c r="Q18" s="118"/>
+      <c r="R18" s="118"/>
+      <c r="S18" s="118"/>
+      <c r="T18" s="119"/>
       <c r="U18" s="3"/>
       <c r="Y18" s="62" t="s">
         <v>35</v>
@@ -52728,25 +52728,25 @@
       <c r="AO18" s="3"/>
     </row>
     <row r="19" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B19" s="94"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="95"/>
-      <c r="P19" s="95"/>
-      <c r="Q19" s="95"/>
-      <c r="R19" s="95"/>
-      <c r="S19" s="95"/>
-      <c r="T19" s="96"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="118"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="118"/>
+      <c r="N19" s="118"/>
+      <c r="O19" s="118"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="118"/>
+      <c r="R19" s="118"/>
+      <c r="S19" s="118"/>
+      <c r="T19" s="119"/>
       <c r="U19" s="3"/>
       <c r="Y19" s="62" t="s">
         <v>42</v>
@@ -52762,25 +52762,25 @@
       <c r="AO19" s="3"/>
     </row>
     <row r="20" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B20" s="94"/>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="95"/>
-      <c r="K20" s="95"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="95"/>
-      <c r="Q20" s="95"/>
-      <c r="R20" s="95"/>
-      <c r="S20" s="95"/>
-      <c r="T20" s="96"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="118"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="118"/>
+      <c r="K20" s="118"/>
+      <c r="L20" s="118"/>
+      <c r="M20" s="118"/>
+      <c r="N20" s="118"/>
+      <c r="O20" s="118"/>
+      <c r="P20" s="118"/>
+      <c r="Q20" s="118"/>
+      <c r="R20" s="118"/>
+      <c r="S20" s="118"/>
+      <c r="T20" s="119"/>
       <c r="U20" s="3"/>
       <c r="Y20" s="62" t="s">
         <v>48</v>
@@ -52794,25 +52794,25 @@
       <c r="AO20" s="3"/>
     </row>
     <row r="21" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B21" s="94"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="95"/>
-      <c r="S21" s="95"/>
-      <c r="T21" s="96"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="118"/>
+      <c r="O21" s="118"/>
+      <c r="P21" s="118"/>
+      <c r="Q21" s="118"/>
+      <c r="R21" s="118"/>
+      <c r="S21" s="118"/>
+      <c r="T21" s="119"/>
       <c r="U21" s="3"/>
       <c r="Y21" s="62" t="s">
         <v>49</v>
@@ -52828,25 +52828,25 @@
       <c r="AO21" s="3"/>
     </row>
     <row r="22" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="95"/>
-      <c r="J22" s="95"/>
-      <c r="K22" s="95"/>
-      <c r="L22" s="95"/>
-      <c r="M22" s="95"/>
-      <c r="N22" s="95"/>
-      <c r="O22" s="95"/>
-      <c r="P22" s="95"/>
-      <c r="Q22" s="95"/>
-      <c r="R22" s="95"/>
-      <c r="S22" s="95"/>
-      <c r="T22" s="96"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="118"/>
+      <c r="O22" s="118"/>
+      <c r="P22" s="118"/>
+      <c r="Q22" s="118"/>
+      <c r="R22" s="118"/>
+      <c r="S22" s="118"/>
+      <c r="T22" s="119"/>
       <c r="U22" s="3"/>
       <c r="Y22" s="62" t="s">
         <v>50</v>
@@ -52863,25 +52863,25 @@
       <c r="AP22" s="3"/>
     </row>
     <row r="23" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B23" s="94"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="95"/>
-      <c r="K23" s="95"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="95"/>
-      <c r="P23" s="95"/>
-      <c r="Q23" s="95"/>
-      <c r="R23" s="95"/>
-      <c r="S23" s="95"/>
-      <c r="T23" s="96"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="118"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="118"/>
+      <c r="M23" s="118"/>
+      <c r="N23" s="118"/>
+      <c r="O23" s="118"/>
+      <c r="P23" s="118"/>
+      <c r="Q23" s="118"/>
+      <c r="R23" s="118"/>
+      <c r="S23" s="118"/>
+      <c r="T23" s="119"/>
       <c r="U23" s="3"/>
       <c r="Y23" s="62" t="s">
         <v>51</v>
@@ -52898,25 +52898,25 @@
       <c r="AP23" s="3"/>
     </row>
     <row r="24" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B24" s="94"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="95"/>
-      <c r="N24" s="95"/>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="95"/>
-      <c r="S24" s="95"/>
-      <c r="T24" s="96"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="118"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="118"/>
+      <c r="M24" s="118"/>
+      <c r="N24" s="118"/>
+      <c r="O24" s="118"/>
+      <c r="P24" s="118"/>
+      <c r="Q24" s="118"/>
+      <c r="R24" s="118"/>
+      <c r="S24" s="118"/>
+      <c r="T24" s="119"/>
       <c r="U24" s="3"/>
       <c r="Y24" s="62" t="s">
         <v>52</v>
@@ -52933,25 +52933,25 @@
       <c r="AP24" s="3"/>
     </row>
     <row r="25" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B25" s="94"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="95"/>
-      <c r="Q25" s="95"/>
-      <c r="R25" s="95"/>
-      <c r="S25" s="95"/>
-      <c r="T25" s="96"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="118"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="118"/>
+      <c r="K25" s="118"/>
+      <c r="L25" s="118"/>
+      <c r="M25" s="118"/>
+      <c r="N25" s="118"/>
+      <c r="O25" s="118"/>
+      <c r="P25" s="118"/>
+      <c r="Q25" s="118"/>
+      <c r="R25" s="118"/>
+      <c r="S25" s="118"/>
+      <c r="T25" s="119"/>
       <c r="U25" s="3"/>
       <c r="Y25" s="62" t="s">
         <v>53</v>
@@ -52966,25 +52966,25 @@
       <c r="AP25" s="3"/>
     </row>
     <row r="26" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B26" s="94"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="95"/>
-      <c r="I26" s="95"/>
-      <c r="J26" s="95"/>
-      <c r="K26" s="95"/>
-      <c r="L26" s="95"/>
-      <c r="M26" s="95"/>
-      <c r="N26" s="95"/>
-      <c r="O26" s="95"/>
-      <c r="P26" s="95"/>
-      <c r="Q26" s="95"/>
-      <c r="R26" s="95"/>
-      <c r="S26" s="95"/>
-      <c r="T26" s="96"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="118"/>
+      <c r="M26" s="118"/>
+      <c r="N26" s="118"/>
+      <c r="O26" s="118"/>
+      <c r="P26" s="118"/>
+      <c r="Q26" s="118"/>
+      <c r="R26" s="118"/>
+      <c r="S26" s="118"/>
+      <c r="T26" s="119"/>
       <c r="U26" s="3"/>
       <c r="Y26" s="62" t="s">
         <v>105</v>
@@ -53004,25 +53004,25 @@
       <c r="AP26" s="3"/>
     </row>
     <row r="27" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B27" s="94"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="95"/>
-      <c r="N27" s="95"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="95"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="96"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="118"/>
+      <c r="O27" s="118"/>
+      <c r="P27" s="118"/>
+      <c r="Q27" s="118"/>
+      <c r="R27" s="118"/>
+      <c r="S27" s="118"/>
+      <c r="T27" s="119"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -53041,25 +53041,25 @@
       <c r="AP27" s="3"/>
     </row>
     <row r="28" spans="2:56" ht="47.25" customHeight="1">
-      <c r="B28" s="97"/>
-      <c r="C28" s="98"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="98"/>
-      <c r="I28" s="98"/>
-      <c r="J28" s="98"/>
-      <c r="K28" s="98"/>
-      <c r="L28" s="98"/>
-      <c r="M28" s="98"/>
-      <c r="N28" s="98"/>
-      <c r="O28" s="98"/>
-      <c r="P28" s="98"/>
-      <c r="Q28" s="98"/>
-      <c r="R28" s="98"/>
-      <c r="S28" s="98"/>
-      <c r="T28" s="99"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="121"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="121"/>
+      <c r="K28" s="121"/>
+      <c r="L28" s="121"/>
+      <c r="M28" s="121"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="121"/>
+      <c r="P28" s="121"/>
+      <c r="Q28" s="121"/>
+      <c r="R28" s="121"/>
+      <c r="S28" s="121"/>
+      <c r="T28" s="122"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -53070,10 +53070,10 @@
       <c r="AC28" s="63"/>
       <c r="AD28" s="63"/>
       <c r="AE28" s="64"/>
-      <c r="AF28" s="87"/>
-      <c r="AG28" s="87"/>
-      <c r="AH28" s="87"/>
-      <c r="AI28" s="87"/>
+      <c r="AF28" s="110"/>
+      <c r="AG28" s="110"/>
+      <c r="AH28" s="110"/>
+      <c r="AI28" s="110"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
     </row>
@@ -53122,34 +53122,34 @@
       <c r="BD29" s="6"/>
     </row>
     <row r="30" spans="2:56" ht="25.5" customHeight="1">
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="108"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="108"/>
-      <c r="F30" s="108"/>
-      <c r="G30" s="108"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="108"/>
-      <c r="J30" s="108"/>
-      <c r="K30" s="108"/>
-      <c r="L30" s="108"/>
-      <c r="M30" s="108"/>
-      <c r="N30" s="108"/>
-      <c r="O30" s="108"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="108"/>
-      <c r="T30" s="108"/>
-      <c r="U30" s="108"/>
-      <c r="V30" s="108"/>
-      <c r="W30" s="108"/>
-      <c r="X30" s="108"/>
-      <c r="Y30" s="108"/>
-      <c r="Z30" s="108"/>
-      <c r="AA30" s="109"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="91"/>
+      <c r="R30" s="91"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="91"/>
+      <c r="X30" s="91"/>
+      <c r="Y30" s="91"/>
+      <c r="Z30" s="91"/>
+      <c r="AA30" s="92"/>
       <c r="AC30" s="63"/>
       <c r="AD30" s="63"/>
       <c r="AE30" s="64"/>
@@ -53212,29 +53212,29 @@
       <c r="E33" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="110" t="s">
+      <c r="G33" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="111"/>
-      <c r="I33" s="111"/>
-      <c r="J33" s="111"/>
-      <c r="K33" s="111"/>
-      <c r="L33" s="111"/>
-      <c r="M33" s="111"/>
-      <c r="N33" s="111"/>
-      <c r="O33" s="111"/>
-      <c r="P33" s="111"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="111"/>
-      <c r="W33" s="111"/>
-      <c r="X33" s="111"/>
-      <c r="Y33" s="111"/>
-      <c r="Z33" s="111"/>
-      <c r="AA33" s="112"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="95"/>
       <c r="AC33" s="63"/>
       <c r="AD33" s="63"/>
       <c r="AE33" s="64"/>
@@ -53257,29 +53257,29 @@
         <v>29</v>
       </c>
       <c r="F34" s="36"/>
-      <c r="G34" s="113" t="s">
+      <c r="G34" s="96" t="s">
         <v>302</v>
       </c>
-      <c r="H34" s="114"/>
-      <c r="I34" s="114"/>
-      <c r="J34" s="114"/>
-      <c r="K34" s="114"/>
-      <c r="L34" s="114"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="114"/>
-      <c r="O34" s="114"/>
-      <c r="P34" s="114"/>
-      <c r="Q34" s="114"/>
-      <c r="R34" s="114"/>
-      <c r="S34" s="114"/>
-      <c r="T34" s="114"/>
-      <c r="U34" s="114"/>
-      <c r="V34" s="114"/>
-      <c r="W34" s="114"/>
-      <c r="X34" s="114"/>
-      <c r="Y34" s="114"/>
-      <c r="Z34" s="114"/>
-      <c r="AA34" s="115"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="97"/>
+      <c r="N34" s="97"/>
+      <c r="O34" s="97"/>
+      <c r="P34" s="97"/>
+      <c r="Q34" s="97"/>
+      <c r="R34" s="97"/>
+      <c r="S34" s="97"/>
+      <c r="T34" s="97"/>
+      <c r="U34" s="97"/>
+      <c r="V34" s="97"/>
+      <c r="W34" s="97"/>
+      <c r="X34" s="97"/>
+      <c r="Y34" s="97"/>
+      <c r="Z34" s="97"/>
+      <c r="AA34" s="98"/>
       <c r="AC34" s="63"/>
       <c r="AD34" s="63"/>
       <c r="AE34" s="64"/>
@@ -53302,29 +53302,29 @@
         <v>51</v>
       </c>
       <c r="F35" s="36"/>
-      <c r="G35" s="116" t="s">
+      <c r="G35" s="99" t="s">
         <v>299</v>
       </c>
-      <c r="H35" s="117"/>
-      <c r="I35" s="117"/>
-      <c r="J35" s="117"/>
-      <c r="K35" s="117"/>
-      <c r="L35" s="117"/>
-      <c r="M35" s="117"/>
-      <c r="N35" s="117"/>
-      <c r="O35" s="117"/>
-      <c r="P35" s="117"/>
-      <c r="Q35" s="117"/>
-      <c r="R35" s="117"/>
-      <c r="S35" s="117"/>
-      <c r="T35" s="117"/>
-      <c r="U35" s="117"/>
-      <c r="V35" s="117"/>
-      <c r="W35" s="117"/>
-      <c r="X35" s="117"/>
-      <c r="Y35" s="117"/>
-      <c r="Z35" s="117"/>
-      <c r="AA35" s="118"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="100"/>
+      <c r="R35" s="100"/>
+      <c r="S35" s="100"/>
+      <c r="T35" s="100"/>
+      <c r="U35" s="100"/>
+      <c r="V35" s="100"/>
+      <c r="W35" s="100"/>
+      <c r="X35" s="100"/>
+      <c r="Y35" s="100"/>
+      <c r="Z35" s="100"/>
+      <c r="AA35" s="101"/>
       <c r="AC35" s="63"/>
       <c r="AD35" s="63"/>
       <c r="AE35" s="64"/>
@@ -53347,29 +53347,29 @@
         <v>95</v>
       </c>
       <c r="F36" s="36"/>
-      <c r="G36" s="119" t="s">
+      <c r="G36" s="102" t="s">
         <v>301</v>
       </c>
-      <c r="H36" s="120"/>
-      <c r="I36" s="120"/>
-      <c r="J36" s="120"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="120"/>
-      <c r="M36" s="120"/>
-      <c r="N36" s="120"/>
-      <c r="O36" s="120"/>
-      <c r="P36" s="120"/>
-      <c r="Q36" s="120"/>
-      <c r="R36" s="120"/>
-      <c r="S36" s="120"/>
-      <c r="T36" s="120"/>
-      <c r="U36" s="120"/>
-      <c r="V36" s="120"/>
-      <c r="W36" s="120"/>
-      <c r="X36" s="120"/>
-      <c r="Y36" s="120"/>
-      <c r="Z36" s="120"/>
-      <c r="AA36" s="121"/>
+      <c r="H36" s="103"/>
+      <c r="I36" s="103"/>
+      <c r="J36" s="103"/>
+      <c r="K36" s="103"/>
+      <c r="L36" s="103"/>
+      <c r="M36" s="103"/>
+      <c r="N36" s="103"/>
+      <c r="O36" s="103"/>
+      <c r="P36" s="103"/>
+      <c r="Q36" s="103"/>
+      <c r="R36" s="103"/>
+      <c r="S36" s="103"/>
+      <c r="T36" s="103"/>
+      <c r="U36" s="103"/>
+      <c r="V36" s="103"/>
+      <c r="W36" s="103"/>
+      <c r="X36" s="103"/>
+      <c r="Y36" s="103"/>
+      <c r="Z36" s="103"/>
+      <c r="AA36" s="104"/>
       <c r="AC36" s="63"/>
       <c r="AD36" s="63"/>
       <c r="AE36" s="64"/>
@@ -54838,20 +54838,20 @@
       <c r="E67" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="110" t="s">
+      <c r="G67" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="H67" s="111"/>
-      <c r="I67" s="111"/>
-      <c r="J67" s="111"/>
-      <c r="K67" s="111"/>
-      <c r="L67" s="111"/>
-      <c r="M67" s="111"/>
-      <c r="N67" s="111"/>
-      <c r="O67" s="111"/>
-      <c r="P67" s="111"/>
-      <c r="Q67" s="111"/>
-      <c r="R67" s="112"/>
+      <c r="H67" s="94"/>
+      <c r="I67" s="94"/>
+      <c r="J67" s="94"/>
+      <c r="K67" s="94"/>
+      <c r="L67" s="94"/>
+      <c r="M67" s="94"/>
+      <c r="N67" s="94"/>
+      <c r="O67" s="94"/>
+      <c r="P67" s="94"/>
+      <c r="Q67" s="94"/>
+      <c r="R67" s="95"/>
       <c r="S67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
@@ -56891,34 +56891,34 @@
       <c r="E104" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G104" s="124" t="s">
+      <c r="G104" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="H104" s="125"/>
-      <c r="I104" s="125"/>
-      <c r="J104" s="125"/>
-      <c r="K104" s="125"/>
-      <c r="L104" s="125"/>
-      <c r="M104" s="125"/>
-      <c r="N104" s="125"/>
-      <c r="O104" s="125"/>
-      <c r="P104" s="125"/>
-      <c r="Q104" s="125"/>
-      <c r="R104" s="125"/>
-      <c r="S104" s="125"/>
-      <c r="T104" s="125"/>
-      <c r="U104" s="125"/>
-      <c r="V104" s="125"/>
-      <c r="W104" s="125"/>
-      <c r="X104" s="125"/>
-      <c r="Y104" s="125"/>
-      <c r="Z104" s="125"/>
-      <c r="AA104" s="125"/>
-      <c r="AB104" s="125"/>
-      <c r="AC104" s="125"/>
-      <c r="AD104" s="125"/>
-      <c r="AE104" s="125"/>
-      <c r="AF104" s="126"/>
+      <c r="H104" s="108"/>
+      <c r="I104" s="108"/>
+      <c r="J104" s="108"/>
+      <c r="K104" s="108"/>
+      <c r="L104" s="108"/>
+      <c r="M104" s="108"/>
+      <c r="N104" s="108"/>
+      <c r="O104" s="108"/>
+      <c r="P104" s="108"/>
+      <c r="Q104" s="108"/>
+      <c r="R104" s="108"/>
+      <c r="S104" s="108"/>
+      <c r="T104" s="108"/>
+      <c r="U104" s="108"/>
+      <c r="V104" s="108"/>
+      <c r="W104" s="108"/>
+      <c r="X104" s="108"/>
+      <c r="Y104" s="108"/>
+      <c r="Z104" s="108"/>
+      <c r="AA104" s="108"/>
+      <c r="AB104" s="108"/>
+      <c r="AC104" s="108"/>
+      <c r="AD104" s="108"/>
+      <c r="AE104" s="108"/>
+      <c r="AF104" s="109"/>
       <c r="AG104" s="6"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
@@ -58634,47 +58634,47 @@
       <c r="G144" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I144" s="104" t="s">
+      <c r="I144" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J144" s="105"/>
-      <c r="K144" s="105"/>
-      <c r="L144" s="105"/>
-      <c r="M144" s="105"/>
-      <c r="N144" s="105"/>
-      <c r="O144" s="105"/>
-      <c r="P144" s="105"/>
-      <c r="Q144" s="105"/>
-      <c r="R144" s="105"/>
-      <c r="S144" s="105"/>
-      <c r="T144" s="105"/>
-      <c r="U144" s="105"/>
-      <c r="V144" s="105"/>
-      <c r="W144" s="105"/>
-      <c r="X144" s="105"/>
-      <c r="Y144" s="105"/>
-      <c r="Z144" s="105"/>
-      <c r="AA144" s="105"/>
-      <c r="AB144" s="105"/>
-      <c r="AC144" s="105"/>
-      <c r="AD144" s="105"/>
-      <c r="AE144" s="105"/>
-      <c r="AF144" s="105"/>
-      <c r="AG144" s="105"/>
-      <c r="AH144" s="105"/>
-      <c r="AI144" s="105"/>
-      <c r="AJ144" s="105"/>
-      <c r="AK144" s="105"/>
-      <c r="AL144" s="105"/>
-      <c r="AM144" s="105"/>
-      <c r="AN144" s="105"/>
-      <c r="AO144" s="105"/>
-      <c r="AP144" s="105"/>
-      <c r="AQ144" s="105"/>
-      <c r="AR144" s="105"/>
-      <c r="AS144" s="105"/>
-      <c r="AT144" s="105"/>
-      <c r="AU144" s="106"/>
+      <c r="J144" s="88"/>
+      <c r="K144" s="88"/>
+      <c r="L144" s="88"/>
+      <c r="M144" s="88"/>
+      <c r="N144" s="88"/>
+      <c r="O144" s="88"/>
+      <c r="P144" s="88"/>
+      <c r="Q144" s="88"/>
+      <c r="R144" s="88"/>
+      <c r="S144" s="88"/>
+      <c r="T144" s="88"/>
+      <c r="U144" s="88"/>
+      <c r="V144" s="88"/>
+      <c r="W144" s="88"/>
+      <c r="X144" s="88"/>
+      <c r="Y144" s="88"/>
+      <c r="Z144" s="88"/>
+      <c r="AA144" s="88"/>
+      <c r="AB144" s="88"/>
+      <c r="AC144" s="88"/>
+      <c r="AD144" s="88"/>
+      <c r="AE144" s="88"/>
+      <c r="AF144" s="88"/>
+      <c r="AG144" s="88"/>
+      <c r="AH144" s="88"/>
+      <c r="AI144" s="88"/>
+      <c r="AJ144" s="88"/>
+      <c r="AK144" s="88"/>
+      <c r="AL144" s="88"/>
+      <c r="AM144" s="88"/>
+      <c r="AN144" s="88"/>
+      <c r="AO144" s="88"/>
+      <c r="AP144" s="88"/>
+      <c r="AQ144" s="88"/>
+      <c r="AR144" s="88"/>
+      <c r="AS144" s="88"/>
+      <c r="AT144" s="88"/>
+      <c r="AU144" s="89"/>
       <c r="AV144" s="6"/>
       <c r="AW144" s="6"/>
       <c r="AX144" s="6"/>
@@ -60326,55 +60326,55 @@
       <c r="G179" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I179" s="104" t="s">
+      <c r="I179" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J179" s="105"/>
-      <c r="K179" s="105"/>
-      <c r="L179" s="105"/>
-      <c r="M179" s="105"/>
-      <c r="N179" s="105"/>
-      <c r="O179" s="105"/>
-      <c r="P179" s="105"/>
-      <c r="Q179" s="105"/>
-      <c r="R179" s="105"/>
-      <c r="S179" s="105"/>
-      <c r="T179" s="105"/>
-      <c r="U179" s="105"/>
-      <c r="V179" s="105"/>
-      <c r="W179" s="105"/>
-      <c r="X179" s="105"/>
-      <c r="Y179" s="105"/>
-      <c r="Z179" s="105"/>
-      <c r="AA179" s="105"/>
-      <c r="AB179" s="105"/>
-      <c r="AC179" s="105"/>
-      <c r="AD179" s="105"/>
-      <c r="AE179" s="105"/>
-      <c r="AF179" s="105"/>
-      <c r="AG179" s="105"/>
-      <c r="AH179" s="105"/>
-      <c r="AI179" s="105"/>
-      <c r="AJ179" s="105"/>
-      <c r="AK179" s="105"/>
-      <c r="AL179" s="105"/>
-      <c r="AM179" s="105"/>
-      <c r="AN179" s="105"/>
-      <c r="AO179" s="105"/>
-      <c r="AP179" s="105"/>
-      <c r="AQ179" s="105"/>
-      <c r="AR179" s="105"/>
-      <c r="AS179" s="105"/>
-      <c r="AT179" s="105"/>
-      <c r="AU179" s="105"/>
-      <c r="AV179" s="105"/>
-      <c r="AW179" s="105"/>
-      <c r="AX179" s="105"/>
-      <c r="AY179" s="105"/>
-      <c r="AZ179" s="105"/>
-      <c r="BA179" s="105"/>
-      <c r="BB179" s="105"/>
-      <c r="BC179" s="106"/>
+      <c r="J179" s="88"/>
+      <c r="K179" s="88"/>
+      <c r="L179" s="88"/>
+      <c r="M179" s="88"/>
+      <c r="N179" s="88"/>
+      <c r="O179" s="88"/>
+      <c r="P179" s="88"/>
+      <c r="Q179" s="88"/>
+      <c r="R179" s="88"/>
+      <c r="S179" s="88"/>
+      <c r="T179" s="88"/>
+      <c r="U179" s="88"/>
+      <c r="V179" s="88"/>
+      <c r="W179" s="88"/>
+      <c r="X179" s="88"/>
+      <c r="Y179" s="88"/>
+      <c r="Z179" s="88"/>
+      <c r="AA179" s="88"/>
+      <c r="AB179" s="88"/>
+      <c r="AC179" s="88"/>
+      <c r="AD179" s="88"/>
+      <c r="AE179" s="88"/>
+      <c r="AF179" s="88"/>
+      <c r="AG179" s="88"/>
+      <c r="AH179" s="88"/>
+      <c r="AI179" s="88"/>
+      <c r="AJ179" s="88"/>
+      <c r="AK179" s="88"/>
+      <c r="AL179" s="88"/>
+      <c r="AM179" s="88"/>
+      <c r="AN179" s="88"/>
+      <c r="AO179" s="88"/>
+      <c r="AP179" s="88"/>
+      <c r="AQ179" s="88"/>
+      <c r="AR179" s="88"/>
+      <c r="AS179" s="88"/>
+      <c r="AT179" s="88"/>
+      <c r="AU179" s="88"/>
+      <c r="AV179" s="88"/>
+      <c r="AW179" s="88"/>
+      <c r="AX179" s="88"/>
+      <c r="AY179" s="88"/>
+      <c r="AZ179" s="88"/>
+      <c r="BA179" s="88"/>
+      <c r="BB179" s="88"/>
+      <c r="BC179" s="89"/>
       <c r="BD179" s="6"/>
     </row>
     <row r="180" spans="2:56" ht="15" thickTop="1">
@@ -62690,12 +62690,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:AA2"/>
-    <mergeCell ref="B4:T4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="G36:AA36"/>
+    <mergeCell ref="G67:R67"/>
+    <mergeCell ref="I179:BC179"/>
+    <mergeCell ref="I144:AU144"/>
+    <mergeCell ref="G104:AF104"/>
     <mergeCell ref="AF28:AG28"/>
     <mergeCell ref="AH28:AI28"/>
     <mergeCell ref="B30:AA30"/>
@@ -62703,11 +62702,12 @@
     <mergeCell ref="G35:AA35"/>
     <mergeCell ref="G34:AA34"/>
     <mergeCell ref="B14:T28"/>
-    <mergeCell ref="G36:AA36"/>
-    <mergeCell ref="G67:R67"/>
-    <mergeCell ref="I179:BC179"/>
-    <mergeCell ref="I144:AU144"/>
-    <mergeCell ref="G104:AF104"/>
+    <mergeCell ref="B2:AA2"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="Y13:AA13"/>
   </mergeCells>
   <conditionalFormatting sqref="Y15:AA26 AE26 AC27:AE39">
     <cfRule type="expression" dxfId="0" priority="16">

</xml_diff>